<commit_message>
tweak Meowsy and Chicks front animation
</commit_message>
<xml_diff>
--- a/trainers/trainers.xlsx
+++ b/trainers/trainers.xlsx
@@ -103,7 +103,7 @@
     <t xml:space="preserve">TRAINER_PETE</t>
   </si>
   <si>
-    <t xml:space="preserve">Doduo</t>
+    <t xml:space="preserve">Chicks</t>
   </si>
   <si>
     <t xml:space="preserve">Elekid</t>
@@ -127,7 +127,7 @@
     <t xml:space="preserve">TRAINER_MIGUEL_1</t>
   </si>
   <si>
-    <t xml:space="preserve">Meowth</t>
+    <t xml:space="preserve">Meowsy</t>
   </si>
   <si>
     <t xml:space="preserve">Covet</t>
@@ -222,12 +222,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -239,11 +239,14 @@
   </sheetPr>
   <dimension ref="A1:E49"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A48" activeCellId="0" sqref="A48"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A11" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A35" activeCellId="0" sqref="A35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.54"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -669,7 +672,7 @@
         <v>6</v>
       </c>
       <c r="C47" s="1"/>
-      <c r="E47" s="0" t="s">
+      <c r="E47" s="1" t="s">
         <v>36</v>
       </c>
     </row>
@@ -683,8 +686,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Normaali"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normaali"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
disable wild double battles and fix typo
</commit_message>
<xml_diff>
--- a/trainers/trainers.xlsx
+++ b/trainers/trainers.xlsx
@@ -181,7 +181,7 @@
     <t xml:space="preserve">TRAINER_MELINA</t>
   </si>
   <si>
-    <t xml:space="preserve">Elektrike</t>
+    <t xml:space="preserve">Electrike</t>
   </si>
   <si>
     <t xml:space="preserve">Poochyena</t>
@@ -332,8 +332,8 @@
   </sheetPr>
   <dimension ref="A1:E94"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A42" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A72" activeCellId="0" sqref="A72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
fix yet another typo
</commit_message>
<xml_diff>
--- a/trainers/trainers.xlsx
+++ b/trainers/trainers.xlsx
@@ -196,7 +196,7 @@
     <t xml:space="preserve">Tyrogue</t>
   </si>
   <si>
-    <t xml:space="preserve">TRAINER_MARIA</t>
+    <t xml:space="preserve">TRAINER_MARIA_1</t>
   </si>
   <si>
     <t xml:space="preserve">Puddi</t>
@@ -330,7 +330,7 @@
   <dimension ref="A1:E94"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A53" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A95" activeCellId="0" sqref="A95"/>
+      <selection pane="topLeft" activeCell="A80" activeCellId="0" sqref="A80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
petalburg gym trainers, fix porymap
</commit_message>
<xml_diff>
--- a/trainers/trainers.xlsx
+++ b/trainers/trainers.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="83">
   <si>
     <t xml:space="preserve">TRAINER_MAY_ROUTE_103_TREECKO</t>
   </si>
@@ -224,6 +224,48 @@
   </si>
   <si>
     <t xml:space="preserve">Bubble, Camouflage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRAINER_BERKE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sentret</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quick Attack</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rattata</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oran Berry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRAINER_JODY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pay Day</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zigzagoon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Headbutt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRAINER_NORMAN_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Galarian_Zigzagoon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Snarl, Headbutt, Sand-Attack, Leer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vigoroth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scratch, Uproar, Fury Swipes, Focus Energy</t>
   </si>
   <si>
     <t xml:space="preserve">END</t>
@@ -327,10 +369,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E94"/>
+  <dimension ref="A1:E111"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A53" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A80" activeCellId="0" sqref="A80"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A67" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E108" activeCellId="0" sqref="E108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1127,8 +1169,148 @@
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="1" t="s">
+      <c r="A94" s="0" t="s">
         <v>68</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D95" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E95" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B96" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="C96" s="1"/>
+      <c r="E96" s="0" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="B97" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="D97" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="E97" s="0" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A99" s="0" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A100" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D100" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E100" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A101" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B101" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="C101" s="1"/>
+      <c r="D101" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="E101" s="0" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A102" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="B102" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="E102" s="0" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A104" s="0" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A105" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B105" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C105" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D105" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E105" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A106" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="B106" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="E106" s="0" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A107" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="B107" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="E107" s="0" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A111" s="1" t="s">
+        <v>82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix typo and adjust trainer mary
</commit_message>
<xml_diff>
--- a/trainers/trainers.xlsx
+++ b/trainers/trainers.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="85">
   <si>
     <t xml:space="preserve">TRAINER_MAY_ROUTE_103_TREECKO</t>
   </si>
@@ -259,13 +259,19 @@
     <t xml:space="preserve">Galarian_Zigzagoon</t>
   </si>
   <si>
-    <t xml:space="preserve">Snarl, Headbutt, Sand-Attack, Leer</t>
+    <t xml:space="preserve">Snarl, Headbutt, Sand Attack, Leer</t>
   </si>
   <si>
     <t xml:space="preserve">Vigoroth</t>
   </si>
   <si>
     <t xml:space="preserve">Scratch, Uproar, Fury Swipes, Focus Energy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRAINER_MARY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cubone</t>
   </si>
   <si>
     <t xml:space="preserve">END</t>
@@ -369,10 +375,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E111"/>
+  <dimension ref="A1:E114"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A67" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E108" activeCellId="0" sqref="E108"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A74" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C112" activeCellId="0" sqref="C112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1308,9 +1314,48 @@
         <v>81</v>
       </c>
     </row>
+    <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A109" s="0" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A110" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C110" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D110" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E110" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="1" t="s">
-        <v>82</v>
+        <v>56</v>
+      </c>
+      <c r="B111" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="C111" s="1"/>
+    </row>
+    <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A112" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="B112" s="0" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A114" s="1" t="s">
+        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix various text snippets
</commit_message>
<xml_diff>
--- a/trainers/trainers.xlsx
+++ b/trainers/trainers.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="93">
   <si>
     <t xml:space="preserve">TRAINER_MAY_ROUTE_103_TREECKO</t>
   </si>
@@ -130,7 +130,7 @@
     <t xml:space="preserve">Meowsy</t>
   </si>
   <si>
-    <t xml:space="preserve">Covet</t>
+    <t xml:space="preserve">Covet, Growl</t>
   </si>
   <si>
     <t xml:space="preserve">Skitty</t>
@@ -272,6 +272,30 @@
   </si>
   <si>
     <t xml:space="preserve">Cubone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">.trainerClass </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> TRAINER_CLASS_BATTLE_GIRL,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">.encounterMusic_gender </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> F_TRAINER_FEMALE | TRAINER_ENCOUNTER_MUSIC_INTENSE,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">.trainerPic </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> TRAINER_PIC_BATTLE_GIRL,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">.items</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{},</t>
   </si>
   <si>
     <t xml:space="preserve">END</t>
@@ -375,10 +399,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E114"/>
+  <dimension ref="A1:E118"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A74" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C112" activeCellId="0" sqref="C112"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A89" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A116" activeCellId="0" sqref="A116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -807,7 +831,7 @@
       </c>
       <c r="C47" s="1"/>
       <c r="E47" s="1" t="s">
-        <v>36</v>
+        <v>11</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1353,9 +1377,41 @@
         <v>5</v>
       </c>
     </row>
+    <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A113" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="B113" s="0" t="s">
+        <v>85</v>
+      </c>
+    </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A114" s="1" t="s">
-        <v>84</v>
+      <c r="A114" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="B114" s="0" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A115" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="B115" s="0" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A116" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="B116" s="0" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A118" s="1" t="s">
+        <v>92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
move cries, fix typos
</commit_message>
<xml_diff>
--- a/trainers/trainers.xlsx
+++ b/trainers/trainers.xlsx
@@ -277,25 +277,25 @@
     <t xml:space="preserve">.trainerClass </t>
   </si>
   <si>
-    <t xml:space="preserve"> TRAINER_CLASS_BATTLE_GIRL,</t>
+    <t xml:space="preserve"> TRAINER_CLASS_BATTLE_GIRL</t>
   </si>
   <si>
     <t xml:space="preserve">.encounterMusic_gender </t>
   </si>
   <si>
-    <t xml:space="preserve"> F_TRAINER_FEMALE | TRAINER_ENCOUNTER_MUSIC_INTENSE,</t>
+    <t xml:space="preserve"> F_TRAINER_FEMALE | TRAINER_ENCOUNTER_MUSIC_INTENSE</t>
   </si>
   <si>
     <t xml:space="preserve">.trainerPic </t>
   </si>
   <si>
-    <t xml:space="preserve"> TRAINER_PIC_BATTLE_GIRL,</t>
+    <t xml:space="preserve"> TRAINER_PIC_BATTLE_GIRL</t>
   </si>
   <si>
     <t xml:space="preserve">.items</t>
   </si>
   <si>
-    <t xml:space="preserve">{},</t>
+    <t xml:space="preserve">{}</t>
   </si>
   <si>
     <t xml:space="preserve">END</t>
@@ -402,7 +402,7 @@
   <dimension ref="A1:E118"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A89" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A116" activeCellId="0" sqref="A116"/>
+      <selection pane="topLeft" activeCell="B117" activeCellId="0" sqref="B117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
change norman's dialogue to verdanturf, fix old flag names, update petalburg woods magma grunt music and party
</commit_message>
<xml_diff>
--- a/trainers/trainers.xlsx
+++ b/trainers/trainers.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="92">
   <si>
     <t xml:space="preserve">TRAINER_MAY_ROUTE_103_TREECKO</t>
   </si>
@@ -287,6 +287,12 @@
   </si>
   <si>
     <t xml:space="preserve">{}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRAINER_GRUNT_PETALBURG_WOODS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Charmander</t>
   </si>
   <si>
     <t xml:space="preserve">END</t>
@@ -390,10 +396,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E118"/>
+  <dimension ref="A1:E122"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A89" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B113" activeCellId="0" sqref="B113"/>
+      <selection pane="topLeft" activeCell="A120" activeCellId="0" sqref="A120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1401,8 +1407,38 @@
       </c>
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A118" s="1" t="s">
+      <c r="A118" s="0" t="s">
         <v>89</v>
+      </c>
+    </row>
+    <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A119" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B119" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C119" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D119" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E119" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A120" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="B120" s="0" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A122" s="1" t="s">
+        <v>91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
document trainer excel better, try to make altering cave show in pokedex areas!
</commit_message>
<xml_diff>
--- a/trainers/trainers.xlsx
+++ b/trainers/trainers.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="97">
   <si>
     <t xml:space="preserve">TRAINER_MAY_ROUTE_103_TREECKO</t>
   </si>
@@ -76,6 +76,9 @@
     <t xml:space="preserve">TRAINER_BRENDAN_ROUTE_103_MUDKIP</t>
   </si>
   <si>
+    <t xml:space="preserve"># Route 103</t>
+  </si>
+  <si>
     <t xml:space="preserve">TRAINER_ISABELLE</t>
   </si>
   <si>
@@ -136,6 +139,9 @@
     <t xml:space="preserve">Skitty</t>
   </si>
   <si>
+    <t xml:space="preserve"># Route 117</t>
+  </si>
+  <si>
     <t xml:space="preserve">TRAINER_LYDIA_1</t>
   </si>
   <si>
@@ -226,6 +232,9 @@
     <t xml:space="preserve">Bubble, Camouflage</t>
   </si>
   <si>
+    <t xml:space="preserve"># Petalburg gym</t>
+  </si>
+  <si>
     <t xml:space="preserve">TRAINER_BERKE</t>
   </si>
   <si>
@@ -268,6 +277,9 @@
     <t xml:space="preserve">Scratch, Uproar, Fury Swipes, Focus Energy</t>
   </si>
   <si>
+    <t xml:space="preserve"># Altering cave (Mary originally in Petalburg Gym)</t>
+  </si>
+  <si>
     <t xml:space="preserve">TRAINER_MARY</t>
   </si>
   <si>
@@ -287,6 +299,9 @@
   </si>
   <si>
     <t xml:space="preserve">{}</t>
+  </si>
+  <si>
+    <t xml:space="preserve"># Petalburg Woods</t>
   </si>
   <si>
     <t xml:space="preserve">TRAINER_GRUNT_PETALBURG_WOODS</t>
@@ -396,10 +411,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E122"/>
+  <dimension ref="A1:E132"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A89" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A120" activeCellId="0" sqref="A120"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A102" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A127" activeCellId="0" sqref="A127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -627,481 +642,460 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="1" t="s">
+      <c r="A25" s="0" t="s">
         <v>18</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B27" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="C27" s="1" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>21</v>
+        <v>2</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
+      </c>
+      <c r="B29" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="C29" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B31" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B32" s="1" t="s">
         <v>26</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B34" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="C34" s="1"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B35" s="1" t="n">
-        <v>4</v>
+        <v>1</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>29</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="B36" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="C36" s="1"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
+      </c>
+      <c r="B37" s="1" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B38" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B39" s="1" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B40" s="1" t="s">
         <v>32</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E41" s="1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B42" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="C42" s="1"/>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="1"/>
-      <c r="B43" s="1"/>
-      <c r="C43" s="1"/>
+      <c r="A43" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B44" s="1"/>
+      <c r="B44" s="1" t="n">
+        <v>5</v>
+      </c>
       <c r="C44" s="1"/>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E45" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="A45" s="1"/>
+      <c r="B45" s="1"/>
+      <c r="C45" s="1"/>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B46" s="1" t="n">
-        <v>5</v>
-      </c>
+      <c r="B46" s="1"/>
       <c r="C46" s="1"/>
-      <c r="D46" s="1"/>
-      <c r="E46" s="1" t="s">
-        <v>36</v>
-      </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B48" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="C48" s="1"/>
+      <c r="D48" s="1"/>
+      <c r="E48" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="B47" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="C47" s="1"/>
-      <c r="E47" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B49" s="1"/>
+      <c r="B49" s="1" t="n">
+        <v>6</v>
+      </c>
       <c r="C49" s="1"/>
-    </row>
-    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E50" s="1" t="s">
-        <v>5</v>
+      <c r="E49" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="1" t="s">
+      <c r="A51" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="B51" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="C51" s="1"/>
-      <c r="D51" s="1"/>
-      <c r="E51" s="1"/>
-    </row>
-    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="1" t="s">
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B52" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="C52" s="1"/>
-      <c r="E52" s="1"/>
-    </row>
-    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="0" t="s">
+      <c r="B53" s="1"/>
+      <c r="C53" s="1"/>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B53" s="0" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="0" t="s">
+      <c r="B55" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="C55" s="1"/>
+      <c r="D55" s="1"/>
+      <c r="E55" s="1"/>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B54" s="0" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="0" t="s">
+      <c r="B56" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="C56" s="1"/>
+      <c r="E56" s="1"/>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="B55" s="0" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="0" t="s">
+      <c r="B57" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="B56" s="0" t="n">
+      <c r="B58" s="0" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="B59" s="0" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="B60" s="0" t="n">
         <v>6</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B59" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C59" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D59" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E59" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B60" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="C60" s="1"/>
-    </row>
-    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="0" t="s">
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B61" s="0" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="B62" s="0" t="n">
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E63" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B64" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="C64" s="1"/>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="0" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B65" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C65" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D65" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E65" s="1" t="s">
+      <c r="B65" s="0" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="1" t="s">
+      <c r="A66" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="B66" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="C66" s="1"/>
-    </row>
-    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="0" t="s">
+      <c r="B66" s="0" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="B67" s="0" t="n">
-        <v>5</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="s">
-        <v>52</v>
+        <v>1</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B70" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C70" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D70" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E70" s="1" t="s">
-        <v>5</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="B70" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="C70" s="1"/>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="1" t="s">
+      <c r="A71" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="B71" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="C71" s="1"/>
-    </row>
-    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="0" t="s">
+      <c r="B71" s="0" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B72" s="0" t="n">
-        <v>6</v>
-      </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="0" t="s">
-        <v>55</v>
+      <c r="A74" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E74" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B75" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C75" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D75" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E75" s="1" t="s">
-        <v>5</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="B75" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="C75" s="1"/>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="1" t="s">
+      <c r="A76" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="B76" s="1" t="n">
+      <c r="B76" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="C76" s="1"/>
-    </row>
-    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="0" t="s">
+    </row>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="B77" s="0" t="n">
-        <v>6</v>
-      </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="0" t="s">
-        <v>58</v>
+      <c r="A79" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E79" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B80" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C80" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D80" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E80" s="1" t="s">
-        <v>5</v>
-      </c>
+        <v>58</v>
+      </c>
+      <c r="B80" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="C80" s="1"/>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="1" t="s">
+      <c r="A81" s="0" t="s">
         <v>59</v>
       </c>
-      <c r="B81" s="1" t="n">
+      <c r="B81" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="C81" s="1"/>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
@@ -1130,315 +1124,361 @@
         <v>61</v>
       </c>
       <c r="B85" s="1" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C85" s="1"/>
-    </row>
-    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="B86" s="0" t="n">
-        <v>5</v>
-      </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="B87" s="0" t="n">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D88" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E88" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B89" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="C89" s="1"/>
+    </row>
+    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="B90" s="0" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B91" s="0" t="n">
         <v>6</v>
       </c>
     </row>
-    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="0" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B90" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C90" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D90" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E90" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B91" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="C91" s="1"/>
-      <c r="E91" s="0" t="s">
+    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="0" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="B92" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="E92" s="0" t="s">
-        <v>67</v>
-      </c>
-    </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="0" t="s">
-        <v>68</v>
+      <c r="A94" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D94" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E94" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B95" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C95" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D95" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E95" s="1" t="s">
-        <v>5</v>
+        <v>66</v>
+      </c>
+      <c r="B95" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="C95" s="1"/>
+      <c r="E95" s="0" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="1" t="s">
+      <c r="A96" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="B96" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="E96" s="0" t="s">
         <v>69</v>
       </c>
-      <c r="B96" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="C96" s="1"/>
-      <c r="E96" s="0" t="s">
+    </row>
+    <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A98" s="0" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="0" t="s">
+    <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A100" s="0" t="s">
         <v>71</v>
-      </c>
-      <c r="B97" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="D97" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="E97" s="0" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A99" s="0" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A100" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B100" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C100" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D100" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E100" s="1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B101" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="C101" s="1"/>
-      <c r="D101" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D101" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E101" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A102" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="E101" s="0" t="s">
+      <c r="B102" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="C102" s="1"/>
+      <c r="E102" s="0" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A103" s="0" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A102" s="0" t="s">
+      <c r="B103" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="D103" s="0" t="s">
         <v>75</v>
       </c>
-      <c r="B102" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="E102" s="0" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A104" s="0" t="s">
-        <v>77</v>
+      <c r="E103" s="0" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B105" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C105" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D105" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="E105" s="0" t="s">
-        <v>5</v>
+        <v>76</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A106" s="0" t="s">
+      <c r="A106" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C106" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D106" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E106" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A107" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B107" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="C107" s="1"/>
+      <c r="D107" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="E107" s="0" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A108" s="0" t="s">
         <v>78</v>
       </c>
-      <c r="B106" s="0" t="n">
-        <v>12</v>
-      </c>
-      <c r="E106" s="0" t="s">
+      <c r="B108" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="E108" s="0" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A107" s="0" t="s">
+    <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A110" s="0" t="s">
         <v>80</v>
       </c>
-      <c r="B107" s="0" t="n">
-        <v>14</v>
-      </c>
-      <c r="E107" s="0" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A109" s="0" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A110" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B110" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C110" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D110" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E110" s="1" t="s">
-        <v>5</v>
-      </c>
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A111" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B111" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="C111" s="1"/>
+      <c r="A111" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B111" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C111" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D111" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E111" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="0" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B112" s="0" t="n">
-        <v>5</v>
+        <v>12</v>
+      </c>
+      <c r="E112" s="0" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="B113" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="B113" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="E113" s="0" t="s">
         <v>84</v>
-      </c>
-    </row>
-    <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A114" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="B114" s="0" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="B115" s="0" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A117" s="0" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A116" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="B116" s="0" t="s">
-        <v>88</v>
-      </c>
-    </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A118" s="0" t="s">
-        <v>89</v>
+      <c r="A118" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B118" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C118" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D118" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E118" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A119" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B119" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C119" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D119" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="E119" s="0" t="s">
-        <v>5</v>
-      </c>
+      <c r="A119" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B119" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="C119" s="1"/>
     </row>
     <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="B120" s="0" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A121" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B121" s="0" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A122" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B122" s="0" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A123" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="B123" s="0" t="s">
         <v>90</v>
       </c>
-      <c r="B120" s="0" t="n">
+    </row>
+    <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A124" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="B124" s="0" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A126" s="0" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A128" s="0" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A129" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B129" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C129" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D129" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E129" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A130" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="B130" s="0" t="n">
         <v>14</v>
       </c>
     </row>
-    <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A122" s="1" t="s">
-        <v>91</v>
+    <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A132" s="1" t="s">
+        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix missing column name
</commit_message>
<xml_diff>
--- a/trainers/trainers.xlsx
+++ b/trainers/trainers.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="125">
   <si>
     <t xml:space="preserve">TRAINER_MAY_ROUTE_103_TREECKO</t>
   </si>
@@ -498,7 +498,7 @@
   <dimension ref="A1:E190"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A150" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B189" activeCellId="0" sqref="B189"/>
+      <selection pane="topLeft" activeCell="E186" activeCellId="0" sqref="E186"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1960,6 +1960,9 @@
       <c r="D185" s="0" t="s">
         <v>4</v>
       </c>
+      <c r="E185" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="186" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="0" t="s">

</xml_diff>

<commit_message>
adjust route 103 east accessibility, fix petalburg woods magma grunt sprite
</commit_message>
<xml_diff>
--- a/trainers/trainers.xlsx
+++ b/trainers/trainers.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="130">
   <si>
     <t xml:space="preserve">TRAINER_MAY_ROUTE_103_TREECKO</t>
   </si>
@@ -346,6 +346,15 @@
     <t xml:space="preserve">Charmander</t>
   </si>
   <si>
+    <t xml:space="preserve">TRAINER_CLASS_TEAM_MAGMA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRAINER_ENCOUNTER_MUSIC_MAGMA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRAINER_PIC_MAGMA_GRUNT_F</t>
+  </si>
+  <si>
     <t xml:space="preserve">TRAINER_LYLE</t>
   </si>
   <si>
@@ -392,6 +401,12 @@
   </si>
   <si>
     <t xml:space="preserve">Poliwag</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Geodude</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anorith</t>
   </si>
   <si>
     <t xml:space="preserve">END</t>
@@ -495,10 +510,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E190"/>
+  <dimension ref="A1:E198"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A144" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A179" activeCellId="0" sqref="A179"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A74" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A74" activeCellId="0" sqref="A74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1735,262 +1750,324 @@
         <v>13</v>
       </c>
     </row>
+    <row r="157" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A157" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="B157" s="0" t="s">
+        <v>108</v>
+      </c>
+    </row>
     <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="0" t="s">
-        <v>108</v>
+        <v>29</v>
+      </c>
+      <c r="B158" s="0" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="0" t="s">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="B159" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C159" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D159" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="E159" s="0" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A160" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="B160" s="0" t="n">
-        <v>10</v>
+        <v>110</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="B161" s="0" t="n">
-        <v>10</v>
+        <v>111</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="0" t="s">
-        <v>109</v>
-      </c>
-      <c r="B162" s="0" t="n">
-        <v>10</v>
+        <v>1</v>
+      </c>
+      <c r="B162" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C162" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D162" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E162" s="0" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="0" t="s">
-        <v>110</v>
+        <v>55</v>
       </c>
       <c r="B163" s="0" t="n">
         <v>10</v>
       </c>
     </row>
+    <row r="164" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A164" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B164" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
     <row r="165" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
+      </c>
+      <c r="B165" s="0" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B166" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C166" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D166" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="E166" s="0" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="167" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A167" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="B167" s="0" t="n">
-        <v>11</v>
+        <v>113</v>
+      </c>
+      <c r="B166" s="0" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="0" t="s">
-        <v>113</v>
-      </c>
-      <c r="B168" s="0" t="n">
-        <v>12</v>
+        <v>114</v>
+      </c>
+    </row>
+    <row r="169" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A169" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B169" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C169" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D169" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E169" s="0" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
+      </c>
+      <c r="B170" s="0" t="n">
+        <v>11</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B171" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C171" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D171" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="E171" s="0" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="172" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A172" s="0" t="s">
-        <v>115</v>
-      </c>
-      <c r="B172" s="0" t="n">
+        <v>116</v>
+      </c>
+      <c r="B171" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="D172" s="0" t="s">
-        <v>101</v>
+    </row>
+    <row r="173" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A173" s="0" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="0" t="s">
-        <v>116</v>
+        <v>1</v>
+      </c>
+      <c r="B174" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C174" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D174" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E174" s="0" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B175" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C175" s="0" t="s">
-        <v>3</v>
+        <v>118</v>
+      </c>
+      <c r="B175" s="0" t="n">
+        <v>12</v>
       </c>
       <c r="D175" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="E175" s="0" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A176" s="0" t="s">
-        <v>117</v>
-      </c>
-      <c r="B176" s="0" t="n">
-        <v>12</v>
+        <v>101</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="0" t="s">
-        <v>118</v>
-      </c>
-      <c r="B177" s="0" t="n">
-        <v>13</v>
+        <v>119</v>
+      </c>
+    </row>
+    <row r="178" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A178" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B178" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C178" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D178" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E178" s="0" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
+      </c>
+      <c r="B179" s="0" t="n">
+        <v>12</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B180" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C180" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D180" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="E180" s="0" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="181" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A181" s="0" t="s">
-        <v>117</v>
-      </c>
-      <c r="B181" s="0" t="n">
+        <v>121</v>
+      </c>
+      <c r="B180" s="0" t="n">
         <v>13</v>
-      </c>
-      <c r="E181" s="0" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="0" t="s">
-        <v>107</v>
-      </c>
-      <c r="B182" s="0" t="n">
-        <v>13</v>
-      </c>
-      <c r="E182" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
+      </c>
+    </row>
+    <row r="183" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A183" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B183" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C183" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D183" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E183" s="0" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="0" t="s">
-        <v>122</v>
+        <v>120</v>
+      </c>
+      <c r="B184" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="E184" s="0" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B185" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C185" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D185" s="0" t="s">
-        <v>4</v>
+        <v>107</v>
+      </c>
+      <c r="B185" s="0" t="n">
+        <v>13</v>
       </c>
       <c r="E185" s="0" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="186" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A186" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="B186" s="0" t="n">
-        <v>15</v>
+        <v>124</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="0" t="s">
-        <v>75</v>
-      </c>
-      <c r="B187" s="0" t="n">
-        <v>13</v>
+        <v>125</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="0" t="s">
-        <v>123</v>
-      </c>
-      <c r="B188" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B188" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C188" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D188" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E188" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="189" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A189" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="B189" s="0" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="190" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A190" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="B190" s="0" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="191" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A191" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="B191" s="0" t="n">
         <v>14</v>
       </c>
     </row>
-    <row r="190" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A190" s="1" t="s">
-        <v>124</v>
+    <row r="193" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A193" s="0" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="194" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A194" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B194" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C194" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D194" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E194" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="195" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A195" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="B195" s="0" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="196" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A196" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="B196" s="0" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="198" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A198" s="1" t="s">
+        <v>129</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adjust petalburg gym, some trainer parties and puddi family stats and moves
</commit_message>
<xml_diff>
--- a/trainers/trainers.xlsx
+++ b/trainers/trainers.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="126">
   <si>
     <t xml:space="preserve">TRAINER_MAY_ROUTE_103_TREECKO</t>
   </si>
@@ -169,21 +169,12 @@
     <t xml:space="preserve">Trifox</t>
   </si>
   <si>
-    <t xml:space="preserve">Eevee</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bellsprout</t>
-  </si>
-  <si>
     <t xml:space="preserve">Pichu</t>
   </si>
   <si>
     <t xml:space="preserve">Azurill</t>
   </si>
   <si>
-    <t xml:space="preserve">Bonsly</t>
-  </si>
-  <si>
     <t xml:space="preserve">TRAINER_DEREK</t>
   </si>
   <si>
@@ -202,18 +193,18 @@
     <t xml:space="preserve">Ralts</t>
   </si>
   <si>
+    <t xml:space="preserve">Natu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRAINER_MELINA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Electrike</t>
+  </si>
+  <si>
     <t xml:space="preserve">Alolan_Rattata</t>
   </si>
   <si>
-    <t xml:space="preserve">TRAINER_MELINA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Electrike</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Poochyena</t>
-  </si>
-  <si>
     <t xml:space="preserve">TRAINER_AISHA</t>
   </si>
   <si>
@@ -292,7 +283,7 @@
     <t xml:space="preserve">Vigoroth</t>
   </si>
   <si>
-    <t xml:space="preserve">Scratch, Uproar, Fury Swipes, Focus Energy</t>
+    <t xml:space="preserve">Scratch, Fury Swipes, Focus Energy</t>
   </si>
   <si>
     <t xml:space="preserve"># Altering cave (Mary originally in Petalburg Gym)</t>
@@ -359,9 +350,6 @@
   </si>
   <si>
     <t xml:space="preserve">Weedle</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ledyba</t>
   </si>
   <si>
     <t xml:space="preserve">TRAINER_JAMES_1</t>
@@ -510,10 +498,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E198"/>
+  <dimension ref="A1:E194"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A74" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A74" activeCellId="0" sqref="A74"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A59" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C59" activeCellId="0" sqref="C59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1057,432 +1045,439 @@
       <c r="E66" s="1"/>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="1" t="s">
+      <c r="A67" s="0" t="s">
         <v>49</v>
       </c>
-      <c r="B67" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="C67" s="1"/>
-      <c r="E67" s="1"/>
+      <c r="B67" s="0" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
         <v>50</v>
       </c>
       <c r="B68" s="0" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B69" s="0" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="0" t="s">
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E71" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B70" s="0" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="0" t="s">
+      <c r="B72" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="C72" s="1"/>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="B71" s="0" t="n">
+      <c r="B73" s="0" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="B74" s="0" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E77" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B78" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="C78" s="1"/>
+    </row>
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="B79" s="0" t="n">
         <v>6</v>
-      </c>
-    </row>
-    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B74" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C74" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D74" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E74" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B75" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="C75" s="1"/>
-    </row>
-    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="B76" s="0" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="B77" s="0" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B80" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C80" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D80" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E80" s="1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E82" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B81" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="C81" s="1"/>
-    </row>
-    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="0" t="s">
+      <c r="B83" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="C83" s="1"/>
+    </row>
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="B82" s="0" t="n">
+      <c r="B84" s="0" t="n">
         <v>6</v>
       </c>
     </row>
-    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="1" t="s">
+    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="0" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B85" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C85" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D85" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E85" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="1" t="s">
+    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D87" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E87" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B86" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="C86" s="1"/>
-    </row>
-    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="B87" s="0" t="n">
+      <c r="B88" s="1" t="n">
         <v>6</v>
       </c>
+      <c r="C88" s="1"/>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="B89" s="0" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="0" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B90" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C90" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D90" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E90" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="1" t="s">
+    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D92" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E92" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B91" s="1" t="n">
+      <c r="B93" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="C91" s="1"/>
-    </row>
-    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="0" t="s">
+      <c r="C93" s="1"/>
+    </row>
+    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="0" t="s">
         <v>66</v>
-      </c>
-      <c r="B92" s="0" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="0" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B95" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C95" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D95" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E95" s="1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="B96" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="C96" s="1"/>
+        <v>1</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D96" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E96" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B97" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="C97" s="1"/>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="s">
-        <v>69</v>
+        <v>68</v>
+      </c>
+      <c r="B98" s="0" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A99" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B99" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C99" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D99" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E99" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A100" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="B100" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="C100" s="1"/>
+      <c r="A99" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B99" s="0" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="0" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A102" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D102" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E102" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A103" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B103" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="C103" s="1"/>
+      <c r="E103" s="0" t="s">
         <v>71</v>
-      </c>
-      <c r="B101" s="0" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A102" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="B102" s="0" t="n">
-        <v>6</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="0" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A105" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B105" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C105" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D105" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E105" s="1" t="s">
-        <v>5</v>
+      <c r="B104" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="E104" s="0" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A106" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="B106" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="C106" s="1"/>
-      <c r="E106" s="0" t="s">
+      <c r="A106" s="0" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A107" s="0" t="s">
+    <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A108" s="0" t="s">
         <v>75</v>
       </c>
-      <c r="B107" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="E107" s="0" t="s">
+    </row>
+    <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A109" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C109" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D109" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E109" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A110" s="1" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A109" s="0" t="s">
+      <c r="B110" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="C110" s="1"/>
+      <c r="E110" s="0" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B111" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="D111" s="0" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A112" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B112" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C112" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D112" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E112" s="1" t="s">
-        <v>5</v>
+      <c r="E111" s="0" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A113" s="1" t="s">
+      <c r="A113" s="0" t="s">
         <v>79</v>
       </c>
-      <c r="B113" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="C113" s="1"/>
-      <c r="E113" s="0" t="s">
-        <v>80</v>
-      </c>
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A114" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="B114" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="D114" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="E114" s="0" t="s">
+      <c r="A114" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B114" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C114" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D114" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E114" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A115" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B115" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="C115" s="1"/>
+      <c r="D115" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="E115" s="0" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="B116" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="E116" s="0" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A117" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B117" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C117" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D117" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E117" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A118" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B118" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="C118" s="1"/>
-      <c r="D118" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="E118" s="0" t="s">
+      <c r="A118" s="0" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B119" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C119" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D119" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E119" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A120" s="0" t="s">
         <v>84</v>
       </c>
-      <c r="B119" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="E119" s="0" t="s">
+      <c r="B120" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="E120" s="0" t="s">
         <v>85</v>
       </c>
     </row>
@@ -1490,385 +1485,377 @@
       <c r="A121" s="0" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A122" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B122" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C122" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D122" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="E122" s="0" t="s">
-        <v>5</v>
+      <c r="B121" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="E121" s="0" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="B123" s="0" t="n">
-        <v>12</v>
-      </c>
-      <c r="E123" s="0" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A124" s="0" t="s">
+    <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A125" s="0" t="s">
         <v>89</v>
       </c>
-      <c r="B124" s="0" t="n">
-        <v>14</v>
-      </c>
-      <c r="E124" s="0" t="s">
-        <v>90</v>
-      </c>
     </row>
     <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A126" s="0" t="s">
-        <v>91</v>
-      </c>
+      <c r="A126" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B126" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C126" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D126" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E126" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A127" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B127" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="C127" s="1"/>
     </row>
     <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="B128" s="0" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A129" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="B129" s="0" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A130" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="B130" s="0" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A129" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B129" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C129" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D129" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E129" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A130" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="B130" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="C130" s="1"/>
     </row>
     <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="B131" s="0" t="s">
         <v>93</v>
-      </c>
-      <c r="B131" s="0" t="n">
-        <v>5</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="0" t="s">
-        <v>27</v>
+        <v>94</v>
       </c>
       <c r="B132" s="0" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A133" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="B133" s="0" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="B134" s="0" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A135" s="0" t="s">
+    <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A136" s="0" t="s">
         <v>97</v>
-      </c>
-      <c r="B135" s="0" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="0" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A139" s="0" t="s">
-        <v>100</v>
+        <v>1</v>
+      </c>
+      <c r="B137" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C137" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D137" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E137" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A138" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="B138" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="D138" s="0" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B140" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C140" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D140" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="E140" s="0" t="s">
-        <v>5</v>
+        <v>99</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="0" t="s">
-        <v>84</v>
-      </c>
-      <c r="B141" s="0" t="n">
-        <v>7</v>
+        <v>1</v>
+      </c>
+      <c r="B141" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C141" s="0" t="s">
+        <v>3</v>
       </c>
       <c r="D141" s="0" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A143" s="0" t="s">
-        <v>102</v>
+        <v>4</v>
+      </c>
+      <c r="E141" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A142" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="B142" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="E142" s="0" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B144" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C144" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D144" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="E144" s="0" t="s">
-        <v>5</v>
+        <v>100</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="B145" s="0" t="n">
-        <v>5</v>
+        <v>1</v>
+      </c>
+      <c r="B145" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C145" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D145" s="0" t="s">
+        <v>4</v>
       </c>
       <c r="E145" s="0" t="s">
-        <v>41</v>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A146" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="B146" s="0" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="0" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A148" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B148" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C148" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D148" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="E148" s="0" t="s">
-        <v>5</v>
+        <v>101</v>
+      </c>
+      <c r="B147" s="0" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="B149" s="0" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A150" s="0" t="s">
-        <v>104</v>
-      </c>
-      <c r="B150" s="0" t="n">
-        <v>6</v>
+        <v>102</v>
+      </c>
+    </row>
+    <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A151" s="0" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="0" t="s">
-        <v>105</v>
+        <v>1</v>
+      </c>
+      <c r="B152" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C152" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D152" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E152" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A153" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="B153" s="0" t="n">
+        <v>13</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="0" t="s">
-        <v>106</v>
+        <v>27</v>
+      </c>
+      <c r="B154" s="0" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="0" t="s">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="B155" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C155" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D155" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="E155" s="0" t="s">
-        <v>5</v>
+        <v>106</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="B156" s="0" t="s">
         <v>107</v>
-      </c>
-      <c r="B156" s="0" t="n">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="157" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A157" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="B157" s="0" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="B158" s="0" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="0" t="s">
-        <v>31</v>
+        <v>1</v>
       </c>
       <c r="B159" s="0" t="s">
-        <v>110</v>
+        <v>2</v>
+      </c>
+      <c r="C159" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D159" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E159" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A160" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="B160" s="0" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="0" t="s">
-        <v>111</v>
+        <v>20</v>
+      </c>
+      <c r="B161" s="0" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B162" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C162" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D162" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="E162" s="0" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="163" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A163" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="B163" s="0" t="n">
+        <v>109</v>
+      </c>
+      <c r="B162" s="0" t="n">
         <v>10</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="B164" s="0" t="n">
-        <v>10</v>
+        <v>110</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="B165" s="0" t="n">
-        <v>10</v>
+        <v>1</v>
+      </c>
+      <c r="B165" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C165" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D165" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E165" s="0" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="0" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B166" s="0" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="168" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A168" s="0" t="s">
-        <v>114</v>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="167" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A167" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="B167" s="0" t="n">
+        <v>12</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B169" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C169" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D169" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="E169" s="0" t="s">
-        <v>5</v>
+        <v>113</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="0" t="s">
-        <v>115</v>
-      </c>
-      <c r="B170" s="0" t="n">
-        <v>11</v>
+        <v>1</v>
+      </c>
+      <c r="B170" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C170" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D170" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E170" s="0" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="0" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B171" s="0" t="n">
         <v>12</v>
       </c>
+      <c r="D171" s="0" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="173" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="0" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1890,184 +1877,151 @@
     </row>
     <row r="175" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="0" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B175" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="D175" s="0" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="177" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A177" s="0" t="s">
-        <v>119</v>
+    </row>
+    <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A176" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="B176" s="0" t="n">
+        <v>13</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B178" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C178" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D178" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="E178" s="0" t="s">
-        <v>5</v>
+        <v>118</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="0" t="s">
-        <v>120</v>
-      </c>
-      <c r="B179" s="0" t="n">
-        <v>12</v>
+        <v>1</v>
+      </c>
+      <c r="B179" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C179" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D179" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E179" s="0" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="0" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="B180" s="0" t="n">
         <v>13</v>
       </c>
-    </row>
-    <row r="182" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A182" s="0" t="s">
-        <v>122</v>
+      <c r="E180" s="0" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="181" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A181" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="B181" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="E181" s="0" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="183" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B183" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C183" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D183" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="E183" s="0" t="s">
-        <v>5</v>
+        <v>121</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="0" t="s">
-        <v>120</v>
-      </c>
-      <c r="B184" s="0" t="n">
-        <v>13</v>
+        <v>1</v>
+      </c>
+      <c r="B184" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C184" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D184" s="0" t="s">
+        <v>4</v>
       </c>
       <c r="E184" s="0" t="s">
-        <v>123</v>
+        <v>5</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="0" t="s">
-        <v>107</v>
+        <v>40</v>
       </c>
       <c r="B185" s="0" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="186" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A186" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="B186" s="0" t="n">
         <v>13</v>
-      </c>
-      <c r="E185" s="0" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="0" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="188" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A188" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B188" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C188" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D188" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="E188" s="0" t="s">
-        <v>5</v>
+        <v>122</v>
+      </c>
+      <c r="B187" s="0" t="n">
+        <v>14</v>
       </c>
     </row>
     <row r="189" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="B189" s="0" t="n">
-        <v>15</v>
+        <v>115</v>
       </c>
     </row>
     <row r="190" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A190" s="0" t="s">
-        <v>75</v>
-      </c>
-      <c r="B190" s="0" t="n">
-        <v>13</v>
+        <v>1</v>
+      </c>
+      <c r="B190" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C190" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D190" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E190" s="0" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A191" s="0" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B191" s="0" t="n">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="193" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A193" s="0" t="s">
-        <v>119</v>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="192" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A192" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="B192" s="0" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="194" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A194" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B194" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C194" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D194" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="E194" s="0" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="195" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A195" s="0" t="s">
-        <v>127</v>
-      </c>
-      <c r="B195" s="0" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="196" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A196" s="0" t="s">
-        <v>128</v>
-      </c>
-      <c r="B196" s="0" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="198" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A198" s="1" t="s">
-        <v>129</v>
+      <c r="A194" s="1" t="s">
+        <v>125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix more typos, disregard extra tabs in snippet matching
</commit_message>
<xml_diff>
--- a/trainers/trainers.xlsx
+++ b/trainers/trainers.xlsx
@@ -79,7 +79,7 @@
     <t xml:space="preserve"># Route 102</t>
   </si>
   <si>
-    <t xml:space="preserve">TRAINER_CALVIN</t>
+    <t xml:space="preserve">TRAINER_CALVIN_1</t>
   </si>
   <si>
     <t xml:space="preserve">Poochyena</t>
@@ -527,8 +527,8 @@
   </sheetPr>
   <dimension ref="A1:E202"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A175" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B217" activeCellId="0" sqref="B217"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A28" activeCellId="0" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
route 116 trainers, rusturf tunnel grunt
</commit_message>
<xml_diff>
--- a/trainers/trainers.xlsx
+++ b/trainers/trainers.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="164">
   <si>
     <t xml:space="preserve">TRAINER_MAY_ROUTE_103_TREECKO</t>
   </si>
@@ -422,6 +422,93 @@
   </si>
   <si>
     <t xml:space="preserve">Anorith</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRAINER_GRUNT_RUSTURF_TUNNEL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Charmeleon</t>
+  </si>
+  <si>
+    <t xml:space="preserve"># Route 116</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRAINER_JOEY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aron</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nidoran</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRAINER_JOSE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ledian</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRAINER_KAREN_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eevee</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRAINER_CLARK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rhyhorn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mawile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRAINER_JOHNSON</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grimey</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Koffing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRAINER_DEVAN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alolan_Geodude</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Larvitar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRAINER_SARAH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Galarian_Minicorn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alolan_Meowth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRAINER_DAWSON</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Delcatty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRAINER_JERRY_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Slakoth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Slowpoke</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRAINER_JANICE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pikachu</t>
   </si>
   <si>
     <t xml:space="preserve">END</t>
@@ -525,10 +612,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E202"/>
+  <dimension ref="A1:E265"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A28" activeCellId="0" sqref="A28"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A182" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A205" activeCellId="0" sqref="A205"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2111,8 +2198,407 @@
       </c>
     </row>
     <row r="202" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A202" s="1" t="s">
+      <c r="A202" s="0" t="s">
         <v>134</v>
+      </c>
+    </row>
+    <row r="203" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A203" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B203" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C203" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D203" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E203" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="204" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A204" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="B204" s="0" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="206" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A206" s="0" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="208" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A208" s="0" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="209" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A209" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B209" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C209" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D209" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E209" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="210" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A210" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="B210" s="0" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="211" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A211" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="B211" s="0" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="213" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A213" s="0" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="214" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A214" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B214" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C214" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D214" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E214" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="215" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A215" s="0" t="s">
+        <v>141</v>
+      </c>
+      <c r="B215" s="0" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="217" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A217" s="0" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="218" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A218" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B218" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C218" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D218" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E218" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="219" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A219" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="B219" s="0" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="220" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A220" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="B220" s="0" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="222" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A222" s="0" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="223" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A223" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B223" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C223" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D223" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E223" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="224" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A224" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="B224" s="0" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="225" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A225" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="B225" s="0" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="227" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A227" s="0" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="228" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A228" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B228" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C228" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D228" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E228" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="229" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A229" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="B229" s="0" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="230" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A230" s="0" t="s">
+        <v>149</v>
+      </c>
+      <c r="B230" s="0" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="232" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A232" s="0" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="233" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A233" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B233" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C233" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D233" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E233" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="234" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A234" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="B234" s="0" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="235" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A235" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="B235" s="0" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="237" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A237" s="0" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="238" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A238" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B238" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C238" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D238" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E238" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="239" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A239" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="B239" s="0" t="n">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="240" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A240" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="B240" s="0" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="242" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A242" s="0" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="243" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A243" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B243" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C243" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D243" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E243" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="244" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A244" s="0" t="s">
+        <v>157</v>
+      </c>
+      <c r="B244" s="0" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="246" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A246" s="0" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="247" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A247" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B247" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C247" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D247" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E247" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="248" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A248" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="B248" s="0" t="n">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="249" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A249" s="0" t="s">
+        <v>160</v>
+      </c>
+      <c r="B249" s="0" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="251" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A251" s="0" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="252" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A252" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B252" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C252" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D252" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E252" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="253" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A253" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B253" s="0" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="254" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A254" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="B254" s="0" t="n">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="265" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A265" s="1" t="s">
+        <v>163</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix nidoran species names
</commit_message>
<xml_diff>
--- a/trainers/trainers.xlsx
+++ b/trainers/trainers.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="165">
   <si>
     <t xml:space="preserve">TRAINER_MAY_ROUTE_103_TREECKO</t>
   </si>
@@ -439,7 +439,7 @@
     <t xml:space="preserve">Aron</t>
   </si>
   <si>
-    <t xml:space="preserve">Nidoran</t>
+    <t xml:space="preserve">Nidoran_M</t>
   </si>
   <si>
     <t xml:space="preserve">TRAINER_JOSE</t>
@@ -449,6 +449,9 @@
   </si>
   <si>
     <t xml:space="preserve">TRAINER_KAREN_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nidoran_F</t>
   </si>
   <si>
     <t xml:space="preserve">Eevee</t>
@@ -615,7 +618,7 @@
   <dimension ref="A1:E265"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A182" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A205" activeCellId="0" sqref="A205"/>
+      <selection pane="topLeft" activeCell="H219" activeCellId="0" sqref="H219"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2324,7 +2327,7 @@
     </row>
     <row r="219" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A219" s="0" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="B219" s="0" t="n">
         <v>16</v>
@@ -2332,7 +2335,7 @@
     </row>
     <row r="220" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A220" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B220" s="0" t="n">
         <v>16</v>
@@ -2340,7 +2343,7 @@
     </row>
     <row r="222" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A222" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="223" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2362,7 +2365,7 @@
     </row>
     <row r="224" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A224" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B224" s="0" t="n">
         <v>16</v>
@@ -2370,7 +2373,7 @@
     </row>
     <row r="225" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A225" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B225" s="0" t="n">
         <v>17</v>
@@ -2378,7 +2381,7 @@
     </row>
     <row r="227" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A227" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="228" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2400,7 +2403,7 @@
     </row>
     <row r="229" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A229" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B229" s="0" t="n">
         <v>17</v>
@@ -2408,7 +2411,7 @@
     </row>
     <row r="230" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A230" s="0" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B230" s="0" t="n">
         <v>17</v>
@@ -2416,7 +2419,7 @@
     </row>
     <row r="232" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A232" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="233" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2438,7 +2441,7 @@
     </row>
     <row r="234" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A234" s="0" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B234" s="0" t="n">
         <v>16</v>
@@ -2446,7 +2449,7 @@
     </row>
     <row r="235" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A235" s="0" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B235" s="0" t="n">
         <v>17</v>
@@ -2454,7 +2457,7 @@
     </row>
     <row r="237" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A237" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="238" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2476,7 +2479,7 @@
     </row>
     <row r="239" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A239" s="0" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B239" s="0" t="n">
         <v>19</v>
@@ -2484,7 +2487,7 @@
     </row>
     <row r="240" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A240" s="0" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B240" s="0" t="n">
         <v>20</v>
@@ -2492,7 +2495,7 @@
     </row>
     <row r="242" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A242" s="0" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="243" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2514,7 +2517,7 @@
     </row>
     <row r="244" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A244" s="0" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B244" s="0" t="n">
         <v>21</v>
@@ -2522,7 +2525,7 @@
     </row>
     <row r="246" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A246" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="247" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2544,7 +2547,7 @@
     </row>
     <row r="248" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A248" s="0" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B248" s="0" t="n">
         <v>23</v>
@@ -2552,7 +2555,7 @@
     </row>
     <row r="249" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A249" s="0" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B249" s="0" t="n">
         <v>21</v>
@@ -2560,7 +2563,7 @@
     </row>
     <row r="251" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A251" s="0" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="252" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2590,7 +2593,7 @@
     </row>
     <row r="254" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A254" s="0" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B254" s="0" t="n">
         <v>23</v>
@@ -2598,7 +2601,7 @@
     </row>
     <row r="265" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A265" s="1" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
rustboro gym trainers & roxanne
</commit_message>
<xml_diff>
--- a/trainers/trainers.xlsx
+++ b/trainers/trainers.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="175">
   <si>
     <t xml:space="preserve">TRAINER_MAY_ROUTE_103_TREECKO</t>
   </si>
@@ -512,6 +512,36 @@
   </si>
   <si>
     <t xml:space="preserve">Pikachu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRAINER_JOSH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRAINER_TOMMY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bonsly</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRAINER_MARC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Onix</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRAINER_ROXANNE_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rock Tomb, Mud Sport, Defense Curl, Magnitude</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Relicanth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rock Tomb, Mud Sport, Water Gun, Harden</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{ITEM_SUPER_POTION, ITEM_SUPER_POTION, ITEM_NONE, ITEM_NONE}</t>
   </si>
   <si>
     <t xml:space="preserve">END</t>
@@ -615,10 +645,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E265"/>
+  <dimension ref="A1:E287"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A182" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H219" activeCellId="0" sqref="H219"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A258" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D277" activeCellId="0" sqref="D277"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2230,378 +2260,574 @@
         <v>18</v>
       </c>
     </row>
+    <row r="205" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A205" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="B205" s="0" t="s">
+        <v>109</v>
+      </c>
+    </row>
     <row r="206" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A206" s="0" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="208" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A208" s="0" t="s">
-        <v>137</v>
+        <v>42</v>
+      </c>
+      <c r="B206" s="0" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="207" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A207" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="B207" s="0" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="209" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A209" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B209" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C209" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D209" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="E209" s="0" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="210" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A210" s="0" t="s">
-        <v>138</v>
-      </c>
-      <c r="B210" s="0" t="n">
-        <v>15</v>
+        <v>136</v>
       </c>
     </row>
     <row r="211" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A211" s="0" t="s">
-        <v>139</v>
-      </c>
-      <c r="B211" s="0" t="n">
-        <v>16</v>
+        <v>137</v>
+      </c>
+    </row>
+    <row r="212" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A212" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B212" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C212" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D212" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E212" s="0" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="213" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A213" s="0" t="s">
-        <v>140</v>
+        <v>138</v>
+      </c>
+      <c r="B213" s="0" t="n">
+        <v>15</v>
       </c>
     </row>
     <row r="214" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A214" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B214" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C214" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D214" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="E214" s="0" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="215" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A215" s="0" t="s">
-        <v>141</v>
-      </c>
-      <c r="B215" s="0" t="n">
-        <v>18</v>
+        <v>139</v>
+      </c>
+      <c r="B214" s="0" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="216" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A216" s="0" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="217" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A217" s="0" t="s">
-        <v>142</v>
+        <v>1</v>
+      </c>
+      <c r="B217" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C217" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D217" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E217" s="0" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="218" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A218" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B218" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C218" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D218" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="E218" s="0" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="219" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A219" s="0" t="s">
-        <v>143</v>
-      </c>
-      <c r="B219" s="0" t="n">
-        <v>16</v>
+        <v>141</v>
+      </c>
+      <c r="B218" s="0" t="n">
+        <v>18</v>
       </c>
     </row>
     <row r="220" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A220" s="0" t="s">
-        <v>144</v>
-      </c>
-      <c r="B220" s="0" t="n">
-        <v>16</v>
+        <v>142</v>
+      </c>
+    </row>
+    <row r="221" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A221" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B221" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C221" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D221" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E221" s="0" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="222" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A222" s="0" t="s">
-        <v>145</v>
+        <v>143</v>
+      </c>
+      <c r="B222" s="0" t="n">
+        <v>16</v>
       </c>
     </row>
     <row r="223" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A223" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B223" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C223" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D223" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="E223" s="0" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="224" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A224" s="0" t="s">
-        <v>146</v>
-      </c>
-      <c r="B224" s="0" t="n">
+        <v>144</v>
+      </c>
+      <c r="B223" s="0" t="n">
         <v>16</v>
       </c>
     </row>
     <row r="225" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A225" s="0" t="s">
-        <v>147</v>
-      </c>
-      <c r="B225" s="0" t="n">
-        <v>17</v>
+        <v>145</v>
+      </c>
+    </row>
+    <row r="226" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A226" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B226" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C226" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D226" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E226" s="0" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="227" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A227" s="0" t="s">
-        <v>148</v>
+        <v>146</v>
+      </c>
+      <c r="B227" s="0" t="n">
+        <v>16</v>
       </c>
     </row>
     <row r="228" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A228" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B228" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C228" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D228" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="E228" s="0" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="229" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A229" s="0" t="s">
-        <v>149</v>
-      </c>
-      <c r="B229" s="0" t="n">
+        <v>147</v>
+      </c>
+      <c r="B228" s="0" t="n">
         <v>17</v>
       </c>
     </row>
     <row r="230" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A230" s="0" t="s">
-        <v>150</v>
-      </c>
-      <c r="B230" s="0" t="n">
-        <v>17</v>
+        <v>148</v>
+      </c>
+    </row>
+    <row r="231" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A231" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B231" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C231" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D231" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E231" s="0" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="232" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A232" s="0" t="s">
-        <v>151</v>
+        <v>149</v>
+      </c>
+      <c r="B232" s="0" t="n">
+        <v>17</v>
       </c>
     </row>
     <row r="233" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A233" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B233" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C233" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D233" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="E233" s="0" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="234" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A234" s="0" t="s">
-        <v>152</v>
-      </c>
-      <c r="B234" s="0" t="n">
-        <v>16</v>
+        <v>150</v>
+      </c>
+      <c r="B233" s="0" t="n">
+        <v>17</v>
       </c>
     </row>
     <row r="235" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A235" s="0" t="s">
-        <v>153</v>
-      </c>
-      <c r="B235" s="0" t="n">
-        <v>17</v>
+        <v>151</v>
+      </c>
+    </row>
+    <row r="236" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A236" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B236" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C236" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D236" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E236" s="0" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="237" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A237" s="0" t="s">
-        <v>154</v>
+        <v>152</v>
+      </c>
+      <c r="B237" s="0" t="n">
+        <v>16</v>
       </c>
     </row>
     <row r="238" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A238" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B238" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C238" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D238" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="E238" s="0" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="239" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A239" s="0" t="s">
-        <v>155</v>
-      </c>
-      <c r="B239" s="0" t="n">
-        <v>19</v>
+        <v>153</v>
+      </c>
+      <c r="B238" s="0" t="n">
+        <v>17</v>
       </c>
     </row>
     <row r="240" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A240" s="0" t="s">
-        <v>156</v>
-      </c>
-      <c r="B240" s="0" t="n">
-        <v>20</v>
+        <v>154</v>
+      </c>
+    </row>
+    <row r="241" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A241" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B241" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C241" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D241" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E241" s="0" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="242" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A242" s="0" t="s">
-        <v>157</v>
+        <v>155</v>
+      </c>
+      <c r="B242" s="0" t="n">
+        <v>19</v>
       </c>
     </row>
     <row r="243" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A243" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B243" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C243" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D243" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="E243" s="0" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="244" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A244" s="0" t="s">
-        <v>158</v>
-      </c>
-      <c r="B244" s="0" t="n">
-        <v>21</v>
+        <v>156</v>
+      </c>
+      <c r="B243" s="0" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="245" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A245" s="0" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="246" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A246" s="0" t="s">
-        <v>159</v>
+        <v>1</v>
+      </c>
+      <c r="B246" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C246" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D246" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E246" s="0" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="247" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A247" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B247" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C247" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D247" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="E247" s="0" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="248" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A248" s="0" t="s">
-        <v>160</v>
-      </c>
-      <c r="B248" s="0" t="n">
-        <v>23</v>
+        <v>158</v>
+      </c>
+      <c r="B247" s="0" t="n">
+        <v>21</v>
       </c>
     </row>
     <row r="249" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A249" s="0" t="s">
-        <v>161</v>
-      </c>
-      <c r="B249" s="0" t="n">
-        <v>21</v>
+        <v>159</v>
+      </c>
+    </row>
+    <row r="250" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A250" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B250" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C250" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D250" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E250" s="0" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="251" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A251" s="0" t="s">
-        <v>162</v>
+        <v>160</v>
+      </c>
+      <c r="B251" s="0" t="n">
+        <v>23</v>
       </c>
     </row>
     <row r="252" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A252" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B252" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C252" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D252" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="E252" s="0" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="253" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A253" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="B253" s="0" t="n">
-        <v>22</v>
+        <v>161</v>
+      </c>
+      <c r="B252" s="0" t="n">
+        <v>21</v>
       </c>
     </row>
     <row r="254" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A254" s="0" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="255" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A255" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B255" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C255" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D255" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E255" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="256" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A256" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B256" s="0" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="257" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A257" s="0" t="s">
         <v>163</v>
       </c>
-      <c r="B254" s="0" t="n">
+      <c r="B257" s="0" t="n">
         <v>23</v>
       </c>
     </row>
+    <row r="259" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A259" s="0" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="260" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A260" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B260" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C260" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D260" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E260" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="261" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A261" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="B261" s="0" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="262" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A262" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="B262" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="D262" s="0" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="264" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A264" s="0" t="s">
+        <v>165</v>
+      </c>
+    </row>
     <row r="265" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A265" s="1" t="s">
-        <v>164</v>
+      <c r="A265" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B265" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C265" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D265" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E265" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="266" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A266" s="0" t="s">
+        <v>166</v>
+      </c>
+      <c r="B266" s="0" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="267" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A267" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="B267" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="D267" s="0" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="269" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A269" s="0" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="270" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A270" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B270" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C270" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D270" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E270" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="271" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A271" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="B271" s="0" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="272" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A272" s="0" t="s">
+        <v>168</v>
+      </c>
+      <c r="B272" s="0" t="n">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="274" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A274" s="0" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="275" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A275" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B275" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C275" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D275" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E275" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="276" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A276" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="B276" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="E276" s="0" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="277" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A277" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="B277" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="E277" s="0" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="278" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A278" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="B278" s="0" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="287" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A287" s="1" t="s">
+        <v>174</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
start building framework for fixed-ability and shiny enemy pokemon
</commit_message>
<xml_diff>
--- a/trainers/trainers.xlsx
+++ b/trainers/trainers.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="646" uniqueCount="190">
   <si>
     <t xml:space="preserve">TRAINER_MAY_ROUTE_103_TREECKO</t>
   </si>
@@ -38,6 +38,12 @@
   </si>
   <si>
     <t xml:space="preserve">moves</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ability</t>
+  </si>
+  <si>
+    <t xml:space="preserve">shiny</t>
   </si>
   <si>
     <t xml:space="preserve">Torchic</t>
@@ -684,10 +690,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E314"/>
+  <dimension ref="A1:G314"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A281" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A310" activeCellId="0" sqref="A310"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A283" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E310" activeCellId="0" sqref="E310:G310"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -716,25 +722,31 @@
       <c r="E2" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="F2" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B3" s="1" t="n">
         <v>5</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -753,22 +765,28 @@
       <c r="E6" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="F6" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G6" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B7" s="1" t="n">
         <v>5</v>
       </c>
       <c r="C7" s="1"/>
       <c r="E7" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -787,22 +805,28 @@
       <c r="E10" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="F10" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G10" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B11" s="1" t="n">
         <v>5</v>
       </c>
       <c r="C11" s="1"/>
       <c r="E11" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -821,22 +845,28 @@
       <c r="E14" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="F14" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G14" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B15" s="1" t="n">
         <v>5</v>
       </c>
       <c r="C15" s="1"/>
       <c r="E15" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -855,22 +885,28 @@
       <c r="E18" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="F18" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G18" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B19" s="1" t="n">
         <v>5</v>
       </c>
       <c r="C19" s="1"/>
       <c r="E19" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -889,27 +925,33 @@
       <c r="E22" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="F22" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G22" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B23" s="1" t="n">
         <v>5</v>
       </c>
       <c r="C23" s="1"/>
       <c r="E23" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -928,22 +970,28 @@
       <c r="E28" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="F28" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G28" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B29" s="1" t="n">
         <v>3</v>
       </c>
       <c r="C29" s="1"/>
       <c r="E29" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -962,10 +1010,16 @@
       <c r="E32" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="F32" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G32" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B33" s="1" t="n">
         <v>3</v>
@@ -974,7 +1028,7 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B34" s="0" t="n">
         <v>4</v>
@@ -982,7 +1036,7 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1001,10 +1055,16 @@
       <c r="E37" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="F37" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G37" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B38" s="1" t="n">
         <v>4</v>
@@ -1013,12 +1073,12 @@
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1034,24 +1094,30 @@
       <c r="D43" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="E43" s="0" t="s">
-        <v>5</v>
+      <c r="E43" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F43" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G43" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B44" s="0" t="n">
         <v>7</v>
       </c>
       <c r="D44" s="0" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1067,24 +1133,30 @@
       <c r="D47" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="E47" s="0" t="s">
-        <v>5</v>
+      <c r="E47" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F47" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G47" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B48" s="0" t="n">
         <v>5</v>
       </c>
       <c r="E48" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1100,13 +1172,19 @@
       <c r="D51" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="E51" s="0" t="s">
-        <v>5</v>
+      <c r="E51" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F51" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G51" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B52" s="0" t="n">
         <v>5</v>
@@ -1114,7 +1192,7 @@
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B53" s="0" t="n">
         <v>6</v>
@@ -1122,12 +1200,12 @@
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1146,10 +1224,16 @@
       <c r="E58" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="F58" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G58" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B59" s="1" t="n">
         <v>5</v>
@@ -1160,31 +1244,31 @@
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1203,10 +1287,16 @@
       <c r="E65" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="F65" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G65" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B66" s="1" t="n">
         <v>5</v>
@@ -1215,7 +1305,7 @@
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B67" s="1" t="n">
         <v>4</v>
@@ -1223,31 +1313,31 @@
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1266,17 +1356,23 @@
       <c r="E73" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="F73" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G73" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B74" s="1" t="n">
         <v>7</v>
       </c>
       <c r="C74" s="1"/>
       <c r="E74" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1286,7 +1382,7 @@
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
@@ -1307,10 +1403,16 @@
       <c r="E77" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="F77" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G77" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B78" s="1" t="n">
         <v>6</v>
@@ -1318,29 +1420,29 @@
       <c r="C78" s="1"/>
       <c r="D78" s="1"/>
       <c r="E78" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B79" s="1" t="n">
         <v>5</v>
       </c>
       <c r="C79" s="1"/>
       <c r="E79" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1359,10 +1461,16 @@
       <c r="E84" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="F84" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G84" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B85" s="1" t="n">
         <v>6</v>
@@ -1371,7 +1479,7 @@
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B86" s="0" t="n">
         <v>6</v>
@@ -1379,44 +1487,44 @@
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B87" s="0" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B88" s="0" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B89" s="0" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B90" s="0" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B94" s="1"/>
       <c r="C94" s="1"/>
@@ -1437,10 +1545,16 @@
       <c r="E95" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="F95" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G95" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B96" s="1" t="n">
         <v>6</v>
@@ -1451,7 +1565,7 @@
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B97" s="0" t="n">
         <v>6</v>
@@ -1459,7 +1573,7 @@
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B98" s="0" t="n">
         <v>6</v>
@@ -1467,7 +1581,7 @@
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1486,10 +1600,16 @@
       <c r="E101" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="F101" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G101" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="1" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B102" s="1" t="n">
         <v>7</v>
@@ -1498,7 +1618,7 @@
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B103" s="0" t="n">
         <v>7</v>
@@ -1506,7 +1626,7 @@
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B104" s="0" t="n">
         <v>7</v>
@@ -1514,7 +1634,7 @@
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1533,10 +1653,16 @@
       <c r="E107" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="F107" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G107" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="1" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B108" s="1" t="n">
         <v>7</v>
@@ -1545,7 +1671,7 @@
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="0" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B109" s="0" t="n">
         <v>8</v>
@@ -1553,7 +1679,7 @@
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="1" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1572,10 +1698,16 @@
       <c r="E112" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="F112" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G112" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="1" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B113" s="1" t="n">
         <v>8</v>
@@ -1584,7 +1716,7 @@
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="0" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B114" s="0" t="n">
         <v>8</v>
@@ -1592,7 +1724,7 @@
     </row>
     <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="0" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1611,10 +1743,16 @@
       <c r="E117" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="F117" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G117" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B118" s="1" t="n">
         <v>7</v>
@@ -1623,7 +1761,7 @@
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="0" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B119" s="0" t="n">
         <v>8</v>
@@ -1631,7 +1769,7 @@
     </row>
     <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="0" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1650,10 +1788,16 @@
       <c r="E122" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="F122" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G122" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="1" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B123" s="1" t="n">
         <v>9</v>
@@ -1662,7 +1806,7 @@
     </row>
     <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1681,10 +1825,16 @@
       <c r="E126" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="F126" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G126" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="1" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B127" s="1" t="n">
         <v>7</v>
@@ -1693,7 +1843,7 @@
     </row>
     <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="0" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B128" s="0" t="n">
         <v>7</v>
@@ -1701,7 +1851,7 @@
     </row>
     <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="0" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B129" s="0" t="n">
         <v>8</v>
@@ -1709,7 +1859,7 @@
     </row>
     <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="0" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1728,38 +1878,44 @@
       <c r="E132" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="F132" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G132" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B133" s="1" t="n">
         <v>8</v>
       </c>
       <c r="C133" s="1"/>
       <c r="E133" s="0" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="0" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B134" s="0" t="n">
         <v>8</v>
       </c>
       <c r="E134" s="0" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="0" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="0" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1778,44 +1934,50 @@
       <c r="E139" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="F139" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G139" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="1" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B140" s="1" t="n">
         <v>9</v>
       </c>
       <c r="C140" s="1"/>
       <c r="E140" s="0" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B141" s="0" t="n">
         <v>10</v>
       </c>
       <c r="D141" s="0" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="E141" s="0" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="0" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B142" s="0" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="0" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1834,36 +1996,42 @@
       <c r="E145" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="F145" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G145" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B146" s="1" t="n">
         <v>9</v>
       </c>
       <c r="C146" s="1"/>
       <c r="D146" s="0" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="E146" s="0" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="0" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B147" s="0" t="n">
         <v>10</v>
       </c>
       <c r="E147" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="0" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1879,48 +2047,54 @@
       <c r="D150" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="E150" s="0" t="s">
-        <v>5</v>
+      <c r="E150" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F150" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G150" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="0" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B151" s="0" t="n">
         <v>12</v>
       </c>
       <c r="E151" s="0" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B152" s="0" t="n">
         <v>14</v>
       </c>
       <c r="E152" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="0" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B153" s="0" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="0" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1936,13 +2110,19 @@
       <c r="D158" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="E158" s="0" t="s">
-        <v>5</v>
+      <c r="E158" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F158" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G158" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="0" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B159" s="0" t="n">
         <v>13</v>
@@ -1950,31 +2130,31 @@
     </row>
     <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B160" s="0" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="0" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B161" s="0" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="0" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B162" s="0" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="0" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1990,46 +2170,52 @@
       <c r="D165" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="E165" s="0" t="s">
-        <v>5</v>
+      <c r="E165" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F165" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G165" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B166" s="0" t="n">
         <v>10</v>
       </c>
       <c r="E166" s="0" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="0" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B167" s="0" t="n">
         <v>10</v>
       </c>
       <c r="E167" s="0" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="0" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B168" s="0" t="n">
         <v>10</v>
       </c>
       <c r="E168" s="0" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="0" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2045,13 +2231,19 @@
       <c r="D171" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="E171" s="0" t="s">
-        <v>5</v>
+      <c r="E171" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F171" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G171" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="0" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B172" s="0" t="n">
         <v>11</v>
@@ -2059,7 +2251,7 @@
     </row>
     <row r="173" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="0" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B173" s="0" t="n">
         <v>12</v>
@@ -2067,7 +2259,7 @@
     </row>
     <row r="175" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="0" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2083,24 +2275,30 @@
       <c r="D176" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="E176" s="0" t="s">
-        <v>5</v>
+      <c r="E176" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F176" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G176" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="0" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B177" s="0" t="n">
         <v>13</v>
       </c>
       <c r="D177" s="0" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="0" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2116,13 +2314,19 @@
       <c r="D180" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="E180" s="0" t="s">
-        <v>5</v>
+      <c r="E180" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F180" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G180" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="0" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B181" s="0" t="n">
         <v>12</v>
@@ -2130,7 +2334,7 @@
     </row>
     <row r="182" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="0" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B182" s="0" t="n">
         <v>13</v>
@@ -2138,7 +2342,7 @@
     </row>
     <row r="184" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="0" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2154,35 +2358,41 @@
       <c r="D185" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="E185" s="0" t="s">
-        <v>5</v>
+      <c r="E185" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F185" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G185" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="186" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="0" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B186" s="0" t="n">
         <v>14</v>
       </c>
       <c r="E186" s="0" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="0" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B187" s="0" t="n">
         <v>14</v>
       </c>
       <c r="E187" s="0" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
     </row>
     <row r="189" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="0" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
     </row>
     <row r="190" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2198,13 +2408,19 @@
       <c r="D190" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="E190" s="0" t="s">
-        <v>5</v>
+      <c r="E190" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F190" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G190" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A191" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B191" s="0" t="n">
         <v>15</v>
@@ -2212,7 +2428,7 @@
     </row>
     <row r="192" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A192" s="0" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B192" s="0" t="n">
         <v>13</v>
@@ -2220,7 +2436,7 @@
     </row>
     <row r="193" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A193" s="0" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="B193" s="0" t="n">
         <v>14</v>
@@ -2228,12 +2444,12 @@
     </row>
     <row r="195" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A195" s="0" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
     </row>
     <row r="197" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="0" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
     </row>
     <row r="198" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2249,13 +2465,19 @@
       <c r="D198" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="E198" s="0" t="s">
-        <v>5</v>
+      <c r="E198" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F198" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G198" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="199" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="0" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="B199" s="0" t="n">
         <v>7</v>
@@ -2263,7 +2485,7 @@
     </row>
     <row r="200" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="0" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="B200" s="0" t="n">
         <v>7</v>
@@ -2271,7 +2493,7 @@
     </row>
     <row r="202" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A202" s="0" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
     </row>
     <row r="203" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2287,13 +2509,19 @@
       <c r="D203" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="E203" s="0" t="s">
-        <v>5</v>
+      <c r="E203" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F203" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G203" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="204" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A204" s="0" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B204" s="0" t="n">
         <v>18</v>
@@ -2301,36 +2529,36 @@
     </row>
     <row r="205" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A205" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B205" s="0" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="206" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A206" s="0" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B206" s="0" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="207" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A207" s="0" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B207" s="0" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="209" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A209" s="0" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
     </row>
     <row r="211" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A211" s="0" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
     </row>
     <row r="212" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2346,13 +2574,19 @@
       <c r="D212" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="E212" s="0" t="s">
-        <v>5</v>
+      <c r="E212" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F212" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G212" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="213" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A213" s="0" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B213" s="0" t="n">
         <v>15</v>
@@ -2360,7 +2594,7 @@
     </row>
     <row r="214" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A214" s="0" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B214" s="0" t="n">
         <v>16</v>
@@ -2368,7 +2602,7 @@
     </row>
     <row r="216" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A216" s="0" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
     </row>
     <row r="217" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2384,13 +2618,19 @@
       <c r="D217" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="E217" s="0" t="s">
-        <v>5</v>
+      <c r="E217" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F217" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G217" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="218" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A218" s="0" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B218" s="0" t="n">
         <v>18</v>
@@ -2398,7 +2638,7 @@
     </row>
     <row r="220" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A220" s="0" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
     </row>
     <row r="221" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2414,13 +2654,19 @@
       <c r="D221" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="E221" s="0" t="s">
-        <v>5</v>
+      <c r="E221" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F221" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G221" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="222" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A222" s="0" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="B222" s="0" t="n">
         <v>16</v>
@@ -2428,7 +2674,7 @@
     </row>
     <row r="223" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A223" s="0" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="B223" s="0" t="n">
         <v>16</v>
@@ -2436,7 +2682,7 @@
     </row>
     <row r="225" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A225" s="0" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
     </row>
     <row r="226" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2452,13 +2698,19 @@
       <c r="D226" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="E226" s="0" t="s">
-        <v>5</v>
+      <c r="E226" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F226" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G226" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="227" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A227" s="0" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="B227" s="0" t="n">
         <v>16</v>
@@ -2466,7 +2718,7 @@
     </row>
     <row r="228" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A228" s="0" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="B228" s="0" t="n">
         <v>17</v>
@@ -2474,7 +2726,7 @@
     </row>
     <row r="230" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A230" s="0" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
     </row>
     <row r="231" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2490,13 +2742,19 @@
       <c r="D231" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="E231" s="0" t="s">
-        <v>5</v>
+      <c r="E231" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F231" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G231" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="232" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A232" s="0" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B232" s="0" t="n">
         <v>17</v>
@@ -2504,7 +2762,7 @@
     </row>
     <row r="233" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A233" s="0" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="B233" s="0" t="n">
         <v>17</v>
@@ -2512,7 +2770,7 @@
     </row>
     <row r="235" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A235" s="0" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
     <row r="236" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2528,13 +2786,19 @@
       <c r="D236" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="E236" s="0" t="s">
-        <v>5</v>
+      <c r="E236" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F236" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G236" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="237" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A237" s="0" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="B237" s="0" t="n">
         <v>16</v>
@@ -2542,7 +2806,7 @@
     </row>
     <row r="238" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A238" s="0" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B238" s="0" t="n">
         <v>17</v>
@@ -2550,7 +2814,7 @@
     </row>
     <row r="240" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A240" s="0" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
     <row r="241" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2566,13 +2830,19 @@
       <c r="D241" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="E241" s="0" t="s">
-        <v>5</v>
+      <c r="E241" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F241" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G241" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="242" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A242" s="0" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="B242" s="0" t="n">
         <v>19</v>
@@ -2580,7 +2850,7 @@
     </row>
     <row r="243" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A243" s="0" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="B243" s="0" t="n">
         <v>20</v>
@@ -2588,7 +2858,7 @@
     </row>
     <row r="245" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A245" s="0" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
     </row>
     <row r="246" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2604,13 +2874,19 @@
       <c r="D246" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="E246" s="0" t="s">
-        <v>5</v>
+      <c r="E246" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F246" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G246" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="247" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A247" s="0" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="B247" s="0" t="n">
         <v>21</v>
@@ -2618,7 +2894,7 @@
     </row>
     <row r="249" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A249" s="0" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
     </row>
     <row r="250" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2634,13 +2910,19 @@
       <c r="D250" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="E250" s="0" t="s">
-        <v>5</v>
+      <c r="E250" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F250" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G250" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="251" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A251" s="0" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="B251" s="0" t="n">
         <v>23</v>
@@ -2648,7 +2930,7 @@
     </row>
     <row r="252" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A252" s="0" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="B252" s="0" t="n">
         <v>21</v>
@@ -2656,7 +2938,7 @@
     </row>
     <row r="254" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A254" s="0" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
     </row>
     <row r="255" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2672,13 +2954,19 @@
       <c r="D255" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="E255" s="0" t="s">
-        <v>5</v>
+      <c r="E255" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F255" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G255" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="256" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A256" s="0" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B256" s="0" t="n">
         <v>22</v>
@@ -2686,7 +2974,7 @@
     </row>
     <row r="257" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A257" s="0" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="B257" s="0" t="n">
         <v>23</v>
@@ -2694,12 +2982,12 @@
     </row>
     <row r="259" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A259" s="0" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
     </row>
     <row r="261" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A261" s="0" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
     </row>
     <row r="262" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2715,13 +3003,19 @@
       <c r="D262" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="E262" s="0" t="s">
-        <v>5</v>
+      <c r="E262" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F262" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G262" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="263" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A263" s="0" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="B263" s="0" t="n">
         <v>18</v>
@@ -2729,18 +3023,18 @@
     </row>
     <row r="264" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A264" s="0" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="B264" s="0" t="n">
         <v>18</v>
       </c>
       <c r="D264" s="0" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="266" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A266" s="0" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
     </row>
     <row r="267" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2756,13 +3050,19 @@
       <c r="D267" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="E267" s="0" t="s">
-        <v>5</v>
+      <c r="E267" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F267" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G267" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="268" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A268" s="0" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B268" s="0" t="n">
         <v>18</v>
@@ -2770,18 +3070,18 @@
     </row>
     <row r="269" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A269" s="0" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B269" s="0" t="n">
         <v>19</v>
       </c>
       <c r="D269" s="0" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="271" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A271" s="0" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
     </row>
     <row r="272" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2797,13 +3097,19 @@
       <c r="D272" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="E272" s="0" t="s">
-        <v>5</v>
+      <c r="E272" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F272" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G272" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="273" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A273" s="0" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B273" s="0" t="n">
         <v>17</v>
@@ -2811,7 +3117,7 @@
     </row>
     <row r="274" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A274" s="0" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B274" s="0" t="n">
         <v>19</v>
@@ -2819,7 +3125,7 @@
     </row>
     <row r="276" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A276" s="0" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
     </row>
     <row r="277" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2835,48 +3141,54 @@
       <c r="D277" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="E277" s="0" t="s">
-        <v>5</v>
+      <c r="E277" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F277" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G277" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="278" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A278" s="0" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="B278" s="0" t="n">
         <v>20</v>
       </c>
       <c r="E278" s="0" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
     </row>
     <row r="279" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A279" s="0" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B279" s="0" t="n">
         <v>22</v>
       </c>
       <c r="E279" s="0" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
     </row>
     <row r="280" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A280" s="0" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B280" s="0" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
     </row>
     <row r="282" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A282" s="0" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
     </row>
     <row r="284" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A284" s="0" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
     </row>
     <row r="285" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2892,24 +3204,30 @@
       <c r="D285" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="E285" s="0" t="s">
-        <v>5</v>
+      <c r="E285" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F285" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G285" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="286" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A286" s="0" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="B286" s="0" t="n">
         <v>20</v>
       </c>
       <c r="D286" s="0" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="287" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A287" s="0" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="B287" s="0" t="n">
         <v>20</v>
@@ -2917,7 +3235,7 @@
     </row>
     <row r="289" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A289" s="0" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
     </row>
     <row r="290" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2933,24 +3251,30 @@
       <c r="D290" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="E290" s="0" t="s">
-        <v>5</v>
+      <c r="E290" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F290" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G290" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="291" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A291" s="0" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="B291" s="0" t="n">
         <v>20</v>
       </c>
       <c r="D291" s="0" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="292" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A292" s="0" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="B292" s="0" t="n">
         <v>20</v>
@@ -2958,7 +3282,7 @@
     </row>
     <row r="294" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A294" s="0" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
     </row>
     <row r="295" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2974,24 +3298,30 @@
       <c r="D295" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="E295" s="0" t="s">
-        <v>5</v>
+      <c r="E295" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F295" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G295" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="296" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A296" s="0" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B296" s="0" t="n">
         <v>20</v>
       </c>
       <c r="D296" s="0" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="297" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A297" s="0" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="B297" s="0" t="n">
         <v>20</v>
@@ -2999,7 +3329,7 @@
     </row>
     <row r="299" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A299" s="0" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
     </row>
     <row r="300" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3015,24 +3345,30 @@
       <c r="D300" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="E300" s="0" t="s">
-        <v>5</v>
+      <c r="E300" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F300" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G300" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="301" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A301" s="0" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="B301" s="0" t="n">
         <v>20</v>
       </c>
       <c r="D301" s="0" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="302" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A302" s="0" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="B302" s="0" t="n">
         <v>20</v>
@@ -3040,7 +3376,7 @@
     </row>
     <row r="304" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A304" s="0" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
     </row>
     <row r="305" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3056,24 +3392,30 @@
       <c r="D305" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="E305" s="0" t="s">
-        <v>5</v>
+      <c r="E305" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F305" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G305" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="306" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A306" s="0" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="B306" s="0" t="n">
         <v>20</v>
       </c>
       <c r="D306" s="0" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="307" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A307" s="0" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="B307" s="0" t="n">
         <v>20</v>
@@ -3081,7 +3423,7 @@
     </row>
     <row r="309" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A309" s="0" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
     </row>
     <row r="310" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3097,24 +3439,30 @@
       <c r="D310" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="E310" s="0" t="s">
-        <v>5</v>
+      <c r="E310" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F310" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G310" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="311" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A311" s="0" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B311" s="0" t="n">
         <v>20</v>
       </c>
       <c r="D311" s="0" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="312" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A312" s="0" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="B312" s="0" t="n">
         <v>20</v>
@@ -3122,7 +3470,7 @@
     </row>
     <row r="314" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A314" s="0" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
continue building custom trainer party type
</commit_message>
<xml_diff>
--- a/trainers/trainers.xlsx
+++ b/trainers/trainers.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="646" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="645" uniqueCount="189">
   <si>
     <t xml:space="preserve">TRAINER_MAY_ROUTE_103_TREECKO</t>
   </si>
@@ -47,9 +47,6 @@
   </si>
   <si>
     <t xml:space="preserve">Torchic</t>
-  </si>
-  <si>
-    <t xml:space="preserve">chesto berry</t>
   </si>
   <si>
     <t xml:space="preserve">Scratch, Growl</t>
@@ -692,8 +689,8 @@
   </sheetPr>
   <dimension ref="A1:G314"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A283" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E310" activeCellId="0" sqref="E310:G310"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -737,16 +734,14 @@
         <v>5</v>
       </c>
       <c r="C3" s="1"/>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="1"/>
+      <c r="E3" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -774,19 +769,19 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B7" s="1" t="n">
         <v>5</v>
       </c>
       <c r="C7" s="1"/>
       <c r="E7" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -814,19 +809,19 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B11" s="1" t="n">
         <v>5</v>
       </c>
       <c r="C11" s="1"/>
       <c r="E11" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -861,12 +856,12 @@
       </c>
       <c r="C15" s="1"/>
       <c r="E15" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -894,19 +889,19 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B19" s="1" t="n">
         <v>5</v>
       </c>
       <c r="C19" s="1"/>
       <c r="E19" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -934,24 +929,24 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B23" s="1" t="n">
         <v>5</v>
       </c>
       <c r="C23" s="1"/>
       <c r="E23" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -979,19 +974,19 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B29" s="1" t="n">
         <v>3</v>
       </c>
       <c r="C29" s="1"/>
       <c r="E29" s="0" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1019,7 +1014,7 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B33" s="1" t="n">
         <v>3</v>
@@ -1028,7 +1023,7 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B34" s="0" t="n">
         <v>4</v>
@@ -1036,7 +1031,7 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1064,7 +1059,7 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B38" s="1" t="n">
         <v>4</v>
@@ -1073,12 +1068,12 @@
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1106,18 +1101,18 @@
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="B44" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="D44" s="0" t="s">
         <v>31</v>
-      </c>
-      <c r="B44" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="D44" s="0" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1145,18 +1140,18 @@
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="B48" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="E48" s="0" t="s">
         <v>34</v>
-      </c>
-      <c r="B48" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="E48" s="0" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1184,7 +1179,7 @@
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B52" s="0" t="n">
         <v>5</v>
@@ -1192,7 +1187,7 @@
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B53" s="0" t="n">
         <v>6</v>
@@ -1200,12 +1195,12 @@
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1233,7 +1228,7 @@
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B59" s="1" t="n">
         <v>5</v>
@@ -1244,31 +1239,31 @@
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B60" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B60" s="1" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B61" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="B61" s="1" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B62" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="B62" s="1" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1296,7 +1291,7 @@
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B66" s="1" t="n">
         <v>5</v>
@@ -1305,7 +1300,7 @@
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B67" s="1" t="n">
         <v>4</v>
@@ -1313,31 +1308,31 @@
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1365,14 +1360,14 @@
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B74" s="1" t="n">
         <v>7</v>
       </c>
       <c r="C74" s="1"/>
       <c r="E74" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1382,7 +1377,7 @@
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
@@ -1412,7 +1407,7 @@
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B78" s="1" t="n">
         <v>6</v>
@@ -1420,29 +1415,29 @@
       <c r="C78" s="1"/>
       <c r="D78" s="1"/>
       <c r="E78" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B79" s="1" t="n">
         <v>5</v>
       </c>
       <c r="C79" s="1"/>
       <c r="E79" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1470,7 +1465,7 @@
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B85" s="1" t="n">
         <v>6</v>
@@ -1479,7 +1474,7 @@
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B86" s="0" t="n">
         <v>6</v>
@@ -1487,44 +1482,44 @@
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B87" s="0" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B88" s="0" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B89" s="0" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="B90" s="0" t="s">
         <v>66</v>
-      </c>
-      <c r="B90" s="0" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B94" s="1"/>
       <c r="C94" s="1"/>
@@ -1554,7 +1549,7 @@
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B96" s="1" t="n">
         <v>6</v>
@@ -1565,7 +1560,7 @@
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B97" s="0" t="n">
         <v>6</v>
@@ -1573,7 +1568,7 @@
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B98" s="0" t="n">
         <v>6</v>
@@ -1581,7 +1576,7 @@
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1609,7 +1604,7 @@
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B102" s="1" t="n">
         <v>7</v>
@@ -1618,7 +1613,7 @@
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="0" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B103" s="0" t="n">
         <v>7</v>
@@ -1626,7 +1621,7 @@
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="0" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B104" s="0" t="n">
         <v>7</v>
@@ -1634,7 +1629,7 @@
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1662,7 +1657,7 @@
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B108" s="1" t="n">
         <v>7</v>
@@ -1671,7 +1666,7 @@
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="0" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B109" s="0" t="n">
         <v>8</v>
@@ -1679,7 +1674,7 @@
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1707,7 +1702,7 @@
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B113" s="1" t="n">
         <v>8</v>
@@ -1716,7 +1711,7 @@
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B114" s="0" t="n">
         <v>8</v>
@@ -1724,7 +1719,7 @@
     </row>
     <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="0" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1752,7 +1747,7 @@
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B118" s="1" t="n">
         <v>7</v>
@@ -1761,7 +1756,7 @@
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="0" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B119" s="0" t="n">
         <v>8</v>
@@ -1769,7 +1764,7 @@
     </row>
     <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="0" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1797,7 +1792,7 @@
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B123" s="1" t="n">
         <v>9</v>
@@ -1806,7 +1801,7 @@
     </row>
     <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="0" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1834,7 +1829,7 @@
     </row>
     <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B127" s="1" t="n">
         <v>7</v>
@@ -1843,7 +1838,7 @@
     </row>
     <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="0" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B128" s="0" t="n">
         <v>7</v>
@@ -1851,7 +1846,7 @@
     </row>
     <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="0" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B129" s="0" t="n">
         <v>8</v>
@@ -1859,7 +1854,7 @@
     </row>
     <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="0" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1887,35 +1882,35 @@
     </row>
     <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B133" s="1" t="n">
         <v>8</v>
       </c>
       <c r="C133" s="1"/>
       <c r="E133" s="0" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="0" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B134" s="0" t="n">
         <v>8</v>
       </c>
       <c r="E134" s="0" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="0" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="0" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1943,41 +1938,41 @@
     </row>
     <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B140" s="1" t="n">
         <v>9</v>
       </c>
       <c r="C140" s="1"/>
       <c r="E140" s="0" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="0" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B141" s="0" t="n">
         <v>10</v>
       </c>
       <c r="D141" s="0" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E141" s="0" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="B142" s="0" t="s">
         <v>66</v>
-      </c>
-      <c r="B142" s="0" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="0" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2005,33 +2000,33 @@
     </row>
     <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B146" s="1" t="n">
         <v>9</v>
       </c>
       <c r="C146" s="1"/>
       <c r="D146" s="0" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E146" s="0" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B147" s="0" t="n">
         <v>10</v>
       </c>
       <c r="E147" s="0" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="0" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2059,42 +2054,42 @@
     </row>
     <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="0" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B151" s="0" t="n">
         <v>12</v>
       </c>
       <c r="E151" s="0" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="0" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B152" s="0" t="n">
         <v>14</v>
       </c>
       <c r="E152" s="0" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="0" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B153" s="0" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="0" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="0" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2122,7 +2117,7 @@
     </row>
     <row r="159" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="0" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B159" s="0" t="n">
         <v>13</v>
@@ -2130,31 +2125,31 @@
     </row>
     <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="0" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B160" s="0" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B161" s="0" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="0" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B162" s="0" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="0" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2182,40 +2177,40 @@
     </row>
     <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="0" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B166" s="0" t="n">
         <v>10</v>
       </c>
       <c r="E166" s="0" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="0" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B167" s="0" t="n">
         <v>10</v>
       </c>
       <c r="E167" s="0" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="0" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B168" s="0" t="n">
         <v>10</v>
       </c>
       <c r="E168" s="0" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="0" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2243,7 +2238,7 @@
     </row>
     <row r="172" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="0" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B172" s="0" t="n">
         <v>11</v>
@@ -2251,7 +2246,7 @@
     </row>
     <row r="173" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="0" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B173" s="0" t="n">
         <v>12</v>
@@ -2259,7 +2254,7 @@
     </row>
     <row r="175" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="0" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2287,18 +2282,18 @@
     </row>
     <row r="177" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="0" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B177" s="0" t="n">
         <v>13</v>
       </c>
       <c r="D177" s="0" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="0" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2326,7 +2321,7 @@
     </row>
     <row r="181" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="0" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B181" s="0" t="n">
         <v>12</v>
@@ -2334,7 +2329,7 @@
     </row>
     <row r="182" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="0" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B182" s="0" t="n">
         <v>13</v>
@@ -2342,7 +2337,7 @@
     </row>
     <row r="184" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="0" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2370,29 +2365,29 @@
     </row>
     <row r="186" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="0" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B186" s="0" t="n">
         <v>14</v>
       </c>
       <c r="E186" s="0" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="0" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B187" s="0" t="n">
         <v>14</v>
       </c>
       <c r="E187" s="0" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="189" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="0" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="190" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2420,7 +2415,7 @@
     </row>
     <row r="191" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A191" s="0" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B191" s="0" t="n">
         <v>15</v>
@@ -2428,7 +2423,7 @@
     </row>
     <row r="192" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A192" s="0" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B192" s="0" t="n">
         <v>13</v>
@@ -2436,7 +2431,7 @@
     </row>
     <row r="193" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A193" s="0" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B193" s="0" t="n">
         <v>14</v>
@@ -2444,12 +2439,12 @@
     </row>
     <row r="195" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A195" s="0" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="197" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="0" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="198" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2477,7 +2472,7 @@
     </row>
     <row r="199" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="0" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B199" s="0" t="n">
         <v>7</v>
@@ -2485,7 +2480,7 @@
     </row>
     <row r="200" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="0" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B200" s="0" t="n">
         <v>7</v>
@@ -2493,7 +2488,7 @@
     </row>
     <row r="202" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A202" s="0" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="203" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2521,7 +2516,7 @@
     </row>
     <row r="204" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A204" s="0" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B204" s="0" t="n">
         <v>18</v>
@@ -2529,36 +2524,36 @@
     </row>
     <row r="205" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A205" s="0" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B205" s="0" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="206" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A206" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B206" s="0" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="207" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A207" s="0" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B207" s="0" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="209" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A209" s="0" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="211" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A211" s="0" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="212" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2586,7 +2581,7 @@
     </row>
     <row r="213" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A213" s="0" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B213" s="0" t="n">
         <v>15</v>
@@ -2594,7 +2589,7 @@
     </row>
     <row r="214" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A214" s="0" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B214" s="0" t="n">
         <v>16</v>
@@ -2602,7 +2597,7 @@
     </row>
     <row r="216" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A216" s="0" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="217" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2630,7 +2625,7 @@
     </row>
     <row r="218" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A218" s="0" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B218" s="0" t="n">
         <v>18</v>
@@ -2638,7 +2633,7 @@
     </row>
     <row r="220" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A220" s="0" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="221" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2666,7 +2661,7 @@
     </row>
     <row r="222" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A222" s="0" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B222" s="0" t="n">
         <v>16</v>
@@ -2674,7 +2669,7 @@
     </row>
     <row r="223" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A223" s="0" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B223" s="0" t="n">
         <v>16</v>
@@ -2682,7 +2677,7 @@
     </row>
     <row r="225" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A225" s="0" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="226" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2710,7 +2705,7 @@
     </row>
     <row r="227" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A227" s="0" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B227" s="0" t="n">
         <v>16</v>
@@ -2718,7 +2713,7 @@
     </row>
     <row r="228" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A228" s="0" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B228" s="0" t="n">
         <v>17</v>
@@ -2726,7 +2721,7 @@
     </row>
     <row r="230" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A230" s="0" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="231" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2754,7 +2749,7 @@
     </row>
     <row r="232" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A232" s="0" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B232" s="0" t="n">
         <v>17</v>
@@ -2762,7 +2757,7 @@
     </row>
     <row r="233" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A233" s="0" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B233" s="0" t="n">
         <v>17</v>
@@ -2770,7 +2765,7 @@
     </row>
     <row r="235" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A235" s="0" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="236" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2798,7 +2793,7 @@
     </row>
     <row r="237" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A237" s="0" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B237" s="0" t="n">
         <v>16</v>
@@ -2806,7 +2801,7 @@
     </row>
     <row r="238" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A238" s="0" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B238" s="0" t="n">
         <v>17</v>
@@ -2814,7 +2809,7 @@
     </row>
     <row r="240" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A240" s="0" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="241" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2842,7 +2837,7 @@
     </row>
     <row r="242" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A242" s="0" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B242" s="0" t="n">
         <v>19</v>
@@ -2850,7 +2845,7 @@
     </row>
     <row r="243" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A243" s="0" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B243" s="0" t="n">
         <v>20</v>
@@ -2858,7 +2853,7 @@
     </row>
     <row r="245" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A245" s="0" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="246" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2886,7 +2881,7 @@
     </row>
     <row r="247" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A247" s="0" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B247" s="0" t="n">
         <v>21</v>
@@ -2894,7 +2889,7 @@
     </row>
     <row r="249" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A249" s="0" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="250" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2922,7 +2917,7 @@
     </row>
     <row r="251" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A251" s="0" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B251" s="0" t="n">
         <v>23</v>
@@ -2930,7 +2925,7 @@
     </row>
     <row r="252" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A252" s="0" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B252" s="0" t="n">
         <v>21</v>
@@ -2938,7 +2933,7 @@
     </row>
     <row r="254" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A254" s="0" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="255" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2974,7 +2969,7 @@
     </row>
     <row r="257" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A257" s="0" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B257" s="0" t="n">
         <v>23</v>
@@ -2982,12 +2977,12 @@
     </row>
     <row r="259" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A259" s="0" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="261" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A261" s="0" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="262" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3015,7 +3010,7 @@
     </row>
     <row r="263" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A263" s="0" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B263" s="0" t="n">
         <v>18</v>
@@ -3023,18 +3018,18 @@
     </row>
     <row r="264" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A264" s="0" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B264" s="0" t="n">
         <v>18</v>
       </c>
       <c r="D264" s="0" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="266" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A266" s="0" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="267" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3062,7 +3057,7 @@
     </row>
     <row r="268" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A268" s="0" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B268" s="0" t="n">
         <v>18</v>
@@ -3070,18 +3065,18 @@
     </row>
     <row r="269" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A269" s="0" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B269" s="0" t="n">
         <v>19</v>
       </c>
       <c r="D269" s="0" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="271" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A271" s="0" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="272" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3109,7 +3104,7 @@
     </row>
     <row r="273" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A273" s="0" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B273" s="0" t="n">
         <v>17</v>
@@ -3117,7 +3112,7 @@
     </row>
     <row r="274" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A274" s="0" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B274" s="0" t="n">
         <v>19</v>
@@ -3125,7 +3120,7 @@
     </row>
     <row r="276" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A276" s="0" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="277" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3153,42 +3148,42 @@
     </row>
     <row r="278" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A278" s="0" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B278" s="0" t="n">
         <v>20</v>
       </c>
       <c r="E278" s="0" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="279" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A279" s="0" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B279" s="0" t="n">
         <v>22</v>
       </c>
       <c r="E279" s="0" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="280" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A280" s="0" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B280" s="0" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="282" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A282" s="0" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="284" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A284" s="0" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="285" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3216,18 +3211,18 @@
     </row>
     <row r="286" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A286" s="0" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B286" s="0" t="n">
         <v>20</v>
       </c>
       <c r="D286" s="0" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="287" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A287" s="0" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B287" s="0" t="n">
         <v>20</v>
@@ -3235,7 +3230,7 @@
     </row>
     <row r="289" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A289" s="0" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="290" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3263,18 +3258,18 @@
     </row>
     <row r="291" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A291" s="0" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B291" s="0" t="n">
         <v>20</v>
       </c>
       <c r="D291" s="0" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="292" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A292" s="0" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B292" s="0" t="n">
         <v>20</v>
@@ -3282,7 +3277,7 @@
     </row>
     <row r="294" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A294" s="0" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="295" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3310,18 +3305,18 @@
     </row>
     <row r="296" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A296" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B296" s="0" t="n">
         <v>20</v>
       </c>
       <c r="D296" s="0" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="297" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A297" s="0" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B297" s="0" t="n">
         <v>20</v>
@@ -3329,7 +3324,7 @@
     </row>
     <row r="299" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A299" s="0" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="300" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3357,18 +3352,18 @@
     </row>
     <row r="301" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A301" s="0" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B301" s="0" t="n">
         <v>20</v>
       </c>
       <c r="D301" s="0" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="302" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A302" s="0" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B302" s="0" t="n">
         <v>20</v>
@@ -3376,7 +3371,7 @@
     </row>
     <row r="304" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A304" s="0" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="305" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3404,18 +3399,18 @@
     </row>
     <row r="306" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A306" s="0" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B306" s="0" t="n">
         <v>20</v>
       </c>
       <c r="D306" s="0" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="307" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A307" s="0" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B307" s="0" t="n">
         <v>20</v>
@@ -3423,7 +3418,7 @@
     </row>
     <row r="309" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A309" s="0" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="310" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3451,18 +3446,18 @@
     </row>
     <row r="311" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A311" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B311" s="0" t="n">
         <v>20</v>
       </c>
       <c r="D311" s="0" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="312" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A312" s="0" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B312" s="0" t="n">
         <v>20</v>
@@ -3470,7 +3465,7 @@
     </row>
     <row r="314" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A314" s="0" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
test fixed shiny enemies
</commit_message>
<xml_diff>
--- a/trainers/trainers.xlsx
+++ b/trainers/trainers.xlsx
@@ -46,31 +46,31 @@
     <t xml:space="preserve">shiny</t>
   </si>
   <si>
+    <t xml:space="preserve">Scratch, Growl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRAINER_MAY_ROUTE_103_TORCHIC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mudkip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tackle, Growl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRAINER_MAY_ROUTE_103_MUDKIP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Treecko</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pound, Leer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRAINER_BRENDAN_ROUTE_103_TREECKO</t>
+  </si>
+  <si>
     <t xml:space="preserve">Torchic</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Scratch, Growl</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TRAINER_MAY_ROUTE_103_TORCHIC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mudkip</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tackle, Growl</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TRAINER_MAY_ROUTE_103_MUDKIP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Treecko</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pound, Leer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TRAINER_BRENDAN_ROUTE_103_TREECKO</t>
   </si>
   <si>
     <t xml:space="preserve">TRAINER_BRENDAN_ROUTE_103_TORCHIC</t>
@@ -689,8 +689,8 @@
   </sheetPr>
   <dimension ref="A1:G314"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A228" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F247" activeCellId="0" sqref="F247"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -728,7 +728,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="B3" s="1" t="n">
         <v>5</v>
@@ -736,12 +736,12 @@
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -769,19 +769,19 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B7" s="1" t="n">
         <v>5</v>
       </c>
       <c r="C7" s="1"/>
       <c r="E7" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -809,19 +809,19 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B11" s="1" t="n">
         <v>5</v>
       </c>
       <c r="C11" s="1"/>
       <c r="E11" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -849,14 +849,14 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="B15" s="1" t="n">
         <v>5</v>
       </c>
       <c r="C15" s="1"/>
       <c r="E15" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -889,14 +889,14 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B19" s="1" t="n">
         <v>5</v>
       </c>
       <c r="C19" s="1"/>
       <c r="E19" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -929,14 +929,14 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B23" s="1" t="n">
         <v>5</v>
       </c>
       <c r="C23" s="1"/>
       <c r="E23" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1427,7 +1427,7 @@
       </c>
       <c r="C79" s="1"/>
       <c r="E79" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2886,6 +2886,9 @@
       <c r="B247" s="0" t="n">
         <v>21</v>
       </c>
+      <c r="G247" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="249" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A249" s="0" t="s">
@@ -2961,7 +2964,7 @@
     </row>
     <row r="256" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A256" s="0" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="B256" s="0" t="n">
         <v>22</v>

</xml_diff>

<commit_message>
fix rusturf tunnel hiker
</commit_message>
<xml_diff>
--- a/trainers/trainers.xlsx
+++ b/trainers/trainers.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="645" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="645" uniqueCount="190">
   <si>
     <t xml:space="preserve">TRAINER_MAY_ROUTE_103_TREECKO</t>
   </si>
@@ -419,6 +419,9 @@
   </si>
   <si>
     <t xml:space="preserve"># Rusturf tunnel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRAINER_MIKE_1</t>
   </si>
   <si>
     <t xml:space="preserve">Geodude</t>
@@ -689,8 +692,8 @@
   </sheetPr>
   <dimension ref="A1:G314"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A228" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F247" activeCellId="0" sqref="F247"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A174" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B201" activeCellId="0" sqref="B201"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2444,7 +2447,7 @@
     </row>
     <row r="197" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="0" t="s">
-        <v>123</v>
+        <v>133</v>
       </c>
     </row>
     <row r="198" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2472,23 +2475,23 @@
     </row>
     <row r="199" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B199" s="0" t="n">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B200" s="0" t="n">
-        <v>7</v>
+        <v>13</v>
       </c>
     </row>
     <row r="202" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A202" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="203" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2516,7 +2519,7 @@
     </row>
     <row r="204" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A204" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B204" s="0" t="n">
         <v>18</v>
@@ -2548,12 +2551,12 @@
     </row>
     <row r="209" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A209" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="211" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A211" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="212" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2581,7 +2584,7 @@
     </row>
     <row r="213" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A213" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B213" s="0" t="n">
         <v>15</v>
@@ -2589,7 +2592,7 @@
     </row>
     <row r="214" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A214" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B214" s="0" t="n">
         <v>16</v>
@@ -2597,7 +2600,7 @@
     </row>
     <row r="216" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A216" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="217" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2625,7 +2628,7 @@
     </row>
     <row r="218" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A218" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B218" s="0" t="n">
         <v>18</v>
@@ -2633,7 +2636,7 @@
     </row>
     <row r="220" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A220" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="221" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2661,7 +2664,7 @@
     </row>
     <row r="222" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A222" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B222" s="0" t="n">
         <v>16</v>
@@ -2669,7 +2672,7 @@
     </row>
     <row r="223" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A223" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B223" s="0" t="n">
         <v>16</v>
@@ -2677,7 +2680,7 @@
     </row>
     <row r="225" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A225" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="226" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2705,7 +2708,7 @@
     </row>
     <row r="227" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A227" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B227" s="0" t="n">
         <v>16</v>
@@ -2713,7 +2716,7 @@
     </row>
     <row r="228" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A228" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B228" s="0" t="n">
         <v>17</v>
@@ -2721,7 +2724,7 @@
     </row>
     <row r="230" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A230" s="0" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="231" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2749,7 +2752,7 @@
     </row>
     <row r="232" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A232" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B232" s="0" t="n">
         <v>17</v>
@@ -2757,7 +2760,7 @@
     </row>
     <row r="233" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A233" s="0" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B233" s="0" t="n">
         <v>17</v>
@@ -2765,7 +2768,7 @@
     </row>
     <row r="235" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A235" s="0" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="236" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2793,7 +2796,7 @@
     </row>
     <row r="237" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A237" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B237" s="0" t="n">
         <v>16</v>
@@ -2801,7 +2804,7 @@
     </row>
     <row r="238" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A238" s="0" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B238" s="0" t="n">
         <v>17</v>
@@ -2809,7 +2812,7 @@
     </row>
     <row r="240" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A240" s="0" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="241" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2837,7 +2840,7 @@
     </row>
     <row r="242" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A242" s="0" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B242" s="0" t="n">
         <v>19</v>
@@ -2845,7 +2848,7 @@
     </row>
     <row r="243" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A243" s="0" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B243" s="0" t="n">
         <v>20</v>
@@ -2853,7 +2856,7 @@
     </row>
     <row r="245" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A245" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="246" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2881,7 +2884,7 @@
     </row>
     <row r="247" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A247" s="0" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B247" s="0" t="n">
         <v>21</v>
@@ -2892,7 +2895,7 @@
     </row>
     <row r="249" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A249" s="0" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="250" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2920,7 +2923,7 @@
     </row>
     <row r="251" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A251" s="0" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B251" s="0" t="n">
         <v>23</v>
@@ -2928,7 +2931,7 @@
     </row>
     <row r="252" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A252" s="0" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B252" s="0" t="n">
         <v>21</v>
@@ -2936,7 +2939,7 @@
     </row>
     <row r="254" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A254" s="0" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="255" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2972,7 +2975,7 @@
     </row>
     <row r="257" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A257" s="0" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B257" s="0" t="n">
         <v>23</v>
@@ -2980,12 +2983,12 @@
     </row>
     <row r="259" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A259" s="0" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="261" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A261" s="0" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="262" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3013,7 +3016,7 @@
     </row>
     <row r="263" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A263" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B263" s="0" t="n">
         <v>18</v>
@@ -3021,7 +3024,7 @@
     </row>
     <row r="264" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A264" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B264" s="0" t="n">
         <v>18</v>
@@ -3032,7 +3035,7 @@
     </row>
     <row r="266" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A266" s="0" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="267" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3060,7 +3063,7 @@
     </row>
     <row r="268" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A268" s="0" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B268" s="0" t="n">
         <v>18</v>
@@ -3068,7 +3071,7 @@
     </row>
     <row r="269" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A269" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B269" s="0" t="n">
         <v>19</v>
@@ -3079,7 +3082,7 @@
     </row>
     <row r="271" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A271" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="272" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3107,7 +3110,7 @@
     </row>
     <row r="273" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A273" s="0" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B273" s="0" t="n">
         <v>17</v>
@@ -3115,7 +3118,7 @@
     </row>
     <row r="274" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A274" s="0" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B274" s="0" t="n">
         <v>19</v>
@@ -3123,7 +3126,7 @@
     </row>
     <row r="276" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A276" s="0" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="277" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3151,24 +3154,24 @@
     </row>
     <row r="278" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A278" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B278" s="0" t="n">
         <v>20</v>
       </c>
       <c r="E278" s="0" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row r="279" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A279" s="0" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B279" s="0" t="n">
         <v>22</v>
       </c>
       <c r="E279" s="0" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="280" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3176,17 +3179,17 @@
         <v>65</v>
       </c>
       <c r="B280" s="0" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="282" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A282" s="0" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
     </row>
     <row r="284" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A284" s="0" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="285" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3214,7 +3217,7 @@
     </row>
     <row r="286" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A286" s="0" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B286" s="0" t="n">
         <v>20</v>
@@ -3225,7 +3228,7 @@
     </row>
     <row r="287" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A287" s="0" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B287" s="0" t="n">
         <v>20</v>
@@ -3233,7 +3236,7 @@
     </row>
     <row r="289" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A289" s="0" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="290" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3261,7 +3264,7 @@
     </row>
     <row r="291" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A291" s="0" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B291" s="0" t="n">
         <v>20</v>
@@ -3272,7 +3275,7 @@
     </row>
     <row r="292" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A292" s="0" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B292" s="0" t="n">
         <v>20</v>
@@ -3280,7 +3283,7 @@
     </row>
     <row r="294" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A294" s="0" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="295" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3319,7 +3322,7 @@
     </row>
     <row r="297" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A297" s="0" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B297" s="0" t="n">
         <v>20</v>
@@ -3327,7 +3330,7 @@
     </row>
     <row r="299" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A299" s="0" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="300" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3355,7 +3358,7 @@
     </row>
     <row r="301" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A301" s="0" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B301" s="0" t="n">
         <v>20</v>
@@ -3366,7 +3369,7 @@
     </row>
     <row r="302" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A302" s="0" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B302" s="0" t="n">
         <v>20</v>
@@ -3374,7 +3377,7 @@
     </row>
     <row r="304" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A304" s="0" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="305" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3402,7 +3405,7 @@
     </row>
     <row r="306" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A306" s="0" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B306" s="0" t="n">
         <v>20</v>
@@ -3413,7 +3416,7 @@
     </row>
     <row r="307" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A307" s="0" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B307" s="0" t="n">
         <v>20</v>
@@ -3421,7 +3424,7 @@
     </row>
     <row r="309" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A309" s="0" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="310" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3460,7 +3463,7 @@
     </row>
     <row r="312" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A312" s="0" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B312" s="0" t="n">
         <v>20</v>
@@ -3468,7 +3471,7 @@
     </row>
     <row r="314" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A314" s="0" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix rusturf tunnel hiker again
</commit_message>
<xml_diff>
--- a/trainers/trainers.xlsx
+++ b/trainers/trainers.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="645" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="646" uniqueCount="191">
   <si>
     <t xml:space="preserve">TRAINER_MAY_ROUTE_103_TREECKO</t>
   </si>
@@ -421,7 +421,10 @@
     <t xml:space="preserve"># Rusturf tunnel</t>
   </si>
   <si>
-    <t xml:space="preserve">TRAINER_MIKE_1</t>
+    <t xml:space="preserve">#NB: TRAINER_MIKE_1 is never battled in vanilla</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRAINER_MIKE_2</t>
   </si>
   <si>
     <t xml:space="preserve">Geodude</t>
@@ -690,10 +693,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G314"/>
+  <dimension ref="A1:G315"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A174" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B201" activeCellId="0" sqref="B201"/>
+      <selection pane="topLeft" activeCell="A197" activeCellId="0" sqref="A197"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2452,33 +2455,30 @@
     </row>
     <row r="198" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A198" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B198" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C198" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D198" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="E198" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F198" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="G198" s="0" t="s">
-        <v>7</v>
+        <v>134</v>
       </c>
     </row>
     <row r="199" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="0" t="s">
-        <v>134</v>
-      </c>
-      <c r="B199" s="0" t="n">
-        <v>12</v>
+        <v>1</v>
+      </c>
+      <c r="B199" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C199" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D199" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E199" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F199" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G199" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2486,108 +2486,108 @@
         <v>135</v>
       </c>
       <c r="B200" s="0" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="201" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A201" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="B201" s="0" t="n">
         <v>13</v>
-      </c>
-    </row>
-    <row r="202" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A202" s="0" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="203" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A203" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B203" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C203" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D203" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="E203" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F203" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="G203" s="0" t="s">
-        <v>7</v>
+        <v>137</v>
       </c>
     </row>
     <row r="204" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A204" s="0" t="s">
-        <v>137</v>
-      </c>
-      <c r="B204" s="0" t="n">
-        <v>18</v>
+        <v>1</v>
+      </c>
+      <c r="B204" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C204" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D204" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E204" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F204" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G204" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="205" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A205" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="B205" s="0" t="s">
-        <v>110</v>
+        <v>138</v>
+      </c>
+      <c r="B205" s="0" t="n">
+        <v>18</v>
       </c>
     </row>
     <row r="206" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A206" s="0" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B206" s="0" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="207" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A207" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="B207" s="0" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="208" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A208" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="B207" s="0" t="s">
+      <c r="B208" s="0" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="209" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A209" s="0" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="211" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A211" s="0" t="s">
+    <row r="210" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A210" s="0" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="212" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A212" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B212" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C212" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D212" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="E212" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F212" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="G212" s="0" t="s">
-        <v>7</v>
+        <v>140</v>
       </c>
     </row>
     <row r="213" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A213" s="0" t="s">
-        <v>140</v>
-      </c>
-      <c r="B213" s="0" t="n">
-        <v>15</v>
+        <v>1</v>
+      </c>
+      <c r="B213" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C213" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D213" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E213" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F213" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G213" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="214" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2595,79 +2595,79 @@
         <v>141</v>
       </c>
       <c r="B214" s="0" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="215" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A215" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="B215" s="0" t="n">
         <v>16</v>
-      </c>
-    </row>
-    <row r="216" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A216" s="0" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="217" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A217" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B217" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C217" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D217" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="E217" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F217" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="G217" s="0" t="s">
-        <v>7</v>
+        <v>143</v>
       </c>
     </row>
     <row r="218" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A218" s="0" t="s">
-        <v>143</v>
-      </c>
-      <c r="B218" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B218" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C218" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D218" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E218" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F218" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G218" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="219" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A219" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="B219" s="0" t="n">
         <v>18</v>
-      </c>
-    </row>
-    <row r="220" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A220" s="0" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="221" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A221" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B221" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C221" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D221" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="E221" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F221" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="G221" s="0" t="s">
-        <v>7</v>
+        <v>145</v>
       </c>
     </row>
     <row r="222" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A222" s="0" t="s">
-        <v>145</v>
-      </c>
-      <c r="B222" s="0" t="n">
-        <v>16</v>
+        <v>1</v>
+      </c>
+      <c r="B222" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C222" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D222" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E222" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F222" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G222" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="223" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2678,40 +2678,40 @@
         <v>16</v>
       </c>
     </row>
-    <row r="225" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A225" s="0" t="s">
+    <row r="224" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A224" s="0" t="s">
         <v>147</v>
+      </c>
+      <c r="B224" s="0" t="n">
+        <v>16</v>
       </c>
     </row>
     <row r="226" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A226" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B226" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C226" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D226" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="E226" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F226" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="G226" s="0" t="s">
-        <v>7</v>
+        <v>148</v>
       </c>
     </row>
     <row r="227" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A227" s="0" t="s">
-        <v>148</v>
-      </c>
-      <c r="B227" s="0" t="n">
-        <v>16</v>
+        <v>1</v>
+      </c>
+      <c r="B227" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C227" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D227" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E227" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F227" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G227" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="228" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2719,43 +2719,43 @@
         <v>149</v>
       </c>
       <c r="B228" s="0" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="229" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A229" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="B229" s="0" t="n">
         <v>17</v>
-      </c>
-    </row>
-    <row r="230" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A230" s="0" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="231" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A231" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B231" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C231" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D231" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="E231" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F231" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="G231" s="0" t="s">
-        <v>7</v>
+        <v>151</v>
       </c>
     </row>
     <row r="232" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A232" s="0" t="s">
-        <v>151</v>
-      </c>
-      <c r="B232" s="0" t="n">
-        <v>17</v>
+        <v>1</v>
+      </c>
+      <c r="B232" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C232" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D232" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E232" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F232" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G232" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="233" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2766,40 +2766,40 @@
         <v>17</v>
       </c>
     </row>
-    <row r="235" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A235" s="0" t="s">
+    <row r="234" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A234" s="0" t="s">
         <v>153</v>
+      </c>
+      <c r="B234" s="0" t="n">
+        <v>17</v>
       </c>
     </row>
     <row r="236" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A236" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B236" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C236" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D236" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="E236" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F236" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="G236" s="0" t="s">
-        <v>7</v>
+        <v>154</v>
       </c>
     </row>
     <row r="237" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A237" s="0" t="s">
-        <v>154</v>
-      </c>
-      <c r="B237" s="0" t="n">
-        <v>16</v>
+        <v>1</v>
+      </c>
+      <c r="B237" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C237" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D237" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E237" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F237" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G237" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="238" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2807,43 +2807,43 @@
         <v>155</v>
       </c>
       <c r="B238" s="0" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="239" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A239" s="0" t="s">
+        <v>156</v>
+      </c>
+      <c r="B239" s="0" t="n">
         <v>17</v>
-      </c>
-    </row>
-    <row r="240" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A240" s="0" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="241" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A241" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B241" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C241" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D241" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="E241" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F241" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="G241" s="0" t="s">
-        <v>7</v>
+        <v>157</v>
       </c>
     </row>
     <row r="242" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A242" s="0" t="s">
-        <v>157</v>
-      </c>
-      <c r="B242" s="0" t="n">
-        <v>19</v>
+        <v>1</v>
+      </c>
+      <c r="B242" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C242" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D242" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E242" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F242" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G242" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="243" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2851,82 +2851,82 @@
         <v>158</v>
       </c>
       <c r="B243" s="0" t="n">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="244" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A244" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="B244" s="0" t="n">
         <v>20</v>
-      </c>
-    </row>
-    <row r="245" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A245" s="0" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="246" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A246" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B246" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C246" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D246" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="E246" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F246" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="G246" s="0" t="s">
-        <v>7</v>
+        <v>160</v>
       </c>
     </row>
     <row r="247" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A247" s="0" t="s">
-        <v>160</v>
-      </c>
-      <c r="B247" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B247" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C247" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D247" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E247" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F247" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G247" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="248" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A248" s="0" t="s">
+        <v>161</v>
+      </c>
+      <c r="B248" s="0" t="n">
         <v>21</v>
       </c>
-      <c r="G247" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="249" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A249" s="0" t="s">
-        <v>161</v>
+      <c r="G248" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="250" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A250" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B250" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C250" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D250" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="E250" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F250" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="G250" s="0" t="s">
-        <v>7</v>
+        <v>162</v>
       </c>
     </row>
     <row r="251" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A251" s="0" t="s">
-        <v>162</v>
-      </c>
-      <c r="B251" s="0" t="n">
-        <v>23</v>
+        <v>1</v>
+      </c>
+      <c r="B251" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C251" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D251" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E251" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F251" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G251" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="252" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2934,296 +2934,293 @@
         <v>163</v>
       </c>
       <c r="B252" s="0" t="n">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="253" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A253" s="0" t="s">
+        <v>164</v>
+      </c>
+      <c r="B253" s="0" t="n">
         <v>21</v>
-      </c>
-    </row>
-    <row r="254" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A254" s="0" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="255" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A255" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B255" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C255" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D255" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="E255" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F255" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="G255" s="0" t="s">
-        <v>7</v>
+        <v>165</v>
       </c>
     </row>
     <row r="256" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A256" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="B256" s="0" t="n">
-        <v>22</v>
+        <v>1</v>
+      </c>
+      <c r="B256" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C256" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D256" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E256" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F256" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G256" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="257" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A257" s="0" t="s">
-        <v>165</v>
+        <v>16</v>
       </c>
       <c r="B257" s="0" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="258" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A258" s="0" t="s">
+        <v>166</v>
+      </c>
+      <c r="B258" s="0" t="n">
         <v>23</v>
       </c>
     </row>
-    <row r="259" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A259" s="0" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="261" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A261" s="0" t="s">
+    <row r="260" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A260" s="0" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="262" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A262" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B262" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C262" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D262" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="E262" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F262" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="G262" s="0" t="s">
-        <v>7</v>
+        <v>168</v>
       </c>
     </row>
     <row r="263" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A263" s="0" t="s">
-        <v>134</v>
-      </c>
-      <c r="B263" s="0" t="n">
-        <v>18</v>
+        <v>1</v>
+      </c>
+      <c r="B263" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C263" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D263" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E263" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F263" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G263" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="264" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A264" s="0" t="s">
-        <v>154</v>
+        <v>135</v>
       </c>
       <c r="B264" s="0" t="n">
         <v>18</v>
       </c>
-      <c r="D264" s="0" t="s">
+    </row>
+    <row r="265" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A265" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="B265" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="D265" s="0" t="s">
         <v>97</v>
-      </c>
-    </row>
-    <row r="266" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A266" s="0" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="267" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A267" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B267" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C267" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D267" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="E267" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F267" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="G267" s="0" t="s">
-        <v>7</v>
+        <v>169</v>
       </c>
     </row>
     <row r="268" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A268" s="0" t="s">
-        <v>169</v>
-      </c>
-      <c r="B268" s="0" t="n">
-        <v>18</v>
+        <v>1</v>
+      </c>
+      <c r="B268" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C268" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D268" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E268" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F268" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G268" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="269" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A269" s="0" t="s">
-        <v>140</v>
+        <v>170</v>
       </c>
       <c r="B269" s="0" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="270" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A270" s="0" t="s">
+        <v>141</v>
+      </c>
+      <c r="B270" s="0" t="n">
         <v>19</v>
       </c>
-      <c r="D269" s="0" t="s">
+      <c r="D270" s="0" t="s">
         <v>97</v>
-      </c>
-    </row>
-    <row r="271" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A271" s="0" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="272" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A272" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B272" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C272" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D272" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="E272" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F272" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="G272" s="0" t="s">
-        <v>7</v>
+        <v>171</v>
       </c>
     </row>
     <row r="273" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A273" s="0" t="s">
-        <v>155</v>
-      </c>
-      <c r="B273" s="0" t="n">
-        <v>17</v>
+        <v>1</v>
+      </c>
+      <c r="B273" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C273" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D273" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E273" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F273" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G273" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="274" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A274" s="0" t="s">
-        <v>171</v>
+        <v>156</v>
       </c>
       <c r="B274" s="0" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="275" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A275" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="B275" s="0" t="n">
         <v>19</v>
-      </c>
-    </row>
-    <row r="276" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A276" s="0" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="277" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A277" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B277" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C277" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D277" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="E277" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F277" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="G277" s="0" t="s">
-        <v>7</v>
+        <v>173</v>
       </c>
     </row>
     <row r="278" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A278" s="0" t="s">
-        <v>134</v>
-      </c>
-      <c r="B278" s="0" t="n">
-        <v>20</v>
-      </c>
-      <c r="E278" s="0" t="s">
-        <v>173</v>
+        <v>1</v>
+      </c>
+      <c r="B278" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C278" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D278" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E278" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F278" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G278" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="279" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A279" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="B279" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="E279" s="0" t="s">
         <v>174</v>
-      </c>
-      <c r="B279" s="0" t="n">
-        <v>22</v>
-      </c>
-      <c r="E279" s="0" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="280" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A280" s="0" t="s">
+        <v>175</v>
+      </c>
+      <c r="B280" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="E280" s="0" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="281" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A281" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="B280" s="0" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="282" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A282" s="0" t="s">
+      <c r="B281" s="0" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="284" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A284" s="0" t="s">
+    <row r="283" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A283" s="0" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="285" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A285" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B285" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C285" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D285" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="E285" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F285" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="G285" s="0" t="s">
-        <v>7</v>
+        <v>179</v>
       </c>
     </row>
     <row r="286" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A286" s="0" t="s">
-        <v>179</v>
-      </c>
-      <c r="B286" s="0" t="n">
-        <v>20</v>
+        <v>1</v>
+      </c>
+      <c r="B286" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C286" s="0" t="s">
+        <v>3</v>
       </c>
       <c r="D286" s="0" t="s">
-        <v>97</v>
+        <v>4</v>
+      </c>
+      <c r="E286" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F286" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G286" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="287" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3233,44 +3230,44 @@
       <c r="B287" s="0" t="n">
         <v>20</v>
       </c>
-    </row>
-    <row r="289" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A289" s="0" t="s">
+      <c r="D287" s="0" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="288" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A288" s="0" t="s">
         <v>181</v>
+      </c>
+      <c r="B288" s="0" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="290" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A290" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B290" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C290" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D290" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="E290" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F290" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="G290" s="0" t="s">
-        <v>7</v>
+        <v>182</v>
       </c>
     </row>
     <row r="291" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A291" s="0" t="s">
-        <v>182</v>
-      </c>
-      <c r="B291" s="0" t="n">
-        <v>20</v>
+        <v>1</v>
+      </c>
+      <c r="B291" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C291" s="0" t="s">
+        <v>3</v>
       </c>
       <c r="D291" s="0" t="s">
-        <v>97</v>
+        <v>4</v>
+      </c>
+      <c r="E291" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F291" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G291" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="292" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3280,91 +3277,91 @@
       <c r="B292" s="0" t="n">
         <v>20</v>
       </c>
-    </row>
-    <row r="294" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A294" s="0" t="s">
+      <c r="D292" s="0" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="293" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A293" s="0" t="s">
         <v>184</v>
+      </c>
+      <c r="B293" s="0" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="295" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A295" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B295" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C295" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D295" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="E295" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F295" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="G295" s="0" t="s">
-        <v>7</v>
+        <v>185</v>
       </c>
     </row>
     <row r="296" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A296" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="B296" s="0" t="n">
-        <v>20</v>
+        <v>1</v>
+      </c>
+      <c r="B296" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C296" s="0" t="s">
+        <v>3</v>
       </c>
       <c r="D296" s="0" t="s">
-        <v>97</v>
+        <v>4</v>
+      </c>
+      <c r="E296" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F296" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G296" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="297" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A297" s="0" t="s">
-        <v>185</v>
+        <v>40</v>
       </c>
       <c r="B297" s="0" t="n">
         <v>20</v>
       </c>
-    </row>
-    <row r="299" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A299" s="0" t="s">
+      <c r="D297" s="0" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="298" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A298" s="0" t="s">
         <v>186</v>
+      </c>
+      <c r="B298" s="0" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="300" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A300" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B300" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C300" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D300" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="E300" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F300" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="G300" s="0" t="s">
-        <v>7</v>
+        <v>187</v>
       </c>
     </row>
     <row r="301" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A301" s="0" t="s">
-        <v>179</v>
-      </c>
-      <c r="B301" s="0" t="n">
-        <v>20</v>
+        <v>1</v>
+      </c>
+      <c r="B301" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C301" s="0" t="s">
+        <v>3</v>
       </c>
       <c r="D301" s="0" t="s">
-        <v>97</v>
+        <v>4</v>
+      </c>
+      <c r="E301" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F301" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G301" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="302" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3374,44 +3371,44 @@
       <c r="B302" s="0" t="n">
         <v>20</v>
       </c>
-    </row>
-    <row r="304" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A304" s="0" t="s">
-        <v>187</v>
+      <c r="D302" s="0" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="303" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A303" s="0" t="s">
+        <v>181</v>
+      </c>
+      <c r="B303" s="0" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="305" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A305" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B305" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C305" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D305" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="E305" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F305" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="G305" s="0" t="s">
-        <v>7</v>
+        <v>188</v>
       </c>
     </row>
     <row r="306" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A306" s="0" t="s">
-        <v>182</v>
-      </c>
-      <c r="B306" s="0" t="n">
-        <v>20</v>
+        <v>1</v>
+      </c>
+      <c r="B306" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C306" s="0" t="s">
+        <v>3</v>
       </c>
       <c r="D306" s="0" t="s">
-        <v>97</v>
+        <v>4</v>
+      </c>
+      <c r="E306" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F306" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G306" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="307" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3421,57 +3418,68 @@
       <c r="B307" s="0" t="n">
         <v>20</v>
       </c>
-    </row>
-    <row r="309" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A309" s="0" t="s">
-        <v>188</v>
+      <c r="D307" s="0" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="308" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A308" s="0" t="s">
+        <v>184</v>
+      </c>
+      <c r="B308" s="0" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="310" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A310" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B310" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C310" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D310" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="E310" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F310" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="G310" s="0" t="s">
-        <v>7</v>
+        <v>189</v>
       </c>
     </row>
     <row r="311" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A311" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="B311" s="0" t="n">
-        <v>20</v>
+        <v>1</v>
+      </c>
+      <c r="B311" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C311" s="0" t="s">
+        <v>3</v>
       </c>
       <c r="D311" s="0" t="s">
-        <v>97</v>
+        <v>4</v>
+      </c>
+      <c r="E311" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F311" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G311" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="312" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A312" s="0" t="s">
-        <v>185</v>
+        <v>40</v>
       </c>
       <c r="B312" s="0" t="n">
         <v>20</v>
       </c>
-    </row>
-    <row r="314" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A314" s="0" t="s">
-        <v>189</v>
+      <c r="D312" s="0" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="313" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A313" s="0" t="s">
+        <v>186</v>
+      </c>
+      <c r="B313" s="0" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="315" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A315" s="0" t="s">
+        <v>190</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
finally fix rusturf hiker
</commit_message>
<xml_diff>
--- a/trainers/trainers.xlsx
+++ b/trainers/trainers.xlsx
@@ -695,8 +695,8 @@
   </sheetPr>
   <dimension ref="A1:G315"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A174" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A197" activeCellId="0" sqref="A197"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A177" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A201" activeCellId="0" sqref="A201"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
adjust brine beach trainers, adjust gen 3 starter and whismur family abilities
</commit_message>
<xml_diff>
--- a/trainers/trainers.xlsx
+++ b/trainers/trainers.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="646" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="727" uniqueCount="212">
   <si>
     <t xml:space="preserve">TRAINER_MAY_ROUTE_103_TREECKO</t>
   </si>
@@ -289,6 +289,18 @@
     <t xml:space="preserve">Aipom</t>
   </si>
   <si>
+    <t xml:space="preserve">TRAINER_ISAAC_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Taillow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Makuhita</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tangel</t>
+  </si>
+  <si>
     <t xml:space="preserve">TRAINER_ANNA_AND_MEG_1</t>
   </si>
   <si>
@@ -547,10 +559,10 @@
     <t xml:space="preserve">Rock Tomb, Mud Sport, Defense Curl, Magnitude</t>
   </si>
   <si>
-    <t xml:space="preserve">Relicanth</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rock Tomb, Mud Sport, Water Gun, Harden</t>
+    <t xml:space="preserve">Omanyte</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rock Tomb, Constrict, Water Gun, Withdraw</t>
   </si>
   <si>
     <t xml:space="preserve">{ITEM_SUPER_POTION, ITEM_SUPER_POTION, ITEM_NONE, ITEM_NONE}</t>
@@ -590,6 +602,57 @@
   </si>
   <si>
     <t xml:space="preserve">TRAINER_BRENDAN_RUSTBORO_MUDKIP</t>
+  </si>
+  <si>
+    <t xml:space="preserve"># Brine Beach</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRAINER_CADEN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hitmontop</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRAINER_TYCHO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shock Wave, Surf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRAINER_CHEVIS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wailmer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Goldeen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRAINER_GRUNT_BRINE_BEACH_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wooper</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zubat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRAINER_GRUNT_BRINE_BEACH_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wartortle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Carvanha</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRAINER_SHELLY_BRINE_BEACH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nidorina</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Croconaw</t>
   </si>
   <si>
     <t xml:space="preserve">END</t>
@@ -693,10 +756,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G315"/>
+  <dimension ref="A1:G359"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A177" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A201" activeCellId="0" sqref="A201"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A308" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B335" activeCellId="0" sqref="B335"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1888,15 +1951,12 @@
     </row>
     <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="1" t="s">
-        <v>36</v>
+        <v>90</v>
       </c>
       <c r="B133" s="1" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C133" s="1"/>
-      <c r="E133" s="0" t="s">
-        <v>90</v>
-      </c>
     </row>
     <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="0" t="s">
@@ -1905,75 +1965,69 @@
       <c r="B134" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="E134" s="0" t="s">
+    </row>
+    <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A135" s="0" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A136" s="0" t="s">
+      <c r="B135" s="0" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A137" s="0" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A138" s="0" t="s">
-        <v>94</v>
+      <c r="A138" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B138" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C138" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D138" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E138" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F138" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G138" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B139" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C139" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D139" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E139" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F139" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="G139" s="0" t="s">
-        <v>7</v>
+        <v>36</v>
+      </c>
+      <c r="B139" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="C139" s="1"/>
+      <c r="E139" s="0" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A140" s="1" t="s">
+      <c r="A140" s="0" t="s">
         <v>95</v>
       </c>
-      <c r="B140" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="C140" s="1"/>
+      <c r="B140" s="0" t="n">
+        <v>8</v>
+      </c>
       <c r="E140" s="0" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A141" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="B141" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="D141" s="0" t="s">
-        <v>97</v>
-      </c>
-      <c r="E141" s="0" t="s">
-        <v>96</v>
-      </c>
-    </row>
     <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="B142" s="0" t="s">
-        <v>66</v>
+        <v>97</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2006,217 +2060,218 @@
     </row>
     <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="1" t="s">
-        <v>55</v>
+        <v>99</v>
       </c>
       <c r="B146" s="1" t="n">
         <v>9</v>
       </c>
       <c r="C146" s="1"/>
-      <c r="D146" s="0" t="s">
-        <v>97</v>
-      </c>
       <c r="E146" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="0" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B147" s="0" t="n">
         <v>10</v>
       </c>
+      <c r="D147" s="0" t="s">
+        <v>101</v>
+      </c>
       <c r="E147" s="0" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A149" s="0" t="s">
-        <v>101</v>
+    <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A148" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="B148" s="0" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B150" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C150" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D150" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="E150" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F150" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="G150" s="0" t="s">
-        <v>7</v>
+        <v>102</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A151" s="0" t="s">
-        <v>102</v>
-      </c>
-      <c r="B151" s="0" t="n">
-        <v>12</v>
-      </c>
-      <c r="E151" s="0" t="s">
+      <c r="A151" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B151" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C151" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D151" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E151" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F151" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G151" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A152" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B152" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="C152" s="1"/>
+      <c r="D152" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="E152" s="0" t="s">
         <v>103</v>
-      </c>
-    </row>
-    <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A152" s="0" t="s">
-        <v>104</v>
-      </c>
-      <c r="B152" s="0" t="n">
-        <v>14</v>
-      </c>
-      <c r="E152" s="0" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="B153" s="0" t="s">
-        <v>106</v>
+        <v>30</v>
+      </c>
+      <c r="B153" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="E153" s="0" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="0" t="s">
-        <v>107</v>
+        <v>105</v>
+      </c>
+    </row>
+    <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A156" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B156" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C156" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D156" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E156" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F156" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G156" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="0" t="s">
-        <v>108</v>
+        <v>106</v>
+      </c>
+      <c r="B157" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="E157" s="0" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B158" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C158" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D158" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="E158" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F158" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="G158" s="0" t="s">
-        <v>7</v>
+        <v>108</v>
+      </c>
+      <c r="B158" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="E158" s="0" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="0" t="s">
-        <v>109</v>
-      </c>
-      <c r="B159" s="0" t="n">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A160" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="B160" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="B159" s="0" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="B161" s="0" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A162" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="B162" s="0" t="s">
+    <row r="163" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A163" s="0" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="0" t="s">
-        <v>113</v>
+        <v>1</v>
+      </c>
+      <c r="B164" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C164" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D164" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E164" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F164" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G164" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B165" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C165" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D165" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="E165" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F165" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="G165" s="0" t="s">
-        <v>7</v>
+        <v>113</v>
+      </c>
+      <c r="B165" s="0" t="n">
+        <v>13</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="B166" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="E166" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="B166" s="0" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="B167" s="0" t="s">
         <v>115</v>
-      </c>
-      <c r="B167" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="E167" s="0" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="B168" s="0" t="s">
         <v>116</v>
-      </c>
-      <c r="B168" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="E168" s="0" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="0" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2244,258 +2299,270 @@
     </row>
     <row r="172" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="0" t="s">
-        <v>119</v>
+        <v>74</v>
       </c>
       <c r="B172" s="0" t="n">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="E172" s="0" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="B173" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="E173" s="0" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="174" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A174" s="0" t="s">
         <v>120</v>
       </c>
-      <c r="B173" s="0" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="175" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A175" s="0" t="s">
+      <c r="B174" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="E174" s="0" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B176" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C176" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D176" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="E176" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F176" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="G176" s="0" t="s">
-        <v>7</v>
+        <v>122</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="0" t="s">
-        <v>122</v>
-      </c>
-      <c r="B177" s="0" t="n">
-        <v>13</v>
+        <v>1</v>
+      </c>
+      <c r="B177" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C177" s="0" t="s">
+        <v>3</v>
       </c>
       <c r="D177" s="0" t="s">
-        <v>31</v>
+        <v>4</v>
+      </c>
+      <c r="E177" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F177" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G177" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="178" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A178" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="B178" s="0" t="n">
+        <v>11</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="0" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="180" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A180" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B180" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C180" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D180" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="E180" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F180" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="G180" s="0" t="s">
-        <v>7</v>
+        <v>124</v>
+      </c>
+      <c r="B179" s="0" t="n">
+        <v>12</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="0" t="s">
-        <v>124</v>
-      </c>
-      <c r="B181" s="0" t="n">
-        <v>12</v>
+        <v>125</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="0" t="s">
-        <v>125</v>
-      </c>
-      <c r="B182" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B182" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C182" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D182" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E182" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F182" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G182" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="183" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A183" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="B183" s="0" t="n">
         <v>13</v>
       </c>
-    </row>
-    <row r="184" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A184" s="0" t="s">
-        <v>126</v>
+      <c r="D183" s="0" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B185" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C185" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D185" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="E185" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F185" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="G185" s="0" t="s">
-        <v>7</v>
+        <v>127</v>
       </c>
     </row>
     <row r="186" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="0" t="s">
-        <v>127</v>
-      </c>
-      <c r="B186" s="0" t="n">
-        <v>14</v>
-      </c>
-      <c r="E186" s="0" t="s">
-        <v>128</v>
+        <v>1</v>
+      </c>
+      <c r="B186" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C186" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D186" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E186" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F186" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G186" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="0" t="s">
-        <v>109</v>
+        <v>128</v>
       </c>
       <c r="B187" s="0" t="n">
-        <v>14</v>
-      </c>
-      <c r="E187" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="188" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A188" s="0" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="189" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A189" s="0" t="s">
-        <v>130</v>
+      <c r="B188" s="0" t="n">
+        <v>13</v>
       </c>
     </row>
     <row r="190" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A190" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B190" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C190" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D190" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="E190" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F190" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="G190" s="0" t="s">
-        <v>7</v>
+        <v>130</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A191" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="B191" s="0" t="n">
-        <v>15</v>
+        <v>1</v>
+      </c>
+      <c r="B191" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C191" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D191" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E191" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F191" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G191" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="192" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A192" s="0" t="s">
-        <v>91</v>
+        <v>131</v>
       </c>
       <c r="B192" s="0" t="n">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="E192" s="0" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="193" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A193" s="0" t="s">
-        <v>131</v>
+        <v>113</v>
       </c>
       <c r="B193" s="0" t="n">
         <v>14</v>
       </c>
+      <c r="E193" s="0" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="195" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A195" s="0" t="s">
-        <v>132</v>
+        <v>134</v>
+      </c>
+    </row>
+    <row r="196" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A196" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B196" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C196" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D196" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E196" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F196" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G196" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="197" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="0" t="s">
-        <v>133</v>
+        <v>33</v>
+      </c>
+      <c r="B197" s="0" t="n">
+        <v>15</v>
       </c>
     </row>
     <row r="198" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A198" s="0" t="s">
-        <v>134</v>
+        <v>95</v>
+      </c>
+      <c r="B198" s="0" t="n">
+        <v>13</v>
       </c>
     </row>
     <row r="199" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B199" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C199" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D199" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="E199" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F199" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="G199" s="0" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="200" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A200" s="0" t="s">
         <v>135</v>
       </c>
-      <c r="B200" s="0" t="n">
-        <v>12</v>
+      <c r="B199" s="0" t="n">
+        <v>14</v>
       </c>
     </row>
     <row r="201" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A201" s="0" t="s">
         <v>136</v>
       </c>
-      <c r="B201" s="0" t="n">
-        <v>13</v>
-      </c>
     </row>
     <row r="203" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A203" s="0" t="s">
@@ -2504,222 +2571,219 @@
     </row>
     <row r="204" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A204" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B204" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C204" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D204" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="E204" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F204" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="G204" s="0" t="s">
-        <v>7</v>
+        <v>138</v>
       </c>
     </row>
     <row r="205" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A205" s="0" t="s">
-        <v>138</v>
-      </c>
-      <c r="B205" s="0" t="n">
-        <v>18</v>
+        <v>1</v>
+      </c>
+      <c r="B205" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C205" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D205" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E205" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F205" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G205" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="206" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A206" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="B206" s="0" t="s">
-        <v>110</v>
+        <v>139</v>
+      </c>
+      <c r="B206" s="0" t="n">
+        <v>12</v>
       </c>
     </row>
     <row r="207" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A207" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="B207" s="0" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="208" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A208" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="B208" s="0" t="s">
-        <v>112</v>
+        <v>140</v>
+      </c>
+      <c r="B207" s="0" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="209" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A209" s="0" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="210" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A210" s="0" t="s">
-        <v>139</v>
+        <v>1</v>
+      </c>
+      <c r="B210" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C210" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D210" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E210" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F210" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G210" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="211" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A211" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="B211" s="0" t="n">
+        <v>18</v>
       </c>
     </row>
     <row r="212" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A212" s="0" t="s">
-        <v>140</v>
+        <v>41</v>
+      </c>
+      <c r="B212" s="0" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="213" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A213" s="0" t="s">
-        <v>1</v>
+        <v>43</v>
       </c>
       <c r="B213" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C213" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D213" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="E213" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F213" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="G213" s="0" t="s">
-        <v>7</v>
+        <v>115</v>
       </c>
     </row>
     <row r="214" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A214" s="0" t="s">
-        <v>141</v>
-      </c>
-      <c r="B214" s="0" t="n">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="215" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A215" s="0" t="s">
-        <v>142</v>
-      </c>
-      <c r="B215" s="0" t="n">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="217" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A217" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="B214" s="0" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="216" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A216" s="0" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="218" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A218" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B218" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C218" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D218" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="E218" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F218" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="G218" s="0" t="s">
-        <v>7</v>
+        <v>144</v>
       </c>
     </row>
     <row r="219" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A219" s="0" t="s">
-        <v>144</v>
-      </c>
-      <c r="B219" s="0" t="n">
-        <v>18</v>
+        <v>1</v>
+      </c>
+      <c r="B219" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C219" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D219" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E219" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F219" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G219" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="220" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A220" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="B220" s="0" t="n">
+        <v>15</v>
       </c>
     </row>
     <row r="221" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A221" s="0" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="222" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A222" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B222" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C222" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D222" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="E222" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F222" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="G222" s="0" t="s">
-        <v>7</v>
+        <v>146</v>
+      </c>
+      <c r="B221" s="0" t="n">
+        <v>16</v>
       </c>
     </row>
     <row r="223" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A223" s="0" t="s">
-        <v>146</v>
-      </c>
-      <c r="B223" s="0" t="n">
-        <v>16</v>
+        <v>147</v>
       </c>
     </row>
     <row r="224" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A224" s="0" t="s">
-        <v>147</v>
-      </c>
-      <c r="B224" s="0" t="n">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="226" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A226" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B224" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C224" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D224" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E224" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F224" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G224" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="225" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A225" s="0" t="s">
         <v>148</v>
+      </c>
+      <c r="B225" s="0" t="n">
+        <v>18</v>
       </c>
     </row>
     <row r="227" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A227" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B227" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C227" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D227" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="E227" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F227" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="G227" s="0" t="s">
-        <v>7</v>
+        <v>149</v>
       </c>
     </row>
     <row r="228" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A228" s="0" t="s">
-        <v>149</v>
-      </c>
-      <c r="B228" s="0" t="n">
-        <v>16</v>
+        <v>1</v>
+      </c>
+      <c r="B228" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C228" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D228" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E228" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F228" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G228" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="229" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2727,43 +2791,43 @@
         <v>150</v>
       </c>
       <c r="B229" s="0" t="n">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="231" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A231" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="230" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A230" s="0" t="s">
         <v>151</v>
+      </c>
+      <c r="B230" s="0" t="n">
+        <v>16</v>
       </c>
     </row>
     <row r="232" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A232" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B232" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C232" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D232" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="E232" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F232" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="G232" s="0" t="s">
-        <v>7</v>
+        <v>152</v>
       </c>
     </row>
     <row r="233" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A233" s="0" t="s">
-        <v>152</v>
-      </c>
-      <c r="B233" s="0" t="n">
-        <v>17</v>
+        <v>1</v>
+      </c>
+      <c r="B233" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C233" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D233" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E233" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F233" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G233" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="234" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2771,43 +2835,43 @@
         <v>153</v>
       </c>
       <c r="B234" s="0" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="235" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A235" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="B235" s="0" t="n">
         <v>17</v>
-      </c>
-    </row>
-    <row r="236" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A236" s="0" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="237" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A237" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B237" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C237" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D237" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="E237" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F237" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="G237" s="0" t="s">
-        <v>7</v>
+        <v>155</v>
       </c>
     </row>
     <row r="238" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A238" s="0" t="s">
-        <v>155</v>
-      </c>
-      <c r="B238" s="0" t="n">
-        <v>16</v>
+        <v>1</v>
+      </c>
+      <c r="B238" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C238" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D238" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E238" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F238" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G238" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="239" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2818,40 +2882,40 @@
         <v>17</v>
       </c>
     </row>
-    <row r="241" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A241" s="0" t="s">
+    <row r="240" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A240" s="0" t="s">
         <v>157</v>
+      </c>
+      <c r="B240" s="0" t="n">
+        <v>17</v>
       </c>
     </row>
     <row r="242" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A242" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B242" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C242" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D242" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="E242" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F242" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="G242" s="0" t="s">
-        <v>7</v>
+        <v>158</v>
       </c>
     </row>
     <row r="243" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A243" s="0" t="s">
-        <v>158</v>
-      </c>
-      <c r="B243" s="0" t="n">
-        <v>19</v>
+        <v>1</v>
+      </c>
+      <c r="B243" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C243" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D243" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E243" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F243" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G243" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="244" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2859,426 +2923,420 @@
         <v>159</v>
       </c>
       <c r="B244" s="0" t="n">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="246" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A246" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="245" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A245" s="0" t="s">
         <v>160</v>
+      </c>
+      <c r="B245" s="0" t="n">
+        <v>17</v>
       </c>
     </row>
     <row r="247" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A247" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B247" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C247" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D247" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="E247" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F247" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="G247" s="0" t="s">
-        <v>7</v>
+        <v>161</v>
       </c>
     </row>
     <row r="248" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A248" s="0" t="s">
-        <v>161</v>
-      </c>
-      <c r="B248" s="0" t="n">
-        <v>21</v>
-      </c>
-      <c r="G248" s="0" t="n">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="B248" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C248" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D248" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E248" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F248" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G248" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="249" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A249" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="B249" s="0" t="n">
+        <v>19</v>
       </c>
     </row>
     <row r="250" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A250" s="0" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="251" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A251" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B251" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C251" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D251" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="E251" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F251" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="G251" s="0" t="s">
-        <v>7</v>
+        <v>163</v>
+      </c>
+      <c r="B250" s="0" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="252" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A252" s="0" t="s">
-        <v>163</v>
-      </c>
-      <c r="B252" s="0" t="n">
-        <v>23</v>
+        <v>164</v>
       </c>
     </row>
     <row r="253" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A253" s="0" t="s">
-        <v>164</v>
-      </c>
-      <c r="B253" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B253" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C253" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D253" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E253" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F253" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G253" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="254" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A254" s="0" t="s">
+        <v>165</v>
+      </c>
+      <c r="B254" s="0" t="n">
         <v>21</v>
       </c>
-    </row>
-    <row r="255" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A255" s="0" t="s">
-        <v>165</v>
+      <c r="G254" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="256" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A256" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B256" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C256" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D256" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="E256" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F256" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="G256" s="0" t="s">
-        <v>7</v>
+        <v>166</v>
       </c>
     </row>
     <row r="257" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A257" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="B257" s="0" t="n">
-        <v>22</v>
+        <v>1</v>
+      </c>
+      <c r="B257" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C257" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D257" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E257" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F257" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G257" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="258" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A258" s="0" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B258" s="0" t="n">
         <v>23</v>
       </c>
     </row>
-    <row r="260" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A260" s="0" t="s">
-        <v>167</v>
+    <row r="259" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A259" s="0" t="s">
+        <v>168</v>
+      </c>
+      <c r="B259" s="0" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="261" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A261" s="0" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="262" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A262" s="0" t="s">
-        <v>168</v>
+        <v>1</v>
+      </c>
+      <c r="B262" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C262" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D262" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E262" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F262" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G262" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="263" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A263" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B263" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C263" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D263" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="E263" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F263" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="G263" s="0" t="s">
-        <v>7</v>
+        <v>16</v>
+      </c>
+      <c r="B263" s="0" t="n">
+        <v>22</v>
       </c>
     </row>
     <row r="264" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A264" s="0" t="s">
-        <v>135</v>
+        <v>170</v>
       </c>
       <c r="B264" s="0" t="n">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="265" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A265" s="0" t="s">
-        <v>155</v>
-      </c>
-      <c r="B265" s="0" t="n">
-        <v>18</v>
-      </c>
-      <c r="D265" s="0" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="267" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A267" s="0" t="s">
-        <v>169</v>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="266" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A266" s="0" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="268" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A268" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B268" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C268" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D268" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="E268" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F268" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="G268" s="0" t="s">
-        <v>7</v>
+        <v>172</v>
       </c>
     </row>
     <row r="269" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A269" s="0" t="s">
-        <v>170</v>
-      </c>
-      <c r="B269" s="0" t="n">
-        <v>18</v>
+        <v>1</v>
+      </c>
+      <c r="B269" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C269" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D269" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E269" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F269" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G269" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="270" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A270" s="0" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B270" s="0" t="n">
-        <v>19</v>
-      </c>
-      <c r="D270" s="0" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="272" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A272" s="0" t="s">
-        <v>171</v>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="271" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A271" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="B271" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="D271" s="0" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="273" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A273" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B273" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C273" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D273" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="E273" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F273" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="G273" s="0" t="s">
-        <v>7</v>
+        <v>173</v>
       </c>
     </row>
     <row r="274" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A274" s="0" t="s">
-        <v>156</v>
-      </c>
-      <c r="B274" s="0" t="n">
-        <v>17</v>
+        <v>1</v>
+      </c>
+      <c r="B274" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C274" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D274" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E274" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F274" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G274" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="275" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A275" s="0" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B275" s="0" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="276" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A276" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="B276" s="0" t="n">
         <v>19</v>
       </c>
-    </row>
-    <row r="277" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A277" s="0" t="s">
-        <v>173</v>
+      <c r="D276" s="0" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="278" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A278" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B278" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C278" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D278" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="E278" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F278" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="G278" s="0" t="s">
-        <v>7</v>
+        <v>175</v>
       </c>
     </row>
     <row r="279" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A279" s="0" t="s">
-        <v>135</v>
-      </c>
-      <c r="B279" s="0" t="n">
-        <v>20</v>
-      </c>
-      <c r="E279" s="0" t="s">
-        <v>174</v>
+        <v>1</v>
+      </c>
+      <c r="B279" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C279" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D279" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E279" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F279" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G279" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="280" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A280" s="0" t="s">
-        <v>175</v>
+        <v>160</v>
       </c>
       <c r="B280" s="0" t="n">
-        <v>22</v>
-      </c>
-      <c r="E280" s="0" t="s">
-        <v>176</v>
+        <v>17</v>
       </c>
     </row>
     <row r="281" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A281" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="B281" s="0" t="s">
-        <v>177</v>
+        <v>176</v>
+      </c>
+      <c r="B281" s="0" t="n">
+        <v>19</v>
       </c>
     </row>
     <row r="283" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A283" s="0" t="s">
-        <v>178</v>
+        <v>177</v>
+      </c>
+    </row>
+    <row r="284" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A284" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B284" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C284" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D284" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E284" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F284" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G284" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="285" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A285" s="0" t="s">
-        <v>179</v>
+        <v>139</v>
+      </c>
+      <c r="B285" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="E285" s="0" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="286" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A286" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B286" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C286" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D286" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="E286" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F286" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="G286" s="0" t="s">
-        <v>7</v>
+        <v>179</v>
+      </c>
+      <c r="B286" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="E286" s="0" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="287" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A287" s="0" t="s">
-        <v>180</v>
-      </c>
-      <c r="B287" s="0" t="n">
-        <v>20</v>
-      </c>
-      <c r="D287" s="0" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="288" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A288" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="B287" s="0" t="s">
         <v>181</v>
       </c>
-      <c r="B288" s="0" t="n">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="290" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A290" s="0" t="s">
+    </row>
+    <row r="289" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A289" s="0" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="291" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A291" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B291" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C291" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D291" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="E291" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F291" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="G291" s="0" t="s">
-        <v>7</v>
+        <v>183</v>
       </c>
     </row>
     <row r="292" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A292" s="0" t="s">
-        <v>183</v>
-      </c>
-      <c r="B292" s="0" t="n">
-        <v>20</v>
+        <v>1</v>
+      </c>
+      <c r="B292" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C292" s="0" t="s">
+        <v>3</v>
       </c>
       <c r="D292" s="0" t="s">
-        <v>97</v>
+        <v>4</v>
+      </c>
+      <c r="E292" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F292" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G292" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="293" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3288,138 +3346,138 @@
       <c r="B293" s="0" t="n">
         <v>20</v>
       </c>
-    </row>
-    <row r="295" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A295" s="0" t="s">
+      <c r="D293" s="0" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="294" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A294" s="0" t="s">
         <v>185</v>
+      </c>
+      <c r="B294" s="0" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="296" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A296" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B296" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C296" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D296" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="E296" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F296" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="G296" s="0" t="s">
-        <v>7</v>
+        <v>186</v>
       </c>
     </row>
     <row r="297" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A297" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="B297" s="0" t="n">
-        <v>20</v>
+        <v>1</v>
+      </c>
+      <c r="B297" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C297" s="0" t="s">
+        <v>3</v>
       </c>
       <c r="D297" s="0" t="s">
-        <v>97</v>
+        <v>4</v>
+      </c>
+      <c r="E297" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F297" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G297" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="298" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A298" s="0" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B298" s="0" t="n">
         <v>20</v>
       </c>
-    </row>
-    <row r="300" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A300" s="0" t="s">
-        <v>187</v>
+      <c r="D298" s="0" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="299" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A299" s="0" t="s">
+        <v>188</v>
+      </c>
+      <c r="B299" s="0" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="301" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A301" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B301" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C301" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D301" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="E301" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F301" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="G301" s="0" t="s">
-        <v>7</v>
+        <v>189</v>
       </c>
     </row>
     <row r="302" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A302" s="0" t="s">
-        <v>180</v>
-      </c>
-      <c r="B302" s="0" t="n">
-        <v>20</v>
+        <v>1</v>
+      </c>
+      <c r="B302" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C302" s="0" t="s">
+        <v>3</v>
       </c>
       <c r="D302" s="0" t="s">
-        <v>97</v>
+        <v>4</v>
+      </c>
+      <c r="E302" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F302" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G302" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="303" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A303" s="0" t="s">
-        <v>181</v>
+        <v>40</v>
       </c>
       <c r="B303" s="0" t="n">
         <v>20</v>
       </c>
-    </row>
-    <row r="305" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A305" s="0" t="s">
-        <v>188</v>
+      <c r="D303" s="0" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="304" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A304" s="0" t="s">
+        <v>190</v>
+      </c>
+      <c r="B304" s="0" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="306" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A306" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B306" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C306" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D306" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="E306" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F306" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="G306" s="0" t="s">
-        <v>7</v>
+        <v>191</v>
       </c>
     </row>
     <row r="307" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A307" s="0" t="s">
-        <v>183</v>
-      </c>
-      <c r="B307" s="0" t="n">
-        <v>20</v>
+        <v>1</v>
+      </c>
+      <c r="B307" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C307" s="0" t="s">
+        <v>3</v>
       </c>
       <c r="D307" s="0" t="s">
-        <v>97</v>
+        <v>4</v>
+      </c>
+      <c r="E307" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F307" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G307" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="308" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3429,57 +3487,410 @@
       <c r="B308" s="0" t="n">
         <v>20</v>
       </c>
-    </row>
-    <row r="310" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A310" s="0" t="s">
-        <v>189</v>
+      <c r="D308" s="0" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="309" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A309" s="0" t="s">
+        <v>185</v>
+      </c>
+      <c r="B309" s="0" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="311" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A311" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B311" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C311" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D311" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="E311" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F311" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="G311" s="0" t="s">
-        <v>7</v>
+        <v>192</v>
       </c>
     </row>
     <row r="312" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A312" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="B312" s="0" t="n">
-        <v>20</v>
+        <v>1</v>
+      </c>
+      <c r="B312" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C312" s="0" t="s">
+        <v>3</v>
       </c>
       <c r="D312" s="0" t="s">
-        <v>97</v>
+        <v>4</v>
+      </c>
+      <c r="E312" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F312" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G312" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="313" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A313" s="0" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B313" s="0" t="n">
         <v>20</v>
       </c>
-    </row>
-    <row r="315" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A315" s="0" t="s">
+      <c r="D313" s="0" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="314" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A314" s="0" t="s">
+        <v>188</v>
+      </c>
+      <c r="B314" s="0" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="316" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A316" s="0" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="317" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A317" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B317" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C317" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D317" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E317" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F317" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G317" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="318" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A318" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="B318" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="D318" s="0" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="319" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A319" s="0" t="s">
         <v>190</v>
+      </c>
+      <c r="B319" s="0" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="321" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A321" s="0" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="323" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A323" s="0" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="324" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A324" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B324" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C324" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D324" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E324" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F324" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G324" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="325" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A325" s="0" t="s">
+        <v>196</v>
+      </c>
+      <c r="B325" s="0" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="327" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A327" s="0" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="328" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A328" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B328" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C328" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D328" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E328" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F328" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G328" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="329" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A329" s="0" t="s">
+        <v>170</v>
+      </c>
+      <c r="B329" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="E329" s="0" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="331" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A331" s="0" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="332" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A332" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B332" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C332" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D332" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E332" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F332" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G332" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="333" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A333" s="0" t="s">
+        <v>200</v>
+      </c>
+      <c r="B333" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="D333" s="0" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="334" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A334" s="0" t="s">
+        <v>201</v>
+      </c>
+      <c r="B334" s="0" t="n">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="336" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A336" s="0" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="337" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A337" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B337" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C337" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D337" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E337" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F337" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G337" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="338" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A338" s="0" t="s">
+        <v>203</v>
+      </c>
+      <c r="B338" s="0" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="339" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A339" s="0" t="s">
+        <v>204</v>
+      </c>
+      <c r="B339" s="0" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="341" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A341" s="0" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="342" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A342" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B342" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C342" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D342" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E342" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F342" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G342" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="343" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A343" s="0" t="s">
+        <v>206</v>
+      </c>
+      <c r="B343" s="0" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="345" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A345" s="0" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="346" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A346" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B346" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C346" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D346" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E346" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F346" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G346" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="347" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A347" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="B347" s="0" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="348" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A348" s="0" t="s">
+        <v>207</v>
+      </c>
+      <c r="B348" s="0" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="350" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A350" s="0" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="351" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A351" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B351" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C351" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D351" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E351" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F351" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G351" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="352" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A352" s="0" t="s">
+        <v>209</v>
+      </c>
+      <c r="B352" s="0" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="353" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A353" s="0" t="s">
+        <v>210</v>
+      </c>
+      <c r="B353" s="0" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="359" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A359" s="0" t="s">
+        <v>211</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adjust wild mon levels and route 106 trainers, add items to granite cave fiery room
</commit_message>
<xml_diff>
--- a/trainers/trainers.xlsx
+++ b/trainers/trainers.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="727" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="747" uniqueCount="218">
   <si>
     <t xml:space="preserve">TRAINER_MAY_ROUTE_103_TREECKO</t>
   </si>
@@ -653,6 +653,24 @@
   </si>
   <si>
     <t xml:space="preserve">Croconaw</t>
+  </si>
+  <si>
+    <t xml:space="preserve"># route 106</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRAINER_NED</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tentacool</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Barboach</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRAINER_ELLIOT_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Huntail</t>
   </si>
   <si>
     <t xml:space="preserve">END</t>
@@ -756,10 +774,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G359"/>
+  <dimension ref="A1:G379"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A308" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B335" activeCellId="0" sqref="B335"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A337" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B365" activeCellId="0" sqref="B365"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3888,9 +3906,94 @@
         <v>24</v>
       </c>
     </row>
+    <row r="355" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A355" s="0" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="357" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A357" s="0" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="358" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A358" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B358" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C358" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D358" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E358" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F358" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G358" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
     <row r="359" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A359" s="0" t="s">
-        <v>211</v>
+        <v>213</v>
+      </c>
+      <c r="B359" s="0" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="360" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A360" s="0" t="s">
+        <v>214</v>
+      </c>
+      <c r="B360" s="0" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="362" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A362" s="0" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="363" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A363" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B363" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C363" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D363" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E363" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F363" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G363" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="364" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A364" s="0" t="s">
+        <v>216</v>
+      </c>
+      <c r="B364" s="0" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="379" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A379" s="0" t="s">
+        <v>217</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
route 109 and seashore house trainers
</commit_message>
<xml_diff>
--- a/trainers/trainers.xlsx
+++ b/trainers/trainers.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="819" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="911" uniqueCount="255">
   <si>
     <t xml:space="preserve">TRAINER_MAY_ROUTE_103_TREECKO</t>
   </si>
@@ -719,6 +719,69 @@
   </si>
   <si>
     <t xml:space="preserve">Damp</t>
+  </si>
+  <si>
+    <t xml:space="preserve"># route 109</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRAINER_HUEY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Poliwhirl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRAINER_HAILEY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Marill</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRAINER_EDMOND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lombre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRAINER_RICKY_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRAINER_LOLA_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Masquerain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Flutter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRAINER_CHANDLER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wingull</t>
+  </si>
+  <si>
+    <t xml:space="preserve"># seashore house</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Machoke</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRAINER_JOHANNA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Linoone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Raichu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRAINER_SIMON</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Psyduck</t>
   </si>
   <si>
     <t xml:space="preserve">END</t>
@@ -822,10 +885,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G404"/>
+  <dimension ref="A1:G448"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A361" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E399" activeCellId="0" sqref="E399"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A409" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B451" activeCellId="0" sqref="B451"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4340,9 +4403,410 @@
         <v>232</v>
       </c>
     </row>
+    <row r="400" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A400" s="0" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="402" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A402" s="0" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="403" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A403" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B403" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C403" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D403" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E403" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F403" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G403" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
     <row r="404" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A404" s="0" t="s">
-        <v>233</v>
+        <v>87</v>
+      </c>
+      <c r="B404" s="0" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="405" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A405" s="0" t="s">
+        <v>235</v>
+      </c>
+      <c r="B405" s="0" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="407" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A407" s="0" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="408" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A408" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B408" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C408" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D408" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E408" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F408" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G408" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="409" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A409" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="B409" s="0" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="410" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A410" s="0" t="s">
+        <v>237</v>
+      </c>
+      <c r="B410" s="0" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="412" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A412" s="0" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="413" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A413" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B413" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C413" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D413" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E413" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F413" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G413" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="414" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A414" s="0" t="s">
+        <v>239</v>
+      </c>
+      <c r="B414" s="0" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="415" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A415" s="0" t="s">
+        <v>240</v>
+      </c>
+      <c r="B415" s="0" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="417" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A417" s="0" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="418" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A418" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B418" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C418" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D418" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E418" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F418" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G418" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="419" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A419" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B419" s="0" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="420" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A420" s="0" t="s">
+        <v>203</v>
+      </c>
+      <c r="B420" s="0" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="422" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A422" s="0" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="423" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A423" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B423" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C423" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D423" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E423" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F423" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G423" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="424" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A424" s="0" t="s">
+        <v>243</v>
+      </c>
+      <c r="B424" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="F424" s="0" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="426" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A426" s="0" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="427" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A427" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B427" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C427" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D427" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E427" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F427" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G427" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="428" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A428" s="0" t="s">
+        <v>246</v>
+      </c>
+      <c r="B428" s="0" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="429" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A429" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="B429" s="0" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="431" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A431" s="0" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="433" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A433" s="0" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="434" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A434" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B434" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C434" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D434" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E434" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F434" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G434" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="435" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A435" s="0" t="s">
+        <v>188</v>
+      </c>
+      <c r="B435" s="0" t="n">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="436" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A436" s="0" t="s">
+        <v>248</v>
+      </c>
+      <c r="B436" s="0" t="n">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="438" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A438" s="0" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="439" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A439" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B439" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C439" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D439" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E439" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F439" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G439" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="440" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A440" s="0" t="s">
+        <v>250</v>
+      </c>
+      <c r="B440" s="0" t="n">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="441" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A441" s="0" t="s">
+        <v>251</v>
+      </c>
+      <c r="B441" s="0" t="n">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="443" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A443" s="0" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="444" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A444" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B444" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C444" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D444" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E444" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F444" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G444" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="445" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A445" s="0" t="s">
+        <v>253</v>
+      </c>
+      <c r="B445" s="0" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="446" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A446" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="B446" s="0" t="n">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="448" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A448" s="0" t="s">
+        <v>254</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
aquatic museum grunts, add flag to route 117 grunts
</commit_message>
<xml_diff>
--- a/trainers/trainers.xlsx
+++ b/trainers/trainers.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="911" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="932" uniqueCount="261">
   <si>
     <t xml:space="preserve">TRAINER_MAY_ROUTE_103_TREECKO</t>
   </si>
@@ -782,6 +782,24 @@
   </si>
   <si>
     <t xml:space="preserve">Psyduck</t>
+  </si>
+  <si>
+    <t xml:space="preserve"># oceanic museum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRAINER_GRUNT_MUSEUM_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mightyena</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRAINER_GRUNT_MUSEUM_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Golbat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Qwilfish</t>
   </si>
   <si>
     <t xml:space="preserve">END</t>
@@ -885,10 +903,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G448"/>
+  <dimension ref="A1:G472"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A409" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B451" activeCellId="0" sqref="B451"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A431" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A460" activeCellId="0" sqref="A460"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4809,6 +4827,99 @@
         <v>254</v>
       </c>
     </row>
+    <row r="450" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A450" s="0" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="451" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A451" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B451" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C451" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D451" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E451" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F451" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G451" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="452" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A452" s="0" t="s">
+        <v>204</v>
+      </c>
+      <c r="B452" s="0" t="n">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="453" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A453" s="0" t="s">
+        <v>256</v>
+      </c>
+      <c r="B453" s="0" t="n">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="455" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A455" s="0" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="456" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A456" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B456" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C456" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D456" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E456" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F456" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G456" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="457" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A457" s="0" t="s">
+        <v>258</v>
+      </c>
+      <c r="B457" s="0" t="n">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="458" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A458" s="0" t="s">
+        <v>259</v>
+      </c>
+      <c r="B458" s="0" t="n">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="472" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A472" s="0" t="s">
+        <v>260</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
fix seashore house trainers, replace devon goods in dialogue
</commit_message>
<xml_diff>
--- a/trainers/trainers.xlsx
+++ b/trainers/trainers.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="932" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="932" uniqueCount="262">
   <si>
     <t xml:space="preserve">TRAINER_MAY_ROUTE_103_TREECKO</t>
   </si>
@@ -764,6 +764,9 @@
   </si>
   <si>
     <t xml:space="preserve"># seashore house</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRAINER_DWAYNE</t>
   </si>
   <si>
     <t xml:space="preserve">Machoke</t>
@@ -905,8 +908,8 @@
   </sheetPr>
   <dimension ref="A1:G472"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A431" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A460" activeCellId="0" sqref="A460"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A403" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A434" activeCellId="0" sqref="A434"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4692,7 +4695,7 @@
     </row>
     <row r="433" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A433" s="0" t="s">
-        <v>241</v>
+        <v>248</v>
       </c>
     </row>
     <row r="434" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4728,7 +4731,7 @@
     </row>
     <row r="436" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A436" s="0" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="B436" s="0" t="n">
         <v>28</v>
@@ -4736,7 +4739,7 @@
     </row>
     <row r="438" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A438" s="0" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
     </row>
     <row r="439" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4764,7 +4767,7 @@
     </row>
     <row r="440" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A440" s="0" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B440" s="0" t="n">
         <v>26</v>
@@ -4772,7 +4775,7 @@
     </row>
     <row r="441" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A441" s="0" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="B441" s="0" t="n">
         <v>27</v>
@@ -4780,7 +4783,7 @@
     </row>
     <row r="443" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A443" s="0" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
     </row>
     <row r="444" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4808,7 +4811,7 @@
     </row>
     <row r="445" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A445" s="0" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="B445" s="0" t="n">
         <v>25</v>
@@ -4824,12 +4827,12 @@
     </row>
     <row r="448" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A448" s="0" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
     </row>
     <row r="450" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A450" s="0" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
     </row>
     <row r="451" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4865,7 +4868,7 @@
     </row>
     <row r="453" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A453" s="0" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="B453" s="0" t="n">
         <v>27</v>
@@ -4873,7 +4876,7 @@
     </row>
     <row r="455" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A455" s="0" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
     </row>
     <row r="456" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4901,7 +4904,7 @@
     </row>
     <row r="457" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A457" s="0" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="B457" s="0" t="n">
         <v>26</v>
@@ -4909,7 +4912,7 @@
     </row>
     <row r="458" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A458" s="0" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="B458" s="0" t="n">
         <v>28</v>
@@ -4917,7 +4920,7 @@
     </row>
     <row r="472" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A472" s="0" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
start route 110 trainers & route 103 eastern end trainers
</commit_message>
<xml_diff>
--- a/trainers/trainers.xlsx
+++ b/trainers/trainers.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="932" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="973" uniqueCount="275">
   <si>
     <t xml:space="preserve">TRAINER_MAY_ROUTE_103_TREECKO</t>
   </si>
@@ -805,7 +805,46 @@
     <t xml:space="preserve">Qwilfish</t>
   </si>
   <si>
-    <t xml:space="preserve">END</t>
+    <t xml:space="preserve"># route 110</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRAINER_KALEB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alolan_Vulpix</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vulpix</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRAINER_ISABEL_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Snubbull</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clefairy</t>
+  </si>
+  <si>
+    <t xml:space="preserve"># route 103 eastern end</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRAINER_AMY_AND_LIV_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plusle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Minun</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRAINER_DAISY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Budew</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bayleef</t>
   </si>
 </sst>
 </file>
@@ -906,10 +945,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G472"/>
+  <dimension ref="A1:G482"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A403" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A434" activeCellId="0" sqref="A434"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A441" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B483" activeCellId="0" sqref="B483"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4918,9 +4957,193 @@
         <v>28</v>
       </c>
     </row>
+    <row r="460" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A460" s="0" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="462" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A462" s="0" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="463" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A463" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B463" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C463" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D463" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E463" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F463" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G463" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="464" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A464" s="0" t="s">
+        <v>263</v>
+      </c>
+      <c r="B464" s="0" t="n">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="465" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A465" s="0" t="s">
+        <v>264</v>
+      </c>
+      <c r="B465" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="G465" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="467" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A467" s="0" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="468" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A468" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B468" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C468" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D468" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E468" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F468" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G468" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="469" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A469" s="0" t="s">
+        <v>266</v>
+      </c>
+      <c r="B469" s="0" t="n">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="470" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A470" s="0" t="s">
+        <v>267</v>
+      </c>
+      <c r="B470" s="0" t="n">
+        <v>28</v>
+      </c>
+    </row>
     <row r="472" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A472" s="0" t="s">
-        <v>261</v>
+        <v>268</v>
+      </c>
+    </row>
+    <row r="474" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A474" s="0" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="475" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A475" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B475" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C475" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D475" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E475" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F475" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G475" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="476" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A476" s="0" t="s">
+        <v>270</v>
+      </c>
+      <c r="B476" s="0" t="n">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="477" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A477" s="0" t="s">
+        <v>271</v>
+      </c>
+      <c r="B477" s="0" t="n">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="479" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A479" s="0" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="480" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A480" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B480" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C480" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D480" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E480" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F480" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G480" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="481" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A481" s="0" t="s">
+        <v>273</v>
+      </c>
+      <c r="B481" s="0" t="n">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="482" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A482" s="0" t="s">
+        <v>274</v>
+      </c>
+      <c r="B482" s="0" t="n">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix typos, route 110 rival pokemon
</commit_message>
<xml_diff>
--- a/trainers/trainers.xlsx
+++ b/trainers/trainers.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="973" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1055" uniqueCount="285">
   <si>
     <t xml:space="preserve">TRAINER_MAY_ROUTE_103_TREECKO</t>
   </si>
@@ -805,6 +805,27 @@
     <t xml:space="preserve">Qwilfish</t>
   </si>
   <si>
+    <t xml:space="preserve"># route 103 eastern end</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRAINER_AMY_AND_LIV_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plusle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Minun</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRAINER_DAISY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Budew</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bayleef</t>
+  </si>
+  <si>
     <t xml:space="preserve"># route 110</t>
   </si>
   <si>
@@ -826,25 +847,34 @@
     <t xml:space="preserve">Clefairy</t>
   </si>
   <si>
-    <t xml:space="preserve"># route 103 eastern end</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TRAINER_AMY_AND_LIV_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Plusle</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Minun</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TRAINER_DAISY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Budew</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bayleef</t>
+    <t xml:space="preserve">TRAINER_TIMMY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Skiploom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRAINER_MAY_ROUTE_110_TREECKO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRAINER_MAY_ROUTE_110_TORCHIC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quilava</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ivysaur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRAINER_MAY_ROUTE_110_MUDKIP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRAINER_BRENDAN_ROUTE_110_TREECKO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRAINER_BRENDAN_ROUTE_110_TORCHIC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRAINER_BRENDAN_ROUTE_110_MUDKIP</t>
   </si>
 </sst>
 </file>
@@ -945,10 +975,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G482"/>
+  <dimension ref="A1:G523"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A441" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B483" activeCellId="0" sqref="B483"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A482" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D522" activeCellId="0" sqref="D522"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4995,7 +5025,7 @@
         <v>263</v>
       </c>
       <c r="B464" s="0" t="n">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="465" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5003,10 +5033,7 @@
         <v>264</v>
       </c>
       <c r="B465" s="0" t="n">
-        <v>27</v>
-      </c>
-      <c r="G465" s="0" t="n">
-        <v>1</v>
+        <v>28</v>
       </c>
     </row>
     <row r="467" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5050,7 +5077,7 @@
         <v>267</v>
       </c>
       <c r="B470" s="0" t="n">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="472" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5091,7 +5118,7 @@
         <v>270</v>
       </c>
       <c r="B476" s="0" t="n">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="477" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5099,7 +5126,10 @@
         <v>271</v>
       </c>
       <c r="B477" s="0" t="n">
-        <v>28</v>
+        <v>27</v>
+      </c>
+      <c r="G477" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="479" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5143,6 +5173,380 @@
         <v>274</v>
       </c>
       <c r="B482" s="0" t="n">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="484" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A484" s="0" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="485" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A485" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B485" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C485" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D485" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E485" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F485" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G485" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="486" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A486" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="B486" s="0" t="n">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="487" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A487" s="0" t="s">
+        <v>276</v>
+      </c>
+      <c r="B487" s="0" t="n">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="489" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A489" s="0" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="490" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A490" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B490" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C490" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D490" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E490" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F490" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G490" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="491" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A491" s="0" t="s">
+        <v>267</v>
+      </c>
+      <c r="B491" s="0" t="n">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="492" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A492" s="0" t="s">
+        <v>206</v>
+      </c>
+      <c r="B492" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="D492" s="0" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="493" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A493" s="0" t="s">
+        <v>185</v>
+      </c>
+      <c r="B493" s="0" t="n">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="495" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A495" s="0" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="496" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A496" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B496" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C496" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D496" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E496" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F496" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G496" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="497" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A497" s="0" t="s">
+        <v>279</v>
+      </c>
+      <c r="B497" s="0" t="n">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="498" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A498" s="0" t="s">
+        <v>280</v>
+      </c>
+      <c r="B498" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="D498" s="0" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="499" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A499" s="0" t="s">
+        <v>188</v>
+      </c>
+      <c r="B499" s="0" t="n">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="501" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A501" s="0" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="502" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A502" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B502" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C502" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D502" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E502" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F502" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G502" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="503" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A503" s="0" t="s">
+        <v>210</v>
+      </c>
+      <c r="B503" s="0" t="n">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="504" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A504" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="B504" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="D504" s="0" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="505" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A505" s="0" t="s">
+        <v>190</v>
+      </c>
+      <c r="B505" s="0" t="n">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="507" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A507" s="0" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="508" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A508" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B508" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C508" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D508" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E508" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F508" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G508" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="509" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A509" s="0" t="s">
+        <v>267</v>
+      </c>
+      <c r="B509" s="0" t="n">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="510" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A510" s="0" t="s">
+        <v>206</v>
+      </c>
+      <c r="B510" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="D510" s="0" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="511" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A511" s="0" t="s">
+        <v>185</v>
+      </c>
+      <c r="B511" s="0" t="n">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="513" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A513" s="0" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="514" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A514" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B514" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C514" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D514" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E514" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F514" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G514" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="515" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A515" s="0" t="s">
+        <v>279</v>
+      </c>
+      <c r="B515" s="0" t="n">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="516" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A516" s="0" t="s">
+        <v>280</v>
+      </c>
+      <c r="B516" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="D516" s="0" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="517" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A517" s="0" t="s">
+        <v>188</v>
+      </c>
+      <c r="B517" s="0" t="n">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="519" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A519" s="0" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="520" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A520" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B520" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C520" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D520" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E520" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F520" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G520" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="521" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A521" s="0" t="s">
+        <v>210</v>
+      </c>
+      <c r="B521" s="0" t="n">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="522" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A522" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="B522" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="D522" s="0" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="523" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A523" s="0" t="s">
+        <v>190</v>
+      </c>
+      <c r="B523" s="0" t="n">
         <v>29</v>
       </c>
     </row>

</xml_diff>

<commit_message>
oceanic museum dialogue, route 110 wild mons and trainers
</commit_message>
<xml_diff>
--- a/trainers/trainers.xlsx
+++ b/trainers/trainers.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1055" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1166" uniqueCount="313">
   <si>
     <t xml:space="preserve">TRAINER_MAY_ROUTE_103_TREECKO</t>
   </si>
@@ -875,6 +875,90 @@
   </si>
   <si>
     <t xml:space="preserve">TRAINER_BRENDAN_ROUTE_110_MUDKIP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRAINER_EDWIN_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Turban</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Razor Shell, Poison Fang, Iron Defense, Clamp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Poison Touch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRAINER_JOSEPH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Galarian_Linoone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Electabuzz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRAINER_ALYSSA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Doduo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jolteon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRAINER_EDWARD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Drowzee</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kadabra</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRAINER_DALE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRAINER_JACLYN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kirlia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Espeon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRAINER_ABIGAIL_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ninjask</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fearow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRAINER_ANTHONY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Electrode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Swellow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRAINER_BENJAMIN_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Growlithe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRAINER_JASMINE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Metang</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRAINER_JACOB</t>
   </si>
 </sst>
 </file>
@@ -975,10 +1059,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G523"/>
+  <dimension ref="A1:G577"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A482" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D522" activeCellId="0" sqref="D522"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A545" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A579" activeCellId="0" sqref="A579"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5550,6 +5634,488 @@
         <v>29</v>
       </c>
     </row>
+    <row r="525" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A525" s="0" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="526" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A526" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B526" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C526" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D526" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E526" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F526" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G526" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="527" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A527" s="0" t="s">
+        <v>286</v>
+      </c>
+      <c r="B527" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="E527" s="0" t="s">
+        <v>287</v>
+      </c>
+      <c r="F527" s="0" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="529" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A529" s="0" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="530" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A530" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B530" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C530" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D530" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E530" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F530" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G530" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="531" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A531" s="0" t="s">
+        <v>290</v>
+      </c>
+      <c r="B531" s="0" t="n">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="532" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A532" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="B532" s="0" t="n">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="534" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A534" s="0" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="535" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A535" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B535" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C535" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D535" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E535" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F535" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G535" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="536" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A536" s="0" t="s">
+        <v>293</v>
+      </c>
+      <c r="B536" s="0" t="n">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="537" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A537" s="0" t="s">
+        <v>294</v>
+      </c>
+      <c r="B537" s="0" t="n">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="539" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A539" s="0" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="540" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A540" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B540" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C540" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D540" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E540" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F540" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G540" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="541" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A541" s="0" t="s">
+        <v>296</v>
+      </c>
+      <c r="B541" s="0" t="n">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="542" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A542" s="0" t="s">
+        <v>297</v>
+      </c>
+      <c r="B542" s="0" t="n">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="544" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A544" s="0" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="545" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A545" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B545" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C545" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D545" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E545" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F545" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G545" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="546" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A546" s="0" t="s">
+        <v>254</v>
+      </c>
+      <c r="B546" s="0" t="n">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="547" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A547" s="0" t="s">
+        <v>235</v>
+      </c>
+      <c r="B547" s="0" t="n">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="549" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A549" s="0" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="550" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A550" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B550" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C550" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D550" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E550" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F550" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G550" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="551" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A551" s="0" t="s">
+        <v>300</v>
+      </c>
+      <c r="B551" s="0" t="n">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="552" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A552" s="0" t="s">
+        <v>301</v>
+      </c>
+      <c r="B552" s="0" t="n">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="554" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A554" s="0" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="555" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A555" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B555" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C555" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D555" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E555" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F555" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G555" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="556" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A556" s="0" t="s">
+        <v>303</v>
+      </c>
+      <c r="B556" s="0" t="n">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="557" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A557" s="0" t="s">
+        <v>304</v>
+      </c>
+      <c r="B557" s="0" t="n">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="559" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A559" s="0" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="560" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A560" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B560" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C560" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D560" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E560" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F560" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G560" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="561" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A561" s="0" t="s">
+        <v>306</v>
+      </c>
+      <c r="B561" s="0" t="n">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="562" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A562" s="0" t="s">
+        <v>307</v>
+      </c>
+      <c r="B562" s="0" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="564" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A564" s="0" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="565" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A565" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B565" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C565" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D565" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E565" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F565" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G565" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A566" s="0" t="s">
+        <v>309</v>
+      </c>
+      <c r="B566" s="0" t="n">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A567" s="0" t="s">
+        <v>251</v>
+      </c>
+      <c r="B567" s="0" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A569" s="0" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A570" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B570" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C570" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D570" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E570" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F570" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G570" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A571" s="0" t="s">
+        <v>249</v>
+      </c>
+      <c r="B571" s="0" t="n">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A572" s="0" t="s">
+        <v>311</v>
+      </c>
+      <c r="B572" s="0" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A574" s="0" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A575" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B575" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C575" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D575" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E575" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F575" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G575" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A576" s="0" t="s">
+        <v>219</v>
+      </c>
+      <c r="B576" s="0" t="n">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="577" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A577" s="0" t="s">
+        <v>311</v>
+      </c>
+      <c r="B577" s="0" t="n">
+        <v>31</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
bike shop scripts, mauville city wally team
</commit_message>
<xml_diff>
--- a/trainers/trainers.xlsx
+++ b/trainers/trainers.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1166" uniqueCount="313">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1176" uniqueCount="315">
   <si>
     <t xml:space="preserve">TRAINER_MAY_ROUTE_103_TREECKO</t>
   </si>
@@ -959,6 +959,12 @@
   </si>
   <si>
     <t xml:space="preserve">TRAINER_JACOB</t>
+  </si>
+  <si>
+    <t xml:space="preserve"># mauville city</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRAINER_WALLY_MAUVILLE</t>
   </si>
 </sst>
 </file>
@@ -1059,10 +1065,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G577"/>
+  <dimension ref="A1:G583"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A545" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A579" activeCellId="0" sqref="A579"/>
+      <selection pane="topLeft" activeCell="A580" activeCellId="0" sqref="A580"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6116,6 +6122,47 @@
         <v>31</v>
       </c>
     </row>
+    <row r="579" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A579" s="0" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="581" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A581" s="0" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="582" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A582" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B582" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C582" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D582" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E582" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F582" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G582" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="583" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A583" s="0" t="s">
+        <v>300</v>
+      </c>
+      <c r="B583" s="0" t="n">
+        <v>29</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
fix game corner second stone set, mauville gym trainers
</commit_message>
<xml_diff>
--- a/trainers/trainers.xlsx
+++ b/trainers/trainers.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1176" uniqueCount="315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1241" uniqueCount="332">
   <si>
     <t xml:space="preserve">TRAINER_MAY_ROUTE_103_TREECKO</t>
   </si>
@@ -961,10 +961,61 @@
     <t xml:space="preserve">TRAINER_JACOB</t>
   </si>
   <si>
+    <t xml:space="preserve">Loudred</t>
+  </si>
+  <si>
     <t xml:space="preserve"># mauville city</t>
   </si>
   <si>
     <t xml:space="preserve">TRAINER_WALLY_MAUVILLE</t>
+  </si>
+  <si>
+    <t xml:space="preserve"># mauville gym</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRAINER_VIVIAN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Flaaffy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRAINER_KIRK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alolan_Graveler</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRAINER_ANGELO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Magneton</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tri Attack, Spark, Magnet Rise</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sturdy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRAINER_SHAWN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Magnemite</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRAINER_BEN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRAINER_WATTSON_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manectric</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alolan_Raichu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Numpuff</t>
   </si>
 </sst>
 </file>
@@ -1065,10 +1116,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G583"/>
+  <dimension ref="A1:G617"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A545" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A580" activeCellId="0" sqref="A580"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A561" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H597" activeCellId="0" sqref="H597"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6116,7 +6167,7 @@
     </row>
     <row r="577" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A577" s="0" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="B577" s="0" t="n">
         <v>31</v>
@@ -6124,12 +6175,12 @@
     </row>
     <row r="579" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A579" s="0" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
     </row>
     <row r="581" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A581" s="0" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
     </row>
     <row r="582" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6161,6 +6212,300 @@
       </c>
       <c r="B583" s="0" t="n">
         <v>29</v>
+      </c>
+    </row>
+    <row r="585" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A585" s="0" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="587" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A587" s="0" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="588" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A588" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B588" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C588" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D588" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E588" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F588" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G588" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="589" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A589" s="0" t="s">
+        <v>170</v>
+      </c>
+      <c r="B589" s="0" t="n">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="590" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A590" s="0" t="s">
+        <v>318</v>
+      </c>
+      <c r="B590" s="0" t="n">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="592" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A592" s="0" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="593" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A593" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B593" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C593" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D593" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E593" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F593" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G593" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="594" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A594" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="B594" s="0" t="n">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="595" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A595" s="0" t="s">
+        <v>320</v>
+      </c>
+      <c r="B595" s="0" t="n">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="597" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A597" s="0" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="598" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A598" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B598" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C598" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D598" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E598" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F598" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G598" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="599" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A599" s="0" t="s">
+        <v>322</v>
+      </c>
+      <c r="B599" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="E599" s="0" t="s">
+        <v>323</v>
+      </c>
+      <c r="F599" s="0" t="s">
+        <v>324</v>
+      </c>
+      <c r="G599" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="600" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A600" s="0" t="s">
+        <v>306</v>
+      </c>
+      <c r="B600" s="0" t="n">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="602" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A602" s="0" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="603" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A603" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B603" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C603" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D603" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E603" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F603" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G603" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="604" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A604" s="0" t="s">
+        <v>326</v>
+      </c>
+      <c r="B604" s="0" t="n">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="605" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A605" s="0" t="s">
+        <v>294</v>
+      </c>
+      <c r="B605" s="0" t="n">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="607" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A607" s="0" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="608" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A608" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B608" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C608" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D608" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E608" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F608" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G608" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="609" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A609" s="0" t="s">
+        <v>170</v>
+      </c>
+      <c r="B609" s="0" t="n">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="610" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A610" s="0" t="s">
+        <v>252</v>
+      </c>
+      <c r="B610" s="0" t="n">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="611" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A611" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="B611" s="0" t="n">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="613" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A613" s="0" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="614" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A614" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B614" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C614" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D614" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E614" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F614" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G614" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="615" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A615" s="0" t="s">
+        <v>329</v>
+      </c>
+      <c r="B615" s="0" t="n">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="616" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A616" s="0" t="s">
+        <v>330</v>
+      </c>
+      <c r="B616" s="0" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="617" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A617" s="0" t="s">
+        <v>331</v>
+      </c>
+      <c r="B617" s="0" t="n">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
wattson's team, adjust qwilfish & numpuff moves
</commit_message>
<xml_diff>
--- a/trainers/trainers.xlsx
+++ b/trainers/trainers.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1241" uniqueCount="332">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1247" uniqueCount="338">
   <si>
     <t xml:space="preserve">TRAINER_MAY_ROUTE_103_TREECKO</t>
   </si>
@@ -1012,10 +1012,28 @@
     <t xml:space="preserve">Manectric</t>
   </si>
   <si>
+    <t xml:space="preserve">Shock Wave, Thunder Fang, Bite, Howl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Static</t>
+  </si>
+  <si>
     <t xml:space="preserve">Alolan_Raichu</t>
   </si>
   <si>
+    <t xml:space="preserve">Shock Wave, Psybeam, Agility, Double Team</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Levitate</t>
+  </si>
+  <si>
     <t xml:space="preserve">Numpuff</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shock Wave, Thunder Wave, Sludge, Water Pulse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aftermath</t>
   </si>
 </sst>
 </file>
@@ -1118,8 +1136,8 @@
   </sheetPr>
   <dimension ref="A1:G617"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A561" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H597" activeCellId="0" sqref="H597"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A580" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F615" activeCellId="0" sqref="F615"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6491,21 +6509,39 @@
       <c r="B615" s="0" t="n">
         <v>34</v>
       </c>
+      <c r="E615" s="0" t="s">
+        <v>330</v>
+      </c>
+      <c r="F615" s="0" t="s">
+        <v>331</v>
+      </c>
     </row>
     <row r="616" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A616" s="0" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="B616" s="0" t="n">
         <v>35</v>
       </c>
+      <c r="E616" s="0" t="s">
+        <v>333</v>
+      </c>
+      <c r="F616" s="0" t="s">
+        <v>334</v>
+      </c>
     </row>
     <row r="617" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A617" s="0" t="s">
-        <v>331</v>
+        <v>335</v>
       </c>
       <c r="B617" s="0" t="n">
         <v>36</v>
+      </c>
+      <c r="E617" s="0" t="s">
+        <v>336</v>
+      </c>
+      <c r="F617" s="0" t="s">
+        <v>337</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
alolan raichu moves, wattson's team
</commit_message>
<xml_diff>
--- a/trainers/trainers.xlsx
+++ b/trainers/trainers.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1247" uniqueCount="338">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1247" uniqueCount="339">
   <si>
     <t xml:space="preserve">TRAINER_MAY_ROUTE_103_TREECKO</t>
   </si>
@@ -991,12 +991,12 @@
     <t xml:space="preserve">Magneton</t>
   </si>
   <si>
-    <t xml:space="preserve">Tri Attack, Spark, Magnet Rise</t>
-  </si>
-  <si>
     <t xml:space="preserve">Sturdy</t>
   </si>
   <si>
+    <t xml:space="preserve">Voltorb</t>
+  </si>
+  <si>
     <t xml:space="preserve">TRAINER_SHAWN</t>
   </si>
   <si>
@@ -1012,7 +1012,7 @@
     <t xml:space="preserve">Manectric</t>
   </si>
   <si>
-    <t xml:space="preserve">Shock Wave, Thunder Fang, Bite, Howl</t>
+    <t xml:space="preserve">Shock Wave, Thunder Fang, Bite</t>
   </si>
   <si>
     <t xml:space="preserve">Static</t>
@@ -1021,7 +1021,7 @@
     <t xml:space="preserve">Alolan_Raichu</t>
   </si>
   <si>
-    <t xml:space="preserve">Shock Wave, Psybeam, Agility, Double Team</t>
+    <t xml:space="preserve">Shock Wave, Confusion, Agility</t>
   </si>
   <si>
     <t xml:space="preserve">Levitate</t>
@@ -1030,10 +1030,13 @@
     <t xml:space="preserve">Numpuff</t>
   </si>
   <si>
-    <t xml:space="preserve">Shock Wave, Thunder Wave, Sludge, Water Pulse</t>
+    <t xml:space="preserve">Shock Wave, Spark, Sludge, Water Pulse</t>
   </si>
   <si>
     <t xml:space="preserve">Aftermath</t>
+  </si>
+  <si>
+    <t xml:space="preserve">END</t>
   </si>
 </sst>
 </file>
@@ -1134,10 +1137,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G617"/>
+  <dimension ref="A1:G619"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A580" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F615" activeCellId="0" sqref="F615"/>
+      <selection pane="topLeft" activeCell="E617" activeCellId="0" sqref="E617"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6360,11 +6363,8 @@
       <c r="B599" s="0" t="n">
         <v>32</v>
       </c>
-      <c r="E599" s="0" t="s">
+      <c r="F599" s="0" t="s">
         <v>323</v>
-      </c>
-      <c r="F599" s="0" t="s">
-        <v>324</v>
       </c>
       <c r="G599" s="0" t="n">
         <v>1</v>
@@ -6372,7 +6372,7 @@
     </row>
     <row r="600" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A600" s="0" t="s">
-        <v>306</v>
+        <v>324</v>
       </c>
       <c r="B600" s="0" t="n">
         <v>33</v>
@@ -6455,7 +6455,7 @@
         <v>170</v>
       </c>
       <c r="B609" s="0" t="n">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="610" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6463,7 +6463,7 @@
         <v>252</v>
       </c>
       <c r="B610" s="0" t="n">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="611" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6471,7 +6471,7 @@
         <v>291</v>
       </c>
       <c r="B611" s="0" t="n">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="613" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6507,7 +6507,7 @@
         <v>329</v>
       </c>
       <c r="B615" s="0" t="n">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E615" s="0" t="s">
         <v>330</v>
@@ -6521,7 +6521,7 @@
         <v>332</v>
       </c>
       <c r="B616" s="0" t="n">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E616" s="0" t="s">
         <v>333</v>
@@ -6535,13 +6535,18 @@
         <v>335</v>
       </c>
       <c r="B617" s="0" t="n">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E617" s="0" t="s">
         <v>336</v>
       </c>
       <c r="F617" s="0" t="s">
         <v>337</v>
+      </c>
+    </row>
+    <row r="619" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A619" s="0" t="s">
+        <v>338</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
rhyolite canyon team magma
</commit_message>
<xml_diff>
--- a/trainers/trainers.xlsx
+++ b/trainers/trainers.xlsx
@@ -1137,10 +1137,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G619"/>
+  <dimension ref="A1:G621"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A580" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E617" activeCellId="0" sqref="E617"/>
+      <selection pane="topLeft" activeCell="A618" activeCellId="0" sqref="618:618"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6544,8 +6544,8 @@
         <v>337</v>
       </c>
     </row>
-    <row r="619" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A619" s="0" t="s">
+    <row r="621" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A621" s="0" t="s">
         <v>338</v>
       </c>
     </row>

</xml_diff>

<commit_message>
adjust wild pokemon and trainer levels on dewford and flanking routes
</commit_message>
<xml_diff>
--- a/trainers/trainers.xlsx
+++ b/trainers/trainers.xlsx
@@ -706,7 +706,7 @@
     <t xml:space="preserve">TRAINER_BRAWLY_1</t>
   </si>
   <si>
-    <t xml:space="preserve">Vital Throw, Knock Off, Belly Drum, Focus Energy</t>
+    <t xml:space="preserve">Vital Throw, Smelling Salt, Belly Drum, Focus Energy</t>
   </si>
   <si>
     <t xml:space="preserve">Guts</t>
@@ -715,7 +715,7 @@
     <t xml:space="preserve">Poliwrath</t>
   </si>
   <si>
-    <t xml:space="preserve">Brick Break, Bubble Beam, Hypnosis, Double Slap</t>
+    <t xml:space="preserve">Brick Break, Bubble Beam, Double Slap</t>
   </si>
   <si>
     <t xml:space="preserve">Damp</t>
@@ -1043,8 +1043,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="0.00\ %"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -1111,12 +1112,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1139,8 +1144,8 @@
   </sheetPr>
   <dimension ref="A1:G621"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A580" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A618" activeCellId="0" sqref="618:618"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A371" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E398" activeCellId="0" sqref="E398"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4048,7 +4053,7 @@
         <v>170</v>
       </c>
       <c r="B329" s="0" t="n">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E329" s="0" t="s">
         <v>198</v>
@@ -4087,7 +4092,7 @@
         <v>200</v>
       </c>
       <c r="B333" s="0" t="n">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D333" s="0" t="s">
         <v>101</v>
@@ -4098,7 +4103,7 @@
         <v>201</v>
       </c>
       <c r="B334" s="0" t="n">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="336" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4134,7 +4139,7 @@
         <v>203</v>
       </c>
       <c r="B338" s="0" t="n">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="339" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4142,7 +4147,7 @@
         <v>204</v>
       </c>
       <c r="B339" s="0" t="n">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="341" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4178,7 +4183,7 @@
         <v>206</v>
       </c>
       <c r="B343" s="0" t="n">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="345" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4214,7 +4219,7 @@
         <v>95</v>
       </c>
       <c r="B347" s="0" t="n">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="348" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4222,7 +4227,7 @@
         <v>207</v>
       </c>
       <c r="B348" s="0" t="n">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="350" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4258,7 +4263,7 @@
         <v>209</v>
       </c>
       <c r="B352" s="0" t="n">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="353" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4266,7 +4271,7 @@
         <v>210</v>
       </c>
       <c r="B353" s="0" t="n">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="355" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4307,7 +4312,7 @@
         <v>213</v>
       </c>
       <c r="B359" s="0" t="n">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="360" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4315,7 +4320,7 @@
         <v>214</v>
       </c>
       <c r="B360" s="0" t="n">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="362" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4351,7 +4356,7 @@
         <v>216</v>
       </c>
       <c r="B364" s="0" t="n">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="366" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4392,7 +4397,7 @@
         <v>219</v>
       </c>
       <c r="B370" s="0" t="n">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="371" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4400,7 +4405,7 @@
         <v>87</v>
       </c>
       <c r="B371" s="0" t="n">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="373" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4436,7 +4441,7 @@
         <v>91</v>
       </c>
       <c r="B375" s="0" t="n">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="376" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4444,7 +4449,7 @@
         <v>87</v>
       </c>
       <c r="B376" s="0" t="n">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="378" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4480,7 +4485,7 @@
         <v>222</v>
       </c>
       <c r="B380" s="0" t="n">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="382" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4516,7 +4521,7 @@
         <v>224</v>
       </c>
       <c r="B384" s="0" t="n">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="386" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4552,7 +4557,7 @@
         <v>60</v>
       </c>
       <c r="B388" s="0" t="n">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="389" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4560,7 +4565,7 @@
         <v>87</v>
       </c>
       <c r="B389" s="0" t="n">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="391" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4596,7 +4601,7 @@
         <v>185</v>
       </c>
       <c r="B393" s="0" t="n">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="395" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4632,7 +4637,7 @@
         <v>91</v>
       </c>
       <c r="B397" s="0" t="n">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E397" s="0" t="s">
         <v>228</v>
@@ -4646,7 +4651,7 @@
         <v>230</v>
       </c>
       <c r="B398" s="0" t="n">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E398" s="0" t="s">
         <v>231</v>
@@ -4791,6 +4796,7 @@
       <c r="B415" s="0" t="n">
         <v>25</v>
       </c>
+      <c r="E415" s="2"/>
     </row>
     <row r="417" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A417" s="0" t="s">

</xml_diff>

<commit_message>
adjust more trainer levels
</commit_message>
<xml_diff>
--- a/trainers/trainers.xlsx
+++ b/trainers/trainers.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1249" uniqueCount="339">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1248" uniqueCount="340">
   <si>
     <t xml:space="preserve">TRAINER_MAY_ROUTE_103_TREECKO</t>
   </si>
@@ -706,7 +706,10 @@
     <t xml:space="preserve">TRAINER_BRAWLY_1</t>
   </si>
   <si>
-    <t xml:space="preserve">Cross Chop, Fire Punch, Bulk Up, Leer</t>
+    <t xml:space="preserve">Salac Berry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cross Chop, Fire Punch, Bulk Up, Focus Energy</t>
   </si>
   <si>
     <t xml:space="preserve">Defiant</t>
@@ -715,10 +718,10 @@
     <t xml:space="preserve">Chesto Berry</t>
   </si>
   <si>
-    <t xml:space="preserve">Bulk Up, Rest, Sleep Talk, Force Palm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Guts</t>
+    <t xml:space="preserve">Bulk Up, Rest, Smelling Salt, Force Palm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thick Fat</t>
   </si>
   <si>
     <t xml:space="preserve"># route 109</t>
@@ -769,9 +772,6 @@
     <t xml:space="preserve">TRAINER_DWAYNE</t>
   </si>
   <si>
-    <t xml:space="preserve">Machoke</t>
-  </si>
-  <si>
     <t xml:space="preserve">TRAINER_JOHANNA</t>
   </si>
   <si>
@@ -953,6 +953,9 @@
   </si>
   <si>
     <t xml:space="preserve">TRAINER_JASMINE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Breloom</t>
   </si>
   <si>
     <t xml:space="preserve">Metang</t>
@@ -1142,10 +1145,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G621"/>
+  <dimension ref="A1:G620"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A371" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D398" activeCellId="0" sqref="D398"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A577" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E616" activeCellId="0" sqref="E616"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4639,14 +4642,17 @@
       <c r="B397" s="0" t="n">
         <v>24</v>
       </c>
+      <c r="C397" s="0" t="n">
+        <v>100</v>
+      </c>
       <c r="D397" s="0" t="s">
-        <v>101</v>
+        <v>228</v>
       </c>
       <c r="E397" s="1" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="F397" s="0" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="398" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4656,24 +4662,27 @@
       <c r="B398" s="0" t="n">
         <v>25</v>
       </c>
+      <c r="C398" s="0" t="n">
+        <v>100</v>
+      </c>
       <c r="D398" s="0" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="E398" s="0" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="F398" s="0" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="400" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A400" s="0" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
     </row>
     <row r="402" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A402" s="0" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
     </row>
     <row r="403" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4701,1770 +4710,1770 @@
     </row>
     <row r="404" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A404" s="0" t="s">
-        <v>87</v>
+        <v>236</v>
       </c>
       <c r="B404" s="0" t="n">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="405" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A405" s="0" t="s">
-        <v>235</v>
-      </c>
-      <c r="B405" s="0" t="n">
-        <v>24</v>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="406" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A406" s="0" t="s">
+        <v>237</v>
       </c>
     </row>
     <row r="407" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A407" s="0" t="s">
-        <v>236</v>
+        <v>1</v>
+      </c>
+      <c r="B407" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C407" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D407" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E407" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F407" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G407" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="408" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A408" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B408" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C408" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D408" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="E408" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F408" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="G408" s="0" t="s">
-        <v>7</v>
+        <v>71</v>
+      </c>
+      <c r="B408" s="0" t="n">
+        <v>22</v>
       </c>
     </row>
     <row r="409" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A409" s="0" t="s">
-        <v>71</v>
+        <v>238</v>
       </c>
       <c r="B409" s="0" t="n">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="410" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A410" s="0" t="s">
-        <v>237</v>
-      </c>
-      <c r="B410" s="0" t="n">
-        <v>25</v>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="411" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A411" s="0" t="s">
+        <v>239</v>
       </c>
     </row>
     <row r="412" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A412" s="0" t="s">
-        <v>238</v>
+        <v>1</v>
+      </c>
+      <c r="B412" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C412" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D412" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E412" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F412" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G412" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="413" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A413" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B413" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C413" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D413" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="E413" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F413" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="G413" s="0" t="s">
-        <v>7</v>
+        <v>240</v>
+      </c>
+      <c r="B413" s="0" t="n">
+        <v>22</v>
       </c>
     </row>
     <row r="414" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A414" s="0" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="B414" s="0" t="n">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="415" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A415" s="0" t="s">
-        <v>240</v>
-      </c>
-      <c r="B415" s="0" t="n">
-        <v>25</v>
-      </c>
-      <c r="E415" s="2"/>
+        <v>22</v>
+      </c>
+      <c r="E414" s="2"/>
+    </row>
+    <row r="416" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A416" s="0" t="s">
+        <v>242</v>
+      </c>
     </row>
     <row r="417" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A417" s="0" t="s">
-        <v>241</v>
+        <v>1</v>
+      </c>
+      <c r="B417" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C417" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D417" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E417" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F417" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G417" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="418" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A418" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B418" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C418" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D418" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="E418" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F418" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="G418" s="0" t="s">
-        <v>7</v>
+        <v>10</v>
+      </c>
+      <c r="B418" s="0" t="n">
+        <v>22</v>
       </c>
     </row>
     <row r="419" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A419" s="0" t="s">
-        <v>10</v>
+        <v>203</v>
       </c>
       <c r="B419" s="0" t="n">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="420" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A420" s="0" t="s">
-        <v>203</v>
-      </c>
-      <c r="B420" s="0" t="n">
-        <v>25</v>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="421" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A421" s="0" t="s">
+        <v>243</v>
       </c>
     </row>
     <row r="422" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A422" s="0" t="s">
-        <v>242</v>
+        <v>1</v>
+      </c>
+      <c r="B422" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C422" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D422" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E422" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F422" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G422" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="423" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A423" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B423" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C423" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D423" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="E423" s="1" t="s">
-        <v>5</v>
+        <v>244</v>
+      </c>
+      <c r="B423" s="0" t="n">
+        <v>24</v>
       </c>
       <c r="F423" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="G423" s="0" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="424" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A424" s="0" t="s">
-        <v>243</v>
-      </c>
-      <c r="B424" s="0" t="n">
-        <v>25</v>
-      </c>
-      <c r="F424" s="0" t="s">
-        <v>244</v>
+        <v>245</v>
+      </c>
+    </row>
+    <row r="425" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A425" s="0" t="s">
+        <v>246</v>
       </c>
     </row>
     <row r="426" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A426" s="0" t="s">
-        <v>245</v>
+        <v>1</v>
+      </c>
+      <c r="B426" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C426" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D426" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E426" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F426" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G426" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="427" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A427" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B427" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C427" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D427" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="E427" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F427" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="G427" s="0" t="s">
-        <v>7</v>
+        <v>247</v>
+      </c>
+      <c r="B427" s="0" t="n">
+        <v>22</v>
       </c>
     </row>
     <row r="428" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A428" s="0" t="s">
-        <v>246</v>
+        <v>37</v>
       </c>
       <c r="B428" s="0" t="n">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="429" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A429" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="B429" s="0" t="n">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="431" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A431" s="0" t="s">
-        <v>247</v>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="430" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A430" s="0" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="432" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A432" s="0" t="s">
+        <v>249</v>
       </c>
     </row>
     <row r="433" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A433" s="0" t="s">
-        <v>248</v>
+        <v>1</v>
+      </c>
+      <c r="B433" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C433" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D433" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E433" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F433" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G433" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="434" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A434" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B434" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C434" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D434" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="E434" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F434" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="G434" s="0" t="s">
-        <v>7</v>
+        <v>188</v>
+      </c>
+      <c r="B434" s="0" t="n">
+        <v>24</v>
       </c>
     </row>
     <row r="435" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A435" s="0" t="s">
-        <v>188</v>
+        <v>87</v>
       </c>
       <c r="B435" s="0" t="n">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="436" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A436" s="0" t="s">
-        <v>249</v>
-      </c>
-      <c r="B436" s="0" t="n">
-        <v>28</v>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="437" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A437" s="0" t="s">
+        <v>250</v>
       </c>
     </row>
     <row r="438" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A438" s="0" t="s">
-        <v>250</v>
+        <v>1</v>
+      </c>
+      <c r="B438" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C438" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D438" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E438" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F438" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G438" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="439" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A439" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B439" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C439" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D439" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="E439" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F439" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="G439" s="0" t="s">
-        <v>7</v>
+        <v>251</v>
+      </c>
+      <c r="B439" s="0" t="n">
+        <v>23</v>
       </c>
     </row>
     <row r="440" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A440" s="0" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="B440" s="0" t="n">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="441" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A441" s="0" t="s">
-        <v>252</v>
-      </c>
-      <c r="B441" s="0" t="n">
-        <v>27</v>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="442" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A442" s="0" t="s">
+        <v>253</v>
       </c>
     </row>
     <row r="443" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A443" s="0" t="s">
-        <v>253</v>
+        <v>1</v>
+      </c>
+      <c r="B443" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C443" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D443" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E443" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F443" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G443" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="444" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A444" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B444" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C444" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D444" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="E444" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F444" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="G444" s="0" t="s">
-        <v>7</v>
+        <v>254</v>
+      </c>
+      <c r="B444" s="0" t="n">
+        <v>24</v>
       </c>
     </row>
     <row r="445" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A445" s="0" t="s">
-        <v>254</v>
+        <v>99</v>
       </c>
       <c r="B445" s="0" t="n">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="446" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A446" s="0" t="s">
-        <v>99</v>
-      </c>
-      <c r="B446" s="0" t="n">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="448" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A448" s="0" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="447" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A447" s="0" t="s">
         <v>255</v>
+      </c>
+    </row>
+    <row r="449" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A449" s="0" t="s">
+        <v>256</v>
       </c>
     </row>
     <row r="450" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A450" s="0" t="s">
-        <v>256</v>
+        <v>1</v>
+      </c>
+      <c r="B450" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C450" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D450" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E450" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F450" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G450" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="451" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A451" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B451" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C451" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D451" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="E451" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F451" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="G451" s="0" t="s">
-        <v>7</v>
+        <v>204</v>
+      </c>
+      <c r="B451" s="0" t="n">
+        <v>24</v>
       </c>
     </row>
     <row r="452" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A452" s="0" t="s">
-        <v>204</v>
+        <v>257</v>
       </c>
       <c r="B452" s="0" t="n">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="453" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A453" s="0" t="s">
-        <v>257</v>
-      </c>
-      <c r="B453" s="0" t="n">
-        <v>27</v>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="454" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A454" s="0" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="455" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A455" s="0" t="s">
-        <v>258</v>
+        <v>1</v>
+      </c>
+      <c r="B455" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C455" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D455" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E455" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F455" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G455" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="456" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A456" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B456" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C456" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D456" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="E456" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F456" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="G456" s="0" t="s">
-        <v>7</v>
+        <v>259</v>
+      </c>
+      <c r="B456" s="0" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="457" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A457" s="0" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="B457" s="0" t="n">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="458" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A458" s="0" t="s">
-        <v>260</v>
-      </c>
-      <c r="B458" s="0" t="n">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="460" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A460" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="459" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A459" s="0" t="s">
         <v>261</v>
+      </c>
+    </row>
+    <row r="461" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A461" s="0" t="s">
+        <v>262</v>
       </c>
     </row>
     <row r="462" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A462" s="0" t="s">
-        <v>262</v>
+        <v>1</v>
+      </c>
+      <c r="B462" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C462" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D462" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E462" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F462" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G462" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="463" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A463" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B463" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C463" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D463" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="E463" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F463" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="G463" s="0" t="s">
-        <v>7</v>
+        <v>263</v>
+      </c>
+      <c r="B463" s="0" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="464" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A464" s="0" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="B464" s="0" t="n">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="465" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A465" s="0" t="s">
-        <v>264</v>
-      </c>
-      <c r="B465" s="0" t="n">
-        <v>28</v>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="466" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A466" s="0" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="467" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A467" s="0" t="s">
-        <v>265</v>
+        <v>1</v>
+      </c>
+      <c r="B467" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C467" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D467" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E467" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F467" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G467" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="468" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A468" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B468" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C468" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D468" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="E468" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F468" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="G468" s="0" t="s">
-        <v>7</v>
+        <v>266</v>
+      </c>
+      <c r="B468" s="0" t="n">
+        <v>24</v>
       </c>
     </row>
     <row r="469" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A469" s="0" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="B469" s="0" t="n">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="470" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A470" s="0" t="s">
-        <v>267</v>
-      </c>
-      <c r="B470" s="0" t="n">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="472" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A472" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="471" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A471" s="0" t="s">
         <v>268</v>
+      </c>
+    </row>
+    <row r="473" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A473" s="0" t="s">
+        <v>269</v>
       </c>
     </row>
     <row r="474" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A474" s="0" t="s">
-        <v>269</v>
+        <v>1</v>
+      </c>
+      <c r="B474" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C474" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D474" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E474" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F474" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G474" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="475" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A475" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B475" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C475" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D475" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="E475" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F475" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="G475" s="0" t="s">
-        <v>7</v>
+        <v>270</v>
+      </c>
+      <c r="B475" s="0" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="476" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A476" s="0" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="B476" s="0" t="n">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="477" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A477" s="0" t="s">
-        <v>271</v>
-      </c>
-      <c r="B477" s="0" t="n">
-        <v>27</v>
-      </c>
-      <c r="G477" s="0" t="n">
-        <v>1</v>
+        <v>25</v>
+      </c>
+      <c r="G476" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="478" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A478" s="0" t="s">
+        <v>272</v>
       </c>
     </row>
     <row r="479" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A479" s="0" t="s">
-        <v>272</v>
+        <v>1</v>
+      </c>
+      <c r="B479" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C479" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D479" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E479" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F479" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G479" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="480" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A480" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B480" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C480" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D480" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="E480" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F480" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="G480" s="0" t="s">
-        <v>7</v>
+        <v>273</v>
+      </c>
+      <c r="B480" s="0" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="481" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A481" s="0" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B481" s="0" t="n">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="482" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A482" s="0" t="s">
-        <v>274</v>
-      </c>
-      <c r="B482" s="0" t="n">
-        <v>28</v>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="483" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A483" s="0" t="s">
+        <v>275</v>
       </c>
     </row>
     <row r="484" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A484" s="0" t="s">
-        <v>275</v>
+        <v>1</v>
+      </c>
+      <c r="B484" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C484" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D484" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E484" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F484" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G484" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="485" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A485" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B485" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C485" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D485" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="E485" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F485" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="G485" s="0" t="s">
-        <v>7</v>
+        <v>80</v>
+      </c>
+      <c r="B485" s="0" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="486" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A486" s="0" t="s">
-        <v>80</v>
+        <v>276</v>
       </c>
       <c r="B486" s="0" t="n">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="487" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A487" s="0" t="s">
-        <v>276</v>
-      </c>
-      <c r="B487" s="0" t="n">
-        <v>27</v>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="488" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A488" s="0" t="s">
+        <v>277</v>
       </c>
     </row>
     <row r="489" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A489" s="0" t="s">
-        <v>277</v>
+        <v>1</v>
+      </c>
+      <c r="B489" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C489" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D489" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E489" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F489" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G489" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="490" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A490" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B490" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C490" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D490" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="E490" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F490" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="G490" s="0" t="s">
-        <v>7</v>
+        <v>267</v>
+      </c>
+      <c r="B490" s="0" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="491" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A491" s="0" t="s">
-        <v>267</v>
+        <v>206</v>
       </c>
       <c r="B491" s="0" t="n">
-        <v>27</v>
+        <v>25</v>
+      </c>
+      <c r="D491" s="0" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="492" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A492" s="0" t="s">
-        <v>206</v>
+        <v>185</v>
       </c>
       <c r="B492" s="0" t="n">
-        <v>27</v>
-      </c>
-      <c r="D492" s="0" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="493" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A493" s="0" t="s">
-        <v>185</v>
-      </c>
-      <c r="B493" s="0" t="n">
-        <v>29</v>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="494" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A494" s="0" t="s">
+        <v>278</v>
       </c>
     </row>
     <row r="495" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A495" s="0" t="s">
-        <v>278</v>
+        <v>1</v>
+      </c>
+      <c r="B495" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C495" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D495" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E495" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F495" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G495" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="496" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A496" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B496" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C496" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D496" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="E496" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F496" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="G496" s="0" t="s">
-        <v>7</v>
+        <v>279</v>
+      </c>
+      <c r="B496" s="0" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="497" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A497" s="0" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="B497" s="0" t="n">
-        <v>27</v>
+        <v>25</v>
+      </c>
+      <c r="D497" s="0" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="498" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A498" s="0" t="s">
-        <v>280</v>
+        <v>188</v>
       </c>
       <c r="B498" s="0" t="n">
-        <v>27</v>
-      </c>
-      <c r="D498" s="0" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="499" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A499" s="0" t="s">
-        <v>188</v>
-      </c>
-      <c r="B499" s="0" t="n">
-        <v>29</v>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="500" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A500" s="0" t="s">
+        <v>281</v>
       </c>
     </row>
     <row r="501" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A501" s="0" t="s">
-        <v>281</v>
+        <v>1</v>
+      </c>
+      <c r="B501" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C501" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D501" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E501" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F501" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G501" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="502" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A502" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B502" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C502" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D502" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="E502" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F502" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="G502" s="0" t="s">
-        <v>7</v>
+        <v>210</v>
+      </c>
+      <c r="B502" s="0" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="503" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A503" s="0" t="s">
-        <v>210</v>
+        <v>142</v>
       </c>
       <c r="B503" s="0" t="n">
-        <v>27</v>
+        <v>25</v>
+      </c>
+      <c r="D503" s="0" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="504" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A504" s="0" t="s">
-        <v>142</v>
+        <v>190</v>
       </c>
       <c r="B504" s="0" t="n">
-        <v>27</v>
-      </c>
-      <c r="D504" s="0" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="505" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A505" s="0" t="s">
-        <v>190</v>
-      </c>
-      <c r="B505" s="0" t="n">
-        <v>29</v>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="506" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A506" s="0" t="s">
+        <v>282</v>
       </c>
     </row>
     <row r="507" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A507" s="0" t="s">
-        <v>282</v>
+        <v>1</v>
+      </c>
+      <c r="B507" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C507" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D507" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E507" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F507" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G507" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="508" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A508" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B508" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C508" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D508" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="E508" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F508" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="G508" s="0" t="s">
-        <v>7</v>
+        <v>267</v>
+      </c>
+      <c r="B508" s="0" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="509" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A509" s="0" t="s">
-        <v>267</v>
+        <v>206</v>
       </c>
       <c r="B509" s="0" t="n">
-        <v>27</v>
+        <v>25</v>
+      </c>
+      <c r="D509" s="0" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="510" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A510" s="0" t="s">
-        <v>206</v>
+        <v>185</v>
       </c>
       <c r="B510" s="0" t="n">
-        <v>27</v>
-      </c>
-      <c r="D510" s="0" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="511" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A511" s="0" t="s">
-        <v>185</v>
-      </c>
-      <c r="B511" s="0" t="n">
-        <v>29</v>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="512" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A512" s="0" t="s">
+        <v>283</v>
       </c>
     </row>
     <row r="513" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A513" s="0" t="s">
-        <v>283</v>
+        <v>1</v>
+      </c>
+      <c r="B513" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C513" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D513" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E513" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F513" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G513" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="514" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A514" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B514" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C514" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D514" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="E514" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F514" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="G514" s="0" t="s">
-        <v>7</v>
+        <v>279</v>
+      </c>
+      <c r="B514" s="0" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="515" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A515" s="0" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="B515" s="0" t="n">
-        <v>27</v>
+        <v>25</v>
+      </c>
+      <c r="D515" s="0" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="516" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A516" s="0" t="s">
-        <v>280</v>
+        <v>188</v>
       </c>
       <c r="B516" s="0" t="n">
-        <v>27</v>
-      </c>
-      <c r="D516" s="0" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="517" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A517" s="0" t="s">
-        <v>188</v>
-      </c>
-      <c r="B517" s="0" t="n">
-        <v>29</v>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="518" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A518" s="0" t="s">
+        <v>284</v>
       </c>
     </row>
     <row r="519" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A519" s="0" t="s">
-        <v>284</v>
+        <v>1</v>
+      </c>
+      <c r="B519" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C519" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D519" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E519" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F519" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G519" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="520" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A520" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B520" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C520" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D520" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="E520" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F520" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="G520" s="0" t="s">
-        <v>7</v>
+        <v>210</v>
+      </c>
+      <c r="B520" s="0" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="521" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A521" s="0" t="s">
-        <v>210</v>
+        <v>142</v>
       </c>
       <c r="B521" s="0" t="n">
-        <v>27</v>
+        <v>25</v>
+      </c>
+      <c r="D521" s="0" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="522" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A522" s="0" t="s">
-        <v>142</v>
+        <v>190</v>
       </c>
       <c r="B522" s="0" t="n">
-        <v>27</v>
-      </c>
-      <c r="D522" s="0" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="523" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A523" s="0" t="s">
-        <v>190</v>
-      </c>
-      <c r="B523" s="0" t="n">
-        <v>29</v>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="524" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A524" s="0" t="s">
+        <v>285</v>
       </c>
     </row>
     <row r="525" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A525" s="0" t="s">
-        <v>285</v>
+        <v>1</v>
+      </c>
+      <c r="B525" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C525" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D525" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E525" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F525" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G525" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="526" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A526" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B526" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C526" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D526" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="E526" s="1" t="s">
-        <v>5</v>
+        <v>286</v>
+      </c>
+      <c r="B526" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="E526" s="0" t="s">
+        <v>287</v>
       </c>
       <c r="F526" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="G526" s="0" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="527" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A527" s="0" t="s">
-        <v>286</v>
-      </c>
-      <c r="B527" s="0" t="n">
-        <v>28</v>
-      </c>
-      <c r="E527" s="0" t="s">
-        <v>287</v>
-      </c>
-      <c r="F527" s="0" t="s">
         <v>288</v>
+      </c>
+    </row>
+    <row r="528" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A528" s="0" t="s">
+        <v>289</v>
       </c>
     </row>
     <row r="529" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A529" s="0" t="s">
-        <v>289</v>
+        <v>1</v>
+      </c>
+      <c r="B529" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C529" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D529" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E529" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F529" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G529" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="530" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A530" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B530" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C530" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D530" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="E530" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F530" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="G530" s="0" t="s">
-        <v>7</v>
+        <v>290</v>
+      </c>
+      <c r="B530" s="0" t="n">
+        <v>24</v>
       </c>
     </row>
     <row r="531" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A531" s="0" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="B531" s="0" t="n">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="532" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A532" s="0" t="s">
-        <v>291</v>
-      </c>
-      <c r="B532" s="0" t="n">
-        <v>26</v>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="533" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A533" s="0" t="s">
+        <v>292</v>
       </c>
     </row>
     <row r="534" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A534" s="0" t="s">
-        <v>292</v>
+        <v>1</v>
+      </c>
+      <c r="B534" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C534" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D534" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E534" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F534" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G534" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="535" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A535" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B535" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C535" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D535" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="E535" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F535" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="G535" s="0" t="s">
-        <v>7</v>
+        <v>293</v>
+      </c>
+      <c r="B535" s="0" t="n">
+        <v>24</v>
       </c>
     </row>
     <row r="536" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A536" s="0" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="B536" s="0" t="n">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="537" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A537" s="0" t="s">
-        <v>294</v>
-      </c>
-      <c r="B537" s="0" t="n">
-        <v>29</v>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="538" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A538" s="0" t="s">
+        <v>295</v>
       </c>
     </row>
     <row r="539" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A539" s="0" t="s">
-        <v>295</v>
+        <v>1</v>
+      </c>
+      <c r="B539" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C539" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D539" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E539" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F539" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G539" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="540" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A540" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B540" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C540" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D540" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="E540" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F540" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="G540" s="0" t="s">
-        <v>7</v>
+        <v>296</v>
+      </c>
+      <c r="B540" s="0" t="n">
+        <v>24</v>
       </c>
     </row>
     <row r="541" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A541" s="0" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="B541" s="0" t="n">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="542" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A542" s="0" t="s">
-        <v>297</v>
-      </c>
-      <c r="B542" s="0" t="n">
-        <v>28</v>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="543" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A543" s="0" t="s">
+        <v>298</v>
       </c>
     </row>
     <row r="544" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A544" s="0" t="s">
-        <v>298</v>
+        <v>1</v>
+      </c>
+      <c r="B544" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C544" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D544" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E544" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F544" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G544" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="545" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A545" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B545" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C545" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D545" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="E545" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F545" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="G545" s="0" t="s">
-        <v>7</v>
+        <v>254</v>
+      </c>
+      <c r="B545" s="0" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="546" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A546" s="0" t="s">
-        <v>254</v>
+        <v>236</v>
       </c>
       <c r="B546" s="0" t="n">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="547" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A547" s="0" t="s">
-        <v>235</v>
-      </c>
-      <c r="B547" s="0" t="n">
-        <v>28</v>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="548" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A548" s="0" t="s">
+        <v>299</v>
       </c>
     </row>
     <row r="549" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A549" s="0" t="s">
-        <v>299</v>
+        <v>1</v>
+      </c>
+      <c r="B549" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C549" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D549" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E549" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F549" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G549" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="550" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A550" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B550" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C550" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D550" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="E550" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F550" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="G550" s="0" t="s">
-        <v>7</v>
+        <v>300</v>
+      </c>
+      <c r="B550" s="0" t="n">
+        <v>24</v>
       </c>
     </row>
     <row r="551" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A551" s="0" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="B551" s="0" t="n">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="552" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A552" s="0" t="s">
-        <v>301</v>
-      </c>
-      <c r="B552" s="0" t="n">
-        <v>29</v>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="553" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A553" s="0" t="s">
+        <v>302</v>
       </c>
     </row>
     <row r="554" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A554" s="0" t="s">
-        <v>302</v>
+        <v>1</v>
+      </c>
+      <c r="B554" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C554" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D554" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E554" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F554" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G554" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="555" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A555" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B555" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C555" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D555" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="E555" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F555" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="G555" s="0" t="s">
-        <v>7</v>
+        <v>303</v>
+      </c>
+      <c r="B555" s="0" t="n">
+        <v>24</v>
       </c>
     </row>
     <row r="556" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A556" s="0" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="B556" s="0" t="n">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="557" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A557" s="0" t="s">
-        <v>304</v>
-      </c>
-      <c r="B557" s="0" t="n">
-        <v>29</v>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="558" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A558" s="0" t="s">
+        <v>305</v>
       </c>
     </row>
     <row r="559" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A559" s="0" t="s">
-        <v>305</v>
+        <v>1</v>
+      </c>
+      <c r="B559" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C559" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D559" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E559" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F559" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G559" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="560" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A560" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B560" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C560" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D560" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="E560" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F560" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="G560" s="0" t="s">
-        <v>7</v>
+        <v>306</v>
+      </c>
+      <c r="B560" s="0" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="561" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A561" s="0" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="B561" s="0" t="n">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="562" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A562" s="0" t="s">
-        <v>307</v>
-      </c>
-      <c r="B562" s="0" t="n">
-        <v>30</v>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="563" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A563" s="0" t="s">
+        <v>308</v>
       </c>
     </row>
     <row r="564" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A564" s="0" t="s">
-        <v>308</v>
+        <v>1</v>
+      </c>
+      <c r="B564" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C564" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D564" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E564" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F564" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G564" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="565" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A565" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B565" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C565" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D565" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="E565" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F565" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="G565" s="0" t="s">
-        <v>7</v>
+        <v>309</v>
+      </c>
+      <c r="B565" s="0" t="n">
+        <v>26</v>
       </c>
     </row>
     <row r="566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A566" s="0" t="s">
-        <v>309</v>
+        <v>251</v>
       </c>
       <c r="B566" s="0" t="n">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A567" s="0" t="s">
-        <v>251</v>
-      </c>
-      <c r="B567" s="0" t="n">
-        <v>30</v>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A568" s="0" t="s">
+        <v>310</v>
       </c>
     </row>
     <row r="569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A569" s="0" t="s">
-        <v>310</v>
+        <v>1</v>
+      </c>
+      <c r="B569" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C569" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D569" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E569" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F569" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G569" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A570" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B570" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C570" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D570" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="E570" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F570" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="G570" s="0" t="s">
-        <v>7</v>
+        <v>311</v>
+      </c>
+      <c r="B570" s="0" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A571" s="0" t="s">
-        <v>249</v>
+        <v>312</v>
       </c>
       <c r="B571" s="0" t="n">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A572" s="0" t="s">
-        <v>311</v>
-      </c>
-      <c r="B572" s="0" t="n">
-        <v>30</v>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A573" s="0" t="s">
+        <v>313</v>
       </c>
     </row>
     <row r="574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A574" s="0" t="s">
-        <v>312</v>
+        <v>1</v>
+      </c>
+      <c r="B574" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C574" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D574" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E574" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F574" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G574" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A575" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B575" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C575" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D575" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="E575" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F575" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="G575" s="0" t="s">
-        <v>7</v>
+        <v>219</v>
+      </c>
+      <c r="B575" s="0" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A576" s="0" t="s">
-        <v>219</v>
+        <v>314</v>
       </c>
       <c r="B576" s="0" t="n">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="577" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A577" s="0" t="s">
-        <v>313</v>
-      </c>
-      <c r="B577" s="0" t="n">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="579" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A579" s="0" t="s">
-        <v>314</v>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="578" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A578" s="0" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="580" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A580" s="0" t="s">
+        <v>316</v>
       </c>
     </row>
     <row r="581" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A581" s="0" t="s">
-        <v>315</v>
+        <v>1</v>
+      </c>
+      <c r="B581" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C581" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D581" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E581" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F581" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G581" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="582" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A582" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B582" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C582" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D582" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="E582" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F582" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="G582" s="0" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="583" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A583" s="0" t="s">
         <v>300</v>
       </c>
-      <c r="B583" s="0" t="n">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="585" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A585" s="0" t="s">
-        <v>316</v>
+      <c r="B582" s="0" t="n">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="584" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A584" s="0" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="586" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A586" s="0" t="s">
+        <v>318</v>
       </c>
     </row>
     <row r="587" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A587" s="0" t="s">
-        <v>317</v>
+        <v>1</v>
+      </c>
+      <c r="B587" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C587" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D587" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E587" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F587" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G587" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="588" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A588" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B588" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C588" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D588" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="E588" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F588" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="G588" s="0" t="s">
-        <v>7</v>
+        <v>170</v>
+      </c>
+      <c r="B588" s="0" t="n">
+        <v>32</v>
       </c>
     </row>
     <row r="589" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A589" s="0" t="s">
-        <v>170</v>
+        <v>319</v>
       </c>
       <c r="B589" s="0" t="n">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="590" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A590" s="0" t="s">
-        <v>318</v>
-      </c>
-      <c r="B590" s="0" t="n">
         <v>33</v>
+      </c>
+    </row>
+    <row r="591" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A591" s="0" t="s">
+        <v>320</v>
       </c>
     </row>
     <row r="592" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A592" s="0" t="s">
-        <v>319</v>
+        <v>1</v>
+      </c>
+      <c r="B592" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C592" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D592" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E592" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F592" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G592" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="593" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A593" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B593" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C593" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D593" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="E593" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F593" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="G593" s="0" t="s">
-        <v>7</v>
+        <v>80</v>
+      </c>
+      <c r="B593" s="0" t="n">
+        <v>31</v>
       </c>
     </row>
     <row r="594" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A594" s="0" t="s">
-        <v>80</v>
+        <v>321</v>
       </c>
       <c r="B594" s="0" t="n">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="595" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A595" s="0" t="s">
-        <v>320</v>
-      </c>
-      <c r="B595" s="0" t="n">
         <v>33</v>
+      </c>
+    </row>
+    <row r="596" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A596" s="0" t="s">
+        <v>322</v>
       </c>
     </row>
     <row r="597" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A597" s="0" t="s">
-        <v>321</v>
+        <v>1</v>
+      </c>
+      <c r="B597" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C597" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D597" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E597" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F597" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G597" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="598" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A598" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B598" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C598" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D598" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="E598" s="1" t="s">
-        <v>5</v>
+        <v>323</v>
+      </c>
+      <c r="B598" s="0" t="n">
+        <v>32</v>
       </c>
       <c r="F598" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="G598" s="0" t="s">
-        <v>7</v>
+        <v>324</v>
+      </c>
+      <c r="G598" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="599" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A599" s="0" t="s">
-        <v>322</v>
+        <v>325</v>
       </c>
       <c r="B599" s="0" t="n">
-        <v>32</v>
-      </c>
-      <c r="F599" s="0" t="s">
-        <v>323</v>
-      </c>
-      <c r="G599" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="600" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A600" s="0" t="s">
-        <v>324</v>
-      </c>
-      <c r="B600" s="0" t="n">
         <v>33</v>
+      </c>
+    </row>
+    <row r="601" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A601" s="0" t="s">
+        <v>326</v>
       </c>
     </row>
     <row r="602" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A602" s="0" t="s">
-        <v>325</v>
+        <v>1</v>
+      </c>
+      <c r="B602" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C602" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D602" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E602" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F602" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G602" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="603" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A603" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B603" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C603" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D603" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="E603" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F603" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="G603" s="0" t="s">
-        <v>7</v>
+        <v>327</v>
+      </c>
+      <c r="B603" s="0" t="n">
+        <v>32</v>
       </c>
     </row>
     <row r="604" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A604" s="0" t="s">
-        <v>326</v>
+        <v>294</v>
       </c>
       <c r="B604" s="0" t="n">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="605" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A605" s="0" t="s">
-        <v>294</v>
-      </c>
-      <c r="B605" s="0" t="n">
         <v>33</v>
+      </c>
+    </row>
+    <row r="606" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A606" s="0" t="s">
+        <v>328</v>
       </c>
     </row>
     <row r="607" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A607" s="0" t="s">
-        <v>327</v>
+        <v>1</v>
+      </c>
+      <c r="B607" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C607" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D607" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E607" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F607" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G607" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="608" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A608" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B608" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C608" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D608" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="E608" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F608" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="G608" s="0" t="s">
-        <v>7</v>
+        <v>170</v>
+      </c>
+      <c r="B608" s="0" t="n">
+        <v>32</v>
       </c>
     </row>
     <row r="609" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A609" s="0" t="s">
-        <v>170</v>
+        <v>252</v>
       </c>
       <c r="B609" s="0" t="n">
         <v>32</v>
@@ -6472,93 +6481,85 @@
     </row>
     <row r="610" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A610" s="0" t="s">
-        <v>252</v>
+        <v>291</v>
       </c>
       <c r="B610" s="0" t="n">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="611" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A611" s="0" t="s">
-        <v>291</v>
-      </c>
-      <c r="B611" s="0" t="n">
         <v>33</v>
+      </c>
+    </row>
+    <row r="612" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A612" s="0" t="s">
+        <v>329</v>
       </c>
     </row>
     <row r="613" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A613" s="0" t="s">
-        <v>328</v>
+        <v>1</v>
+      </c>
+      <c r="B613" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C613" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D613" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E613" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F613" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="G613" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="614" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A614" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B614" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C614" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="D614" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="E614" s="1" t="s">
-        <v>5</v>
+        <v>330</v>
+      </c>
+      <c r="B614" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="E614" s="0" t="s">
+        <v>331</v>
       </c>
       <c r="F614" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="G614" s="0" t="s">
-        <v>7</v>
+        <v>332</v>
       </c>
     </row>
     <row r="615" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A615" s="0" t="s">
-        <v>329</v>
+        <v>333</v>
       </c>
       <c r="B615" s="0" t="n">
         <v>33</v>
       </c>
       <c r="E615" s="0" t="s">
-        <v>330</v>
+        <v>334</v>
       </c>
       <c r="F615" s="0" t="s">
-        <v>331</v>
+        <v>335</v>
       </c>
     </row>
     <row r="616" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A616" s="0" t="s">
-        <v>332</v>
+        <v>336</v>
       </c>
       <c r="B616" s="0" t="n">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E616" s="0" t="s">
-        <v>333</v>
+        <v>337</v>
       </c>
       <c r="F616" s="0" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="617" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A617" s="0" t="s">
-        <v>335</v>
-      </c>
-      <c r="B617" s="0" t="n">
-        <v>35</v>
-      </c>
-      <c r="E617" s="0" t="s">
-        <v>336</v>
-      </c>
-      <c r="F617" s="0" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="621" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A621" s="0" t="s">
         <v>338</v>
+      </c>
+    </row>
+    <row r="620" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A620" s="0" t="s">
+        <v>339</v>
       </c>
     </row>
   </sheetData>

</xml_diff>